<commit_message>
- parsed `10.1016/j.matchemphys.2017.05.056` missed by Lorenzo
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A5B34-F55F-974C-AEC6-1D2DC52485E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D5261E-4E81-3441-985E-DF6AD9CC4DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="165">
   <si>
     <r>
       <rPr>
@@ -336,6 +336,12 @@
     <t>UCS</t>
   </si>
   <si>
+    <t>VAM</t>
+  </si>
+  <si>
+    <t>minimum compressive ductility</t>
+  </si>
+  <si>
     <t>tensile yield stress</t>
   </si>
   <si>
@@ -361,6 +367,12 @@
   </si>
   <si>
     <t>peak magnetic entropy change</t>
+  </si>
+  <si>
+    <t>minimum UCS</t>
+  </si>
+  <si>
+    <t>F6</t>
   </si>
   <si>
     <t>Co31.5 Fe18.5 Ni31.5 Al18.5</t>
@@ -587,6 +599,33 @@
   </si>
   <si>
     <t>10.20517/microstructures.2022.40</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2017.05.056</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.1</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.2</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.3</t>
+  </si>
+  <si>
+    <t>CoCrFeNi</t>
+  </si>
+  <si>
+    <t>minimum plastic strain</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.4</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.5</t>
+  </si>
+  <si>
+    <t>CoCrFeNiTa0.75</t>
   </si>
 </sst>
 </file>
@@ -3074,8 +3113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T962"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N97" sqref="N97"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3327,7 +3366,7 @@
       </c>
       <c r="O7" s="104"/>
       <c r="P7" s="69" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Q7" s="69" t="s">
         <v>36</v>
@@ -3433,23 +3472,23 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="72" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C10" s="73" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E10" s="72"/>
       <c r="F10" s="74" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G10" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="75" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I10" s="76">
         <v>298</v>
@@ -3465,7 +3504,7 @@
       </c>
       <c r="M10" s="74"/>
       <c r="N10" s="78" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O10" s="79"/>
       <c r="P10" s="80"/>
@@ -3477,23 +3516,23 @@
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="30"/>
       <c r="B11" s="72" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D11" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E11" s="72"/>
       <c r="F11" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G11" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I11" s="76">
         <v>298</v>
@@ -3509,7 +3548,7 @@
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="78" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O11" s="37"/>
       <c r="P11" s="38"/>
@@ -3521,23 +3560,23 @@
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="30"/>
       <c r="B12" s="72" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D12" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="72"/>
       <c r="F12" s="32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G12" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H12" s="75" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I12" s="76">
         <v>298</v>
@@ -3553,7 +3592,7 @@
       </c>
       <c r="M12" s="32"/>
       <c r="N12" s="78" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O12" s="37"/>
       <c r="P12" s="38"/>
@@ -3565,16 +3604,16 @@
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="30"/>
       <c r="B13" s="72" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D13" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F13" s="32" t="s">
         <v>64</v>
@@ -3583,7 +3622,7 @@
         <v>29</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I13" s="76">
         <v>298</v>
@@ -3596,10 +3635,10 @@
         <v>33</v>
       </c>
       <c r="M13" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N13" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O13" s="37"/>
       <c r="P13" s="38"/>
@@ -3611,16 +3650,16 @@
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="30"/>
       <c r="B14" s="72" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D14" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F14" s="32" t="s">
         <v>64</v>
@@ -3629,7 +3668,7 @@
         <v>29</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I14" s="76">
         <v>298</v>
@@ -3642,10 +3681,10 @@
         <v>33</v>
       </c>
       <c r="M14" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N14" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O14" s="37"/>
       <c r="P14" s="38"/>
@@ -3657,16 +3696,16 @@
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="72" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D15" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>64</v>
@@ -3675,7 +3714,7 @@
         <v>29</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I15" s="76">
         <v>298</v>
@@ -3688,10 +3727,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N15" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
@@ -3703,16 +3742,16 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="30"/>
       <c r="B16" s="72" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D16" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>64</v>
@@ -3721,7 +3760,7 @@
         <v>29</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I16" s="76">
         <v>298</v>
@@ -3734,10 +3773,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N16" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O16" s="37"/>
       <c r="P16" s="37"/>
@@ -3749,16 +3788,16 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="38"/>
       <c r="B17" s="72" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D17" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F17" s="32" t="s">
         <v>67</v>
@@ -3767,7 +3806,7 @@
         <v>29</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I17" s="76">
         <v>298</v>
@@ -3780,10 +3819,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N17" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O17" s="37"/>
       <c r="P17" s="37"/>
@@ -3795,16 +3834,16 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="38"/>
       <c r="B18" s="72" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D18" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>67</v>
@@ -3813,7 +3852,7 @@
         <v>29</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I18" s="76">
         <v>298</v>
@@ -3826,10 +3865,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N18" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O18" s="37"/>
       <c r="P18" s="37"/>
@@ -3841,16 +3880,16 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="38"/>
       <c r="B19" s="72" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D19" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>67</v>
@@ -3859,7 +3898,7 @@
         <v>29</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I19" s="76">
         <v>298</v>
@@ -3872,10 +3911,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N19" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
@@ -3887,16 +3926,16 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="38"/>
       <c r="B20" s="72" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D20" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>67</v>
@@ -3905,7 +3944,7 @@
         <v>29</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I20" s="76">
         <v>298</v>
@@ -3918,10 +3957,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N20" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
@@ -3933,16 +3972,16 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="38"/>
       <c r="B21" s="72" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C21" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D21" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F21" s="32" t="s">
         <v>65</v>
@@ -3951,7 +3990,7 @@
         <v>29</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I21" s="76">
         <v>298</v>
@@ -3964,10 +4003,10 @@
         <v>66</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N21" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O21" s="37"/>
       <c r="P21" s="37"/>
@@ -3979,16 +4018,16 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="38"/>
       <c r="B22" s="72" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C22" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D22" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F22" s="32" t="s">
         <v>65</v>
@@ -3997,7 +4036,7 @@
         <v>29</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I22" s="76">
         <v>298</v>
@@ -4010,10 +4049,10 @@
         <v>66</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N22" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O22" s="37"/>
       <c r="P22" s="37"/>
@@ -4025,16 +4064,16 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="30"/>
       <c r="B23" s="72" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C23" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D23" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F23" s="32" t="s">
         <v>65</v>
@@ -4043,7 +4082,7 @@
         <v>29</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I23" s="76">
         <v>298</v>
@@ -4056,10 +4095,10 @@
         <v>66</v>
       </c>
       <c r="M23" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N23" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O23" s="37"/>
       <c r="P23" s="37"/>
@@ -4071,16 +4110,16 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="30"/>
       <c r="B24" s="72" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C24" s="73" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D24" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F24" s="32" t="s">
         <v>65</v>
@@ -4089,7 +4128,7 @@
         <v>29</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I24" s="76">
         <v>298</v>
@@ -4102,10 +4141,10 @@
         <v>66</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="N24" s="78" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
@@ -4116,22 +4155,22 @@
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="139" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B25" s="140" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G25" s="32" t="s">
         <v>29</v>
@@ -4143,13 +4182,13 @@
       </c>
       <c r="K25" s="62"/>
       <c r="L25" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M25" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N25" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O25" s="37"/>
       <c r="P25" s="38"/>
@@ -4160,22 +4199,22 @@
     </row>
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G26" s="32" t="s">
         <v>29</v>
@@ -4187,13 +4226,13 @@
       </c>
       <c r="K26" s="62"/>
       <c r="L26" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M26" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N26" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O26" s="37"/>
       <c r="P26" s="43"/>
@@ -4204,22 +4243,22 @@
     </row>
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G27" s="32" t="s">
         <v>29</v>
@@ -4231,13 +4270,13 @@
       </c>
       <c r="K27" s="62"/>
       <c r="L27" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M27" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N27" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O27" s="37"/>
       <c r="P27" s="43"/>
@@ -4248,22 +4287,22 @@
     </row>
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="30" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>29</v>
@@ -4275,13 +4314,13 @@
       </c>
       <c r="K28" s="62"/>
       <c r="L28" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M28" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O28" s="37"/>
       <c r="P28" s="43"/>
@@ -4292,22 +4331,22 @@
     </row>
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="139" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B29" s="140" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>29</v>
@@ -4319,13 +4358,13 @@
       </c>
       <c r="K29" s="62"/>
       <c r="L29" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M29" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N29" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O29" s="37"/>
       <c r="P29" s="43"/>
@@ -4336,22 +4375,22 @@
     </row>
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G30" s="32" t="s">
         <v>29</v>
@@ -4363,13 +4402,13 @@
       </c>
       <c r="K30" s="62"/>
       <c r="L30" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M30" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N30" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O30" s="37"/>
       <c r="P30" s="43"/>
@@ -4380,22 +4419,22 @@
     </row>
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G31" s="32" t="s">
         <v>29</v>
@@ -4407,13 +4446,13 @@
       </c>
       <c r="K31" s="62"/>
       <c r="L31" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M31" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N31" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O31" s="37"/>
       <c r="P31" s="43"/>
@@ -4424,22 +4463,22 @@
     </row>
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G32" s="32" t="s">
         <v>29</v>
@@ -4451,13 +4490,13 @@
       </c>
       <c r="K32" s="62"/>
       <c r="L32" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M32" s="40" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N32" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O32" s="37"/>
       <c r="P32" s="43"/>
@@ -4468,28 +4507,28 @@
     </row>
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="62">
@@ -4497,13 +4536,13 @@
       </c>
       <c r="K33" s="62"/>
       <c r="L33" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M33" s="40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N33" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O33" s="37"/>
       <c r="P33" s="43"/>
@@ -4514,28 +4553,28 @@
     </row>
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G34" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H34" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I34" s="34"/>
       <c r="J34" s="62">
@@ -4543,13 +4582,13 @@
       </c>
       <c r="K34" s="62"/>
       <c r="L34" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M34" s="40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N34" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O34" s="37"/>
       <c r="P34" s="38"/>
@@ -4560,28 +4599,28 @@
     </row>
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="30" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G35" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I35" s="34"/>
       <c r="J35" s="38">
@@ -4589,13 +4628,13 @@
       </c>
       <c r="K35" s="38"/>
       <c r="L35" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M35" s="40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N35" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O35" s="37"/>
       <c r="P35" s="38"/>
@@ -4606,28 +4645,28 @@
     </row>
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G36" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="38">
@@ -4635,13 +4674,13 @@
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M36" s="40" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N36" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O36" s="37"/>
       <c r="P36" s="38"/>
@@ -4652,28 +4691,28 @@
     </row>
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G37" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H37" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I37" s="34"/>
       <c r="J37" s="38">
@@ -4681,13 +4720,13 @@
       </c>
       <c r="K37" s="35"/>
       <c r="L37" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M37" s="40" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N37" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O37" s="37"/>
       <c r="P37" s="38"/>
@@ -4698,28 +4737,28 @@
     </row>
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="30" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G38" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="38">
@@ -4727,13 +4766,13 @@
       </c>
       <c r="K38" s="35"/>
       <c r="L38" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M38" s="40" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N38" s="36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O38" s="46"/>
       <c r="P38" s="39"/>
@@ -4745,25 +4784,25 @@
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="30"/>
       <c r="B39" s="41" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G39" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I39" s="34"/>
       <c r="J39" s="38">
@@ -4771,13 +4810,13 @@
       </c>
       <c r="K39" s="35"/>
       <c r="L39" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M39" s="40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N39" s="36" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="O39" s="46"/>
       <c r="P39" s="39"/>
@@ -4789,23 +4828,23 @@
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
       <c r="A40" s="30"/>
       <c r="B40" s="41" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G40" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H40" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="46">
@@ -4813,11 +4852,11 @@
       </c>
       <c r="K40" s="47"/>
       <c r="L40" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M40" s="40"/>
       <c r="N40" s="36" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="O40" s="46"/>
       <c r="P40" s="39"/>
@@ -4829,23 +4868,23 @@
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
       <c r="A41" s="30"/>
       <c r="B41" s="41" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G41" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I41" s="34"/>
       <c r="J41" s="94">
@@ -4853,11 +4892,11 @@
       </c>
       <c r="K41" s="47"/>
       <c r="L41" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M41" s="40"/>
       <c r="N41" s="36" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O41" s="46"/>
       <c r="P41" s="39"/>
@@ -4869,23 +4908,23 @@
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
       <c r="A42" s="30"/>
       <c r="B42" s="41" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G42" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H42" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I42" s="34"/>
       <c r="J42" s="94">
@@ -4893,11 +4932,11 @@
       </c>
       <c r="K42" s="47"/>
       <c r="L42" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M42" s="40"/>
       <c r="N42" s="36" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="O42" s="46"/>
       <c r="P42" s="47"/>
@@ -4909,23 +4948,23 @@
     <row r="43" spans="1:20" ht="18" customHeight="1">
       <c r="A43" s="30"/>
       <c r="B43" s="41" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G43" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H43" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="94">
@@ -4933,11 +4972,11 @@
       </c>
       <c r="K43" s="47"/>
       <c r="L43" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M43" s="40"/>
       <c r="N43" s="36" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="O43" s="46"/>
       <c r="P43" s="47"/>
@@ -4949,23 +4988,23 @@
     <row r="44" spans="1:20" ht="18" customHeight="1">
       <c r="A44" s="30"/>
       <c r="B44" s="41" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G44" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I44" s="34"/>
       <c r="J44" s="94">
@@ -4973,11 +5012,11 @@
       </c>
       <c r="K44" s="49"/>
       <c r="L44" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M44" s="40"/>
       <c r="N44" s="141" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O44" s="46"/>
       <c r="P44" s="46"/>
@@ -4989,23 +5028,23 @@
     <row r="45" spans="1:20" ht="18" customHeight="1">
       <c r="A45" s="30"/>
       <c r="B45" s="41" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G45" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="46">
@@ -5013,11 +5052,11 @@
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M45" s="40"/>
       <c r="N45" s="141" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="O45" s="46"/>
       <c r="P45" s="46"/>
@@ -5029,25 +5068,25 @@
     <row r="46" spans="1:20" ht="18" customHeight="1">
       <c r="A46" s="30"/>
       <c r="B46" s="41" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G46" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H46" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="38">
@@ -5055,13 +5094,13 @@
       </c>
       <c r="K46" s="35"/>
       <c r="L46" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M46" s="40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N46" s="36" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="O46" s="46"/>
       <c r="P46" s="46"/>
@@ -5073,23 +5112,23 @@
     <row r="47" spans="1:20" ht="18" customHeight="1">
       <c r="A47" s="30"/>
       <c r="B47" s="41" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G47" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H47" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I47" s="34"/>
       <c r="J47" s="46">
@@ -5097,11 +5136,11 @@
       </c>
       <c r="K47" s="47"/>
       <c r="L47" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M47" s="40"/>
       <c r="N47" s="36" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="O47" s="46"/>
       <c r="P47" s="46"/>
@@ -5113,23 +5152,23 @@
     <row r="48" spans="1:20" ht="18" customHeight="1">
       <c r="A48" s="30"/>
       <c r="B48" s="41" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G48" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I48" s="34"/>
       <c r="J48" s="94">
@@ -5137,11 +5176,11 @@
       </c>
       <c r="K48" s="47"/>
       <c r="L48" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M48" s="40"/>
       <c r="N48" s="36" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O48" s="46"/>
       <c r="P48" s="46"/>
@@ -5153,23 +5192,23 @@
     <row r="49" spans="1:20" ht="18" customHeight="1">
       <c r="A49" s="30"/>
       <c r="B49" s="41" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G49" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="94">
@@ -5177,11 +5216,11 @@
       </c>
       <c r="K49" s="47"/>
       <c r="L49" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M49" s="40"/>
       <c r="N49" s="36" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="O49" s="46"/>
       <c r="P49" s="46"/>
@@ -5193,23 +5232,23 @@
     <row r="50" spans="1:20" ht="18" customHeight="1">
       <c r="A50" s="30"/>
       <c r="B50" s="41" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G50" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I50" s="34"/>
       <c r="J50" s="94">
@@ -5217,11 +5256,11 @@
       </c>
       <c r="K50" s="47"/>
       <c r="L50" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M50" s="40"/>
       <c r="N50" s="36" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="O50" s="46"/>
       <c r="P50" s="46"/>
@@ -5233,23 +5272,23 @@
     <row r="51" spans="1:20" ht="18" customHeight="1">
       <c r="A51" s="30"/>
       <c r="B51" s="41" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G51" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I51" s="34"/>
       <c r="J51" s="94">
@@ -5257,11 +5296,11 @@
       </c>
       <c r="K51" s="49"/>
       <c r="L51" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M51" s="40"/>
       <c r="N51" s="141" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O51" s="46"/>
       <c r="P51" s="46"/>
@@ -5273,23 +5312,23 @@
     <row r="52" spans="1:20" ht="18" customHeight="1">
       <c r="A52" s="30"/>
       <c r="B52" s="41" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="31" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F52" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G52" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I52" s="34"/>
       <c r="J52" s="46">
@@ -5297,11 +5336,11 @@
       </c>
       <c r="K52" s="49"/>
       <c r="L52" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M52" s="40"/>
       <c r="N52" s="141" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="O52" s="46"/>
       <c r="P52" s="47"/>
@@ -5313,25 +5352,25 @@
     <row r="53" spans="1:20" ht="18" customHeight="1">
       <c r="A53" s="30"/>
       <c r="B53" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F53" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G53" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H53" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I53" s="34"/>
       <c r="J53" s="49">
@@ -5339,13 +5378,13 @@
       </c>
       <c r="K53" s="49"/>
       <c r="L53" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M53" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N53" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O53" s="46"/>
       <c r="P53" s="47"/>
@@ -5357,25 +5396,25 @@
     <row r="54" spans="1:20" ht="18" customHeight="1">
       <c r="A54" s="30"/>
       <c r="B54" s="31" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F54" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G54" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H54" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I54" s="34"/>
       <c r="J54" s="49">
@@ -5383,13 +5422,13 @@
       </c>
       <c r="K54" s="49"/>
       <c r="L54" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M54" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N54" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O54" s="46"/>
       <c r="P54" s="47"/>
@@ -5401,25 +5440,25 @@
     <row r="55" spans="1:20" ht="18" customHeight="1">
       <c r="A55" s="30"/>
       <c r="B55" s="31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E55" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F55" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G55" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="49">
@@ -5427,13 +5466,13 @@
       </c>
       <c r="K55" s="49"/>
       <c r="L55" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M55" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N55" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O55" s="46"/>
       <c r="P55" s="47"/>
@@ -5445,25 +5484,25 @@
     <row r="56" spans="1:20" ht="18" customHeight="1">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F56" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G56" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I56" s="34"/>
       <c r="J56" s="49">
@@ -5471,13 +5510,13 @@
       </c>
       <c r="K56" s="49"/>
       <c r="L56" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M56" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N56" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O56" s="46"/>
       <c r="P56" s="46"/>
@@ -5489,25 +5528,25 @@
     <row r="57" spans="1:20" ht="18" customHeight="1">
       <c r="A57" s="30"/>
       <c r="B57" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F57" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G57" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H57" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I57" s="34"/>
       <c r="J57" s="49">
@@ -5515,13 +5554,13 @@
       </c>
       <c r="K57" s="49"/>
       <c r="L57" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M57" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N57" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O57" s="46"/>
       <c r="P57" s="46"/>
@@ -5533,25 +5572,25 @@
     <row r="58" spans="1:20" ht="18" customHeight="1">
       <c r="A58" s="30"/>
       <c r="B58" s="31" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F58" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G58" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H58" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="49">
@@ -5559,13 +5598,13 @@
       </c>
       <c r="K58" s="49"/>
       <c r="L58" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M58" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N58" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O58" s="46"/>
       <c r="P58" s="46"/>
@@ -5577,25 +5616,25 @@
     <row r="59" spans="1:20" ht="18" customHeight="1">
       <c r="A59" s="30"/>
       <c r="B59" s="31" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E59" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F59" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G59" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I59" s="34"/>
       <c r="J59" s="49">
@@ -5603,13 +5642,13 @@
       </c>
       <c r="K59" s="49"/>
       <c r="L59" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M59" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N59" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O59" s="46"/>
       <c r="P59" s="46"/>
@@ -5621,25 +5660,25 @@
     <row r="60" spans="1:20" ht="18" customHeight="1">
       <c r="A60" s="30"/>
       <c r="B60" s="31" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E60" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F60" s="48" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G60" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H60" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I60" s="34"/>
       <c r="J60" s="49">
@@ -5647,13 +5686,13 @@
       </c>
       <c r="K60" s="49"/>
       <c r="L60" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M60" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N60" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O60" s="46"/>
       <c r="P60" s="46"/>
@@ -5665,25 +5704,25 @@
     <row r="61" spans="1:20" ht="18" customHeight="1">
       <c r="A61" s="30"/>
       <c r="B61" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D61" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E61" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F61" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G61" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H61" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I61" s="34"/>
       <c r="J61" s="49">
@@ -5691,13 +5730,13 @@
       </c>
       <c r="K61" s="49"/>
       <c r="L61" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M61" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N61" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O61" s="46"/>
       <c r="P61" s="46"/>
@@ -5709,25 +5748,25 @@
     <row r="62" spans="1:20" ht="18" customHeight="1">
       <c r="A62" s="30"/>
       <c r="B62" s="31" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D62" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E62" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F62" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G62" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H62" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="49">
@@ -5735,13 +5774,13 @@
       </c>
       <c r="K62" s="49"/>
       <c r="L62" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M62" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N62" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O62" s="46"/>
       <c r="P62" s="46"/>
@@ -5753,25 +5792,25 @@
     <row r="63" spans="1:20" ht="18" customHeight="1">
       <c r="A63" s="30"/>
       <c r="B63" s="31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C63" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D63" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E63" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F63" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G63" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H63" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I63" s="34"/>
       <c r="J63" s="49">
@@ -5779,13 +5818,13 @@
       </c>
       <c r="K63" s="49"/>
       <c r="L63" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M63" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N63" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O63" s="46"/>
       <c r="P63" s="46"/>
@@ -5797,25 +5836,25 @@
     <row r="64" spans="1:20" ht="18" customHeight="1">
       <c r="A64" s="30"/>
       <c r="B64" s="31" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E64" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F64" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G64" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H64" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I64" s="34"/>
       <c r="J64" s="49">
@@ -5823,13 +5862,13 @@
       </c>
       <c r="K64" s="49"/>
       <c r="L64" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M64" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N64" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O64" s="46"/>
       <c r="P64" s="46"/>
@@ -5841,25 +5880,25 @@
     <row r="65" spans="1:20" ht="18" customHeight="1">
       <c r="A65" s="30"/>
       <c r="B65" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F65" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G65" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H65" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I65" s="34"/>
       <c r="J65" s="49">
@@ -5867,13 +5906,13 @@
       </c>
       <c r="K65" s="49"/>
       <c r="L65" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M65" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N65" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O65" s="46"/>
       <c r="P65" s="46"/>
@@ -5885,25 +5924,25 @@
     <row r="66" spans="1:20" ht="18" customHeight="1">
       <c r="A66" s="30"/>
       <c r="B66" s="31" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F66" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G66" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H66" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I66" s="34"/>
       <c r="J66" s="94">
@@ -5911,13 +5950,13 @@
       </c>
       <c r="K66" s="47"/>
       <c r="L66" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M66" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N66" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O66" s="46"/>
       <c r="P66" s="46"/>
@@ -5929,25 +5968,25 @@
     <row r="67" spans="1:20" ht="18" customHeight="1">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D67" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E67" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F67" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G67" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H67" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I67" s="34"/>
       <c r="J67" s="46">
@@ -5955,13 +5994,13 @@
       </c>
       <c r="K67" s="47"/>
       <c r="L67" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M67" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N67" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O67" s="46"/>
       <c r="P67" s="46"/>
@@ -5973,25 +6012,25 @@
     <row r="68" spans="1:20" ht="18" customHeight="1">
       <c r="A68" s="30"/>
       <c r="B68" s="31" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D68" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E68" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F68" s="48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G68" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H68" s="34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="46">
@@ -5999,13 +6038,13 @@
       </c>
       <c r="K68" s="47"/>
       <c r="L68" s="50" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M68" s="50" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N68" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O68" s="46"/>
       <c r="P68" s="46"/>
@@ -6017,16 +6056,16 @@
     <row r="69" spans="1:20" ht="18" customHeight="1">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>62</v>
@@ -6050,10 +6089,10 @@
         <v>33</v>
       </c>
       <c r="M69" s="50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N69" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O69" s="46"/>
       <c r="P69" s="46">
@@ -6069,16 +6108,16 @@
     <row r="70" spans="1:20" ht="18" customHeight="1">
       <c r="A70" s="30"/>
       <c r="B70" s="31" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E70" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>62</v>
@@ -6102,10 +6141,10 @@
         <v>33</v>
       </c>
       <c r="M70" s="50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N70" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O70" s="46"/>
       <c r="P70" s="46">
@@ -6121,16 +6160,16 @@
     <row r="71" spans="1:20" ht="18" customHeight="1">
       <c r="A71" s="30"/>
       <c r="B71" s="31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D71" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>62</v>
@@ -6154,10 +6193,10 @@
         <v>33</v>
       </c>
       <c r="M71" s="50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N71" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O71" s="46"/>
       <c r="P71" s="1">
@@ -6173,16 +6212,16 @@
     <row r="72" spans="1:20" ht="18" customHeight="1">
       <c r="A72" s="30"/>
       <c r="B72" s="31" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E72" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>62</v>
@@ -6206,10 +6245,10 @@
         <v>33</v>
       </c>
       <c r="M72" s="50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N72" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O72" s="46"/>
       <c r="P72" s="47">
@@ -6225,16 +6264,16 @@
     <row r="73" spans="1:20" ht="18" customHeight="1">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E73" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>62</v>
@@ -6258,10 +6297,10 @@
         <v>33</v>
       </c>
       <c r="M73" s="50" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N73" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O73" s="46"/>
       <c r="P73" s="46">
@@ -6277,16 +6316,16 @@
     <row r="74" spans="1:20" ht="18" customHeight="1">
       <c r="A74" s="30"/>
       <c r="B74" s="31" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E74" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F74" s="48" t="s">
         <v>62</v>
@@ -6310,10 +6349,10 @@
         <v>33</v>
       </c>
       <c r="M74" s="50" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N74" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O74" s="46"/>
       <c r="P74" s="46">
@@ -6329,16 +6368,16 @@
     <row r="75" spans="1:20" ht="18" customHeight="1">
       <c r="A75" s="30"/>
       <c r="B75" s="31" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C75" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E75" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F75" s="48" t="s">
         <v>62</v>
@@ -6362,10 +6401,10 @@
         <v>33</v>
       </c>
       <c r="M75" s="50" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N75" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O75" s="46"/>
       <c r="P75" s="46">
@@ -6381,16 +6420,16 @@
     <row r="76" spans="1:20" ht="18" customHeight="1">
       <c r="A76" s="30"/>
       <c r="B76" s="31" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C76" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D76" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E76" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F76" s="48" t="s">
         <v>62</v>
@@ -6414,10 +6453,10 @@
         <v>33</v>
       </c>
       <c r="M76" s="50" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N76" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O76" s="46"/>
       <c r="P76" s="46">
@@ -6433,16 +6472,16 @@
     <row r="77" spans="1:20" ht="18" customHeight="1">
       <c r="A77" s="30"/>
       <c r="B77" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C77" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E77" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F77" s="48" t="s">
         <v>67</v>
@@ -6462,10 +6501,10 @@
         <v>33</v>
       </c>
       <c r="M77" s="50" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="N77" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O77" s="46"/>
       <c r="P77" s="49"/>
@@ -6477,16 +6516,16 @@
     <row r="78" spans="1:20" ht="18" customHeight="1">
       <c r="A78" s="30"/>
       <c r="B78" s="31" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C78" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E78" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F78" s="48" t="s">
         <v>67</v>
@@ -6506,10 +6545,10 @@
         <v>33</v>
       </c>
       <c r="M78" s="50" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="N78" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O78" s="46"/>
       <c r="P78" s="49"/>
@@ -6521,16 +6560,16 @@
     <row r="79" spans="1:20" ht="18" customHeight="1">
       <c r="A79" s="30"/>
       <c r="B79" s="31" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E79" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F79" s="48" t="s">
         <v>67</v>
@@ -6550,10 +6589,10 @@
         <v>33</v>
       </c>
       <c r="M79" s="50" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="N79" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O79" s="46"/>
       <c r="P79" s="46"/>
@@ -6565,16 +6604,16 @@
     <row r="80" spans="1:20" ht="18" customHeight="1">
       <c r="A80" s="30"/>
       <c r="B80" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C80" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D80" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E80" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F80" s="48" t="s">
         <v>65</v>
@@ -6594,10 +6633,10 @@
         <v>66</v>
       </c>
       <c r="M80" s="50" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="N80" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O80" s="46"/>
       <c r="P80" s="39"/>
@@ -6609,16 +6648,16 @@
     <row r="81" spans="1:20" ht="18" customHeight="1">
       <c r="A81" s="30"/>
       <c r="B81" s="31" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C81" s="30" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E81" s="31" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F81" s="48" t="s">
         <v>65</v>
@@ -6638,10 +6677,10 @@
         <v>66</v>
       </c>
       <c r="M81" s="50" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="N81" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O81" s="46"/>
       <c r="P81" s="39"/>
@@ -6653,16 +6692,16 @@
     <row r="82" spans="1:20" ht="18" customHeight="1">
       <c r="A82" s="30"/>
       <c r="B82" s="31" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D82" s="30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E82" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F82" s="48" t="s">
         <v>65</v>
@@ -6682,10 +6721,10 @@
         <v>66</v>
       </c>
       <c r="M82" s="50" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="N82" s="30" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O82" s="46"/>
       <c r="P82" s="39"/>
@@ -6697,19 +6736,19 @@
     <row r="83" spans="1:20" ht="18" customHeight="1">
       <c r="A83" s="30"/>
       <c r="B83" s="31" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C83" s="30" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D83" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E83" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F83" s="48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G83" s="32" t="s">
         <v>29</v>
@@ -6727,7 +6766,7 @@
       </c>
       <c r="M83" s="50"/>
       <c r="N83" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O83" s="46"/>
       <c r="P83" s="39"/>
@@ -6739,19 +6778,19 @@
     <row r="84" spans="1:20" ht="18" customHeight="1">
       <c r="A84" s="30"/>
       <c r="B84" s="31" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C84" s="30" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D84" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E84" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F84" s="48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G84" s="32" t="s">
         <v>29</v>
@@ -6769,7 +6808,7 @@
       </c>
       <c r="M84" s="50"/>
       <c r="N84" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O84" s="46"/>
       <c r="P84" s="39"/>
@@ -6781,19 +6820,19 @@
     <row r="85" spans="1:20" ht="18" customHeight="1">
       <c r="A85" s="30"/>
       <c r="B85" s="31" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C85" s="30" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E85" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F85" s="48" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G85" s="32" t="s">
         <v>29</v>
@@ -6811,7 +6850,7 @@
       </c>
       <c r="M85" s="50"/>
       <c r="N85" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O85" s="46"/>
       <c r="P85" s="39"/>
@@ -6823,19 +6862,19 @@
     <row r="86" spans="1:20" ht="18" customHeight="1">
       <c r="A86" s="30"/>
       <c r="B86" s="31" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C86" s="30" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D86" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E86" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G86" s="32" t="s">
         <v>29</v>
@@ -6853,7 +6892,7 @@
       </c>
       <c r="M86" s="50"/>
       <c r="N86" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O86" s="46"/>
       <c r="P86" s="39"/>
@@ -6865,19 +6904,19 @@
     <row r="87" spans="1:20" ht="18" customHeight="1">
       <c r="A87" s="30"/>
       <c r="B87" s="31" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C87" s="30" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D87" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E87" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F87" s="48" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G87" s="32" t="s">
         <v>29</v>
@@ -6895,7 +6934,7 @@
       </c>
       <c r="M87" s="50"/>
       <c r="N87" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O87" s="46"/>
       <c r="P87" s="39"/>
@@ -6907,19 +6946,19 @@
     <row r="88" spans="1:20" ht="18" customHeight="1">
       <c r="A88" s="30"/>
       <c r="B88" s="31" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C88" s="30" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D88" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E88" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F88" s="48" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G88" s="32" t="s">
         <v>29</v>
@@ -6937,7 +6976,7 @@
       </c>
       <c r="M88" s="50"/>
       <c r="N88" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O88" s="46"/>
       <c r="P88" s="39"/>
@@ -6949,17 +6988,17 @@
     <row r="89" spans="1:20" ht="18" customHeight="1">
       <c r="A89" s="30"/>
       <c r="B89" s="31" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C89" s="30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D89" s="30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E89" s="31"/>
       <c r="F89" s="48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G89" s="32" t="s">
         <v>29</v>
@@ -6977,7 +7016,7 @@
       </c>
       <c r="M89" s="50"/>
       <c r="N89" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O89" s="46"/>
       <c r="P89" s="39"/>
@@ -6989,17 +7028,17 @@
     <row r="90" spans="1:20" ht="18" customHeight="1">
       <c r="A90" s="30"/>
       <c r="B90" s="31" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D90" s="30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E90" s="31"/>
       <c r="F90" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G90" s="32" t="s">
         <v>29</v>
@@ -7017,7 +7056,7 @@
       </c>
       <c r="M90" s="50"/>
       <c r="N90" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O90" s="46"/>
       <c r="P90" s="39"/>
@@ -7029,17 +7068,17 @@
     <row r="91" spans="1:20" ht="18" customHeight="1">
       <c r="A91" s="30"/>
       <c r="B91" s="31" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C91" s="30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D91" s="30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E91" s="31"/>
       <c r="F91" s="32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G91" s="32" t="s">
         <v>29</v>
@@ -7057,7 +7096,7 @@
       </c>
       <c r="M91" s="50"/>
       <c r="N91" s="30" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="O91" s="46"/>
       <c r="P91" s="47"/>
@@ -7068,21 +7107,44 @@
     </row>
     <row r="92" spans="1:20" ht="18" customHeight="1">
       <c r="A92" s="30"/>
-      <c r="B92" s="31"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
+      <c r="B92" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E92" s="31"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="32"/>
+      <c r="F92" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G92" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H92" s="33"/>
-      <c r="I92" s="34"/>
-      <c r="J92" s="39"/>
+      <c r="I92" s="34">
+        <v>298</v>
+      </c>
+      <c r="J92" s="142">
+        <f t="shared" ref="J92" si="2">P92*9807000</f>
+        <v>1765260000</v>
+      </c>
       <c r="K92" s="49"/>
-      <c r="L92" s="32"/>
-      <c r="M92" s="50"/>
-      <c r="N92" s="30"/>
+      <c r="L92" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M92" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="N92" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O92" s="46"/>
-      <c r="P92" s="47"/>
+      <c r="P92" s="47">
+        <v>180</v>
+      </c>
       <c r="Q92" s="39"/>
       <c r="R92" s="46"/>
       <c r="S92" s="37"/>
@@ -7090,19 +7152,39 @@
     </row>
     <row r="93" spans="1:20" ht="18" customHeight="1">
       <c r="A93" s="30"/>
-      <c r="B93" s="31"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
+      <c r="B93" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E93" s="31"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32"/>
+      <c r="F93" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G93" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H93" s="33"/>
-      <c r="I93" s="34"/>
-      <c r="J93" s="39"/>
+      <c r="I93" s="34">
+        <v>298</v>
+      </c>
+      <c r="J93" s="39">
+        <v>50</v>
+      </c>
       <c r="K93" s="49"/>
-      <c r="L93" s="32"/>
-      <c r="M93" s="50"/>
-      <c r="N93" s="30"/>
+      <c r="L93" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M93" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N93" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O93" s="46"/>
       <c r="P93" s="47"/>
       <c r="Q93" s="39"/>
@@ -7112,19 +7194,39 @@
     </row>
     <row r="94" spans="1:20" ht="18" customHeight="1">
       <c r="A94" s="30"/>
-      <c r="B94" s="31"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
+      <c r="B94" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C94" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E94" s="31"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="32"/>
+      <c r="F94" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G94" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H94" s="33"/>
-      <c r="I94" s="34"/>
-      <c r="J94" s="39"/>
+      <c r="I94" s="34">
+        <v>298</v>
+      </c>
+      <c r="J94" s="39">
+        <v>50</v>
+      </c>
       <c r="K94" s="49"/>
-      <c r="L94" s="32"/>
-      <c r="M94" s="50"/>
-      <c r="N94" s="30"/>
+      <c r="L94" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M94" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N94" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O94" s="46"/>
       <c r="P94" s="47"/>
       <c r="Q94" s="39"/>
@@ -7134,19 +7236,39 @@
     </row>
     <row r="95" spans="1:20" ht="18" customHeight="1">
       <c r="A95" s="30"/>
-      <c r="B95" s="31"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
+      <c r="B95" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E95" s="31"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="32"/>
+      <c r="F95" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G95" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H95" s="33"/>
-      <c r="I95" s="34"/>
-      <c r="J95" s="39"/>
+      <c r="I95" s="34">
+        <v>298</v>
+      </c>
+      <c r="J95" s="39">
+        <v>50</v>
+      </c>
       <c r="K95" s="49"/>
-      <c r="L95" s="32"/>
-      <c r="M95" s="50"/>
-      <c r="N95" s="30"/>
+      <c r="L95" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M95" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N95" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O95" s="46"/>
       <c r="P95" s="47"/>
       <c r="Q95" s="39"/>
@@ -7156,173 +7278,368 @@
     </row>
     <row r="96" spans="1:20" ht="18" customHeight="1">
       <c r="A96" s="30"/>
-      <c r="B96" s="31"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
+      <c r="B96" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C96" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E96" s="31"/>
-      <c r="F96" s="32"/>
-      <c r="G96" s="32"/>
+      <c r="F96" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G96" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H96" s="33"/>
-      <c r="I96" s="34"/>
-      <c r="J96" s="39"/>
+      <c r="I96" s="34">
+        <v>298</v>
+      </c>
+      <c r="J96" s="39">
+        <f>P96-Q96</f>
+        <v>47.934322033898297</v>
+      </c>
       <c r="K96" s="49"/>
-      <c r="L96" s="32"/>
-      <c r="M96" s="50"/>
-      <c r="N96" s="30"/>
+      <c r="L96" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M96" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N96" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O96" s="46"/>
-      <c r="P96" s="47"/>
-      <c r="Q96" s="39"/>
+      <c r="P96" s="46">
+        <v>60.010593220338897</v>
+      </c>
+      <c r="Q96" s="46">
+        <v>12.0762711864406</v>
+      </c>
       <c r="R96" s="46"/>
       <c r="S96" s="37"/>
       <c r="T96" s="37"/>
     </row>
     <row r="97" spans="1:20" ht="18" customHeight="1">
       <c r="A97" s="30"/>
-      <c r="B97" s="31"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
+      <c r="B97" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C97" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E97" s="31"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="32"/>
+      <c r="F97" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G97" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H97" s="33"/>
-      <c r="I97" s="34"/>
-      <c r="J97" s="39"/>
+      <c r="I97" s="34">
+        <v>298</v>
+      </c>
+      <c r="J97" s="39">
+        <f t="shared" ref="J97:J102" si="3">P97-Q97</f>
+        <v>48.6758474576271</v>
+      </c>
       <c r="K97" s="49"/>
-      <c r="L97" s="32"/>
-      <c r="M97" s="50"/>
-      <c r="N97" s="30"/>
+      <c r="L97" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M97" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N97" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O97" s="46"/>
-      <c r="P97" s="39"/>
-      <c r="Q97" s="39"/>
+      <c r="P97" s="46">
+        <v>60.010593220338897</v>
+      </c>
+      <c r="Q97" s="46">
+        <v>11.334745762711799</v>
+      </c>
       <c r="R97" s="46"/>
       <c r="S97" s="37"/>
       <c r="T97" s="37"/>
     </row>
     <row r="98" spans="1:20" ht="18" customHeight="1">
       <c r="A98" s="30"/>
-      <c r="B98" s="31"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
+      <c r="B98" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C98" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E98" s="31"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="32"/>
+      <c r="F98" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G98" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H98" s="33"/>
-      <c r="I98" s="34"/>
-      <c r="J98" s="39"/>
+      <c r="I98" s="34">
+        <v>298</v>
+      </c>
+      <c r="J98" s="39">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="K98" s="49"/>
-      <c r="L98" s="32"/>
-      <c r="M98" s="32"/>
-      <c r="N98" s="30"/>
+      <c r="L98" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M98" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N98" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O98" s="46"/>
-      <c r="P98" s="39"/>
-      <c r="Q98" s="38"/>
+      <c r="P98" s="46">
+        <v>60.010593220338897</v>
+      </c>
+      <c r="Q98" s="46">
+        <v>10.010593220338899</v>
+      </c>
       <c r="R98" s="46"/>
       <c r="S98" s="37"/>
       <c r="T98" s="37"/>
     </row>
     <row r="99" spans="1:20" ht="18" customHeight="1">
       <c r="A99" s="30"/>
-      <c r="B99" s="31"/>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
+      <c r="B99" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C99" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E99" s="31"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="32"/>
+      <c r="F99" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G99" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H99" s="33"/>
-      <c r="I99" s="34"/>
-      <c r="J99" s="49"/>
+      <c r="I99" s="34">
+        <v>298</v>
+      </c>
+      <c r="J99" s="39">
+        <f t="shared" si="3"/>
+        <v>36.493644067796552</v>
+      </c>
       <c r="K99" s="49"/>
-      <c r="L99" s="32"/>
-      <c r="M99" s="32"/>
-      <c r="N99" s="30"/>
+      <c r="L99" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M99" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N99" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O99" s="46"/>
-      <c r="P99" s="47"/>
-      <c r="Q99" s="38"/>
+      <c r="P99" s="46">
+        <v>44.332627118643998</v>
+      </c>
+      <c r="Q99" s="46">
+        <v>7.8389830508474496</v>
+      </c>
       <c r="R99" s="46"/>
       <c r="S99" s="37"/>
       <c r="T99" s="37"/>
     </row>
     <row r="100" spans="1:20" ht="18" customHeight="1">
       <c r="A100" s="30"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="30"/>
-      <c r="D100" s="30"/>
+      <c r="B100" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C100" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E100" s="31"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="32"/>
+      <c r="F100" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G100" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H100" s="33"/>
-      <c r="I100" s="34"/>
-      <c r="J100" s="49"/>
+      <c r="I100" s="34">
+        <v>298</v>
+      </c>
+      <c r="J100" s="39">
+        <f t="shared" si="3"/>
+        <v>28.601694915254239</v>
+      </c>
       <c r="K100" s="49"/>
-      <c r="L100" s="32"/>
-      <c r="M100" s="32"/>
-      <c r="N100" s="30"/>
+      <c r="L100" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M100" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N100" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O100" s="46"/>
-      <c r="P100" s="47"/>
-      <c r="Q100" s="39"/>
+      <c r="P100" s="46">
+        <v>34.375</v>
+      </c>
+      <c r="Q100" s="46">
+        <v>5.7733050847457603</v>
+      </c>
       <c r="R100" s="46"/>
       <c r="S100" s="37"/>
       <c r="T100" s="37"/>
     </row>
     <row r="101" spans="1:20" ht="18" customHeight="1">
       <c r="A101" s="30"/>
-      <c r="B101" s="31"/>
-      <c r="C101" s="30"/>
-      <c r="D101" s="30"/>
+      <c r="B101" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C101" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E101" s="31"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
+      <c r="F101" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G101" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H101" s="33"/>
-      <c r="I101" s="38"/>
-      <c r="J101" s="49"/>
+      <c r="I101" s="34">
+        <v>298</v>
+      </c>
+      <c r="J101" s="39">
+        <f t="shared" si="3"/>
+        <v>26.324152542372861</v>
+      </c>
       <c r="K101" s="49"/>
-      <c r="L101" s="32"/>
-      <c r="M101" s="32"/>
-      <c r="N101" s="30"/>
+      <c r="L101" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M101" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N101" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O101" s="46"/>
-      <c r="P101" s="39"/>
-      <c r="Q101" s="39"/>
+      <c r="P101" s="46">
+        <v>29.608050847457601</v>
+      </c>
+      <c r="Q101" s="46">
+        <v>3.2838983050847399</v>
+      </c>
       <c r="R101" s="46"/>
       <c r="S101" s="37"/>
       <c r="T101" s="37"/>
     </row>
     <row r="102" spans="1:20" ht="18" customHeight="1">
       <c r="A102" s="30"/>
-      <c r="B102" s="31"/>
-      <c r="C102" s="30"/>
-      <c r="D102" s="30"/>
+      <c r="B102" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C102" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E102" s="31"/>
-      <c r="F102" s="32"/>
-      <c r="G102" s="32"/>
+      <c r="F102" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G102" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H102" s="33"/>
-      <c r="I102" s="38"/>
-      <c r="J102" s="49"/>
+      <c r="I102" s="34">
+        <v>298</v>
+      </c>
+      <c r="J102" s="39">
+        <f t="shared" si="3"/>
+        <v>11.864406779660985</v>
+      </c>
       <c r="K102" s="49"/>
-      <c r="L102" s="32"/>
-      <c r="M102" s="32"/>
-      <c r="N102" s="30"/>
+      <c r="L102" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="M102" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N102" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O102" s="46"/>
-      <c r="P102" s="39"/>
-      <c r="Q102" s="39"/>
+      <c r="P102" s="46">
+        <v>11.917372881355901</v>
+      </c>
+      <c r="Q102" s="37">
+        <v>5.2966101694916001E-2</v>
+      </c>
       <c r="R102" s="46"/>
       <c r="S102" s="37"/>
       <c r="T102" s="37"/>
     </row>
     <row r="103" spans="1:20" ht="18" customHeight="1">
       <c r="A103" s="51"/>
-      <c r="B103" s="31"/>
-      <c r="C103" s="30"/>
-      <c r="D103" s="30"/>
+      <c r="B103" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C103" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E103" s="31"/>
-      <c r="F103" s="32"/>
-      <c r="G103" s="32"/>
+      <c r="F103" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G103" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H103" s="33"/>
-      <c r="I103" s="38"/>
-      <c r="J103" s="49"/>
+      <c r="I103" s="38">
+        <v>298</v>
+      </c>
+      <c r="J103" s="49">
+        <v>1500000000</v>
+      </c>
       <c r="K103" s="49"/>
-      <c r="L103" s="32"/>
-      <c r="M103" s="32"/>
-      <c r="N103" s="30"/>
+      <c r="L103" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M103" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N103" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O103" s="46"/>
       <c r="P103" s="39"/>
       <c r="Q103" s="39"/>
@@ -7332,19 +7649,39 @@
     </row>
     <row r="104" spans="1:20" ht="18" customHeight="1">
       <c r="A104" s="51"/>
-      <c r="B104" s="31"/>
-      <c r="C104" s="30"/>
-      <c r="D104" s="30"/>
+      <c r="B104" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C104" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D104" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E104" s="31"/>
-      <c r="F104" s="32"/>
-      <c r="G104" s="32"/>
+      <c r="F104" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G104" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H104" s="33"/>
-      <c r="I104" s="38"/>
-      <c r="J104" s="39"/>
+      <c r="I104" s="38">
+        <v>298</v>
+      </c>
+      <c r="J104" s="39">
+        <v>2012000000</v>
+      </c>
       <c r="K104" s="49"/>
-      <c r="L104" s="32"/>
-      <c r="M104" s="32"/>
-      <c r="N104" s="30"/>
+      <c r="L104" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M104" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N104" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O104" s="46"/>
       <c r="P104" s="39"/>
       <c r="Q104" s="39"/>
@@ -7354,19 +7691,39 @@
     </row>
     <row r="105" spans="1:20" ht="18" customHeight="1">
       <c r="A105" s="51"/>
-      <c r="B105" s="31"/>
-      <c r="C105" s="30"/>
-      <c r="D105" s="30"/>
+      <c r="B105" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C105" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>68</v>
+      </c>
       <c r="E105" s="31"/>
-      <c r="F105" s="32"/>
-      <c r="G105" s="32"/>
+      <c r="F105" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G105" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H105" s="33"/>
-      <c r="I105" s="38"/>
-      <c r="J105" s="52"/>
+      <c r="I105" s="38">
+        <v>298</v>
+      </c>
+      <c r="J105" s="52">
+        <v>2453000000</v>
+      </c>
       <c r="K105" s="49"/>
-      <c r="L105" s="32"/>
-      <c r="M105" s="32"/>
-      <c r="N105" s="30"/>
+      <c r="L105" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="M105" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N105" s="30" t="s">
+        <v>156</v>
+      </c>
       <c r="O105" s="46"/>
       <c r="P105" s="39"/>
       <c r="Q105" s="39"/>

</xml_diff>

<commit_message>
- parsed `10.3390/e21050483 `
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D5261E-4E81-3441-985E-DF6AD9CC4DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E7C70-911C-7142-8FFA-F0B389259F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="176">
   <si>
     <r>
       <rPr>
@@ -324,6 +324,9 @@
     <t>AAM</t>
   </si>
   <si>
+    <t>BCC</t>
+  </si>
+  <si>
     <t>compressive yield stress</t>
   </si>
   <si>
@@ -358,6 +361,9 @@
   </si>
   <si>
     <t>hardness HV</t>
+  </si>
+  <si>
+    <t>F3</t>
   </si>
   <si>
     <t>amorphous</t>
@@ -626,6 +632,33 @@
   </si>
   <si>
     <t>CoCrFeNiTa0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.3390/e21050483 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TiNbTaZr </t>
+  </si>
+  <si>
+    <t>TiNbTaZrV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TiNbTaZrMo </t>
+  </si>
+  <si>
+    <t>TiNbTaZrW</t>
+  </si>
+  <si>
+    <t>high quality AAM with 10 times 180s melting events</t>
+  </si>
+  <si>
+    <t>BCC+BCC</t>
+  </si>
+  <si>
+    <t>AAM+CCLM(LM)</t>
+  </si>
+  <si>
+    <t>high quality AAM with 10 times 180s melting events; cold crucible levitation melted (CCLM) ingots with superior homogenity</t>
   </si>
 </sst>
 </file>
@@ -3113,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T962"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A83" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3366,7 +3399,7 @@
       </c>
       <c r="O7" s="104"/>
       <c r="P7" s="69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="69" t="s">
         <v>36</v>
@@ -3472,23 +3505,23 @@
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="72" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C10" s="73" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E10" s="72"/>
       <c r="F10" s="74" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="75" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I10" s="76">
         <v>298</v>
@@ -3504,7 +3537,7 @@
       </c>
       <c r="M10" s="74"/>
       <c r="N10" s="78" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O10" s="79"/>
       <c r="P10" s="80"/>
@@ -3516,23 +3549,23 @@
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="30"/>
       <c r="B11" s="72" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D11" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E11" s="72"/>
       <c r="F11" s="32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G11" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I11" s="76">
         <v>298</v>
@@ -3548,7 +3581,7 @@
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="78" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O11" s="37"/>
       <c r="P11" s="38"/>
@@ -3560,23 +3593,23 @@
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="30"/>
       <c r="B12" s="72" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D12" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="72"/>
       <c r="F12" s="32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G12" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H12" s="75" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I12" s="76">
         <v>298</v>
@@ -3588,11 +3621,11 @@
         <v>0.3</v>
       </c>
       <c r="L12" s="74" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M12" s="32"/>
       <c r="N12" s="78" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O12" s="37"/>
       <c r="P12" s="38"/>
@@ -3604,25 +3637,25 @@
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="30"/>
       <c r="B13" s="72" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D13" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G13" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I13" s="76">
         <v>298</v>
@@ -3635,10 +3668,10 @@
         <v>33</v>
       </c>
       <c r="M13" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N13" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O13" s="37"/>
       <c r="P13" s="38"/>
@@ -3650,25 +3683,25 @@
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="30"/>
       <c r="B14" s="72" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D14" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G14" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I14" s="76">
         <v>298</v>
@@ -3681,10 +3714,10 @@
         <v>33</v>
       </c>
       <c r="M14" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N14" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O14" s="37"/>
       <c r="P14" s="38"/>
@@ -3696,25 +3729,25 @@
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="72" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D15" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G15" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I15" s="76">
         <v>298</v>
@@ -3727,10 +3760,10 @@
         <v>33</v>
       </c>
       <c r="M15" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N15" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
@@ -3742,25 +3775,25 @@
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="30"/>
       <c r="B16" s="72" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D16" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G16" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I16" s="76">
         <v>298</v>
@@ -3773,10 +3806,10 @@
         <v>33</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N16" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O16" s="37"/>
       <c r="P16" s="37"/>
@@ -3788,25 +3821,25 @@
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="38"/>
       <c r="B17" s="72" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D17" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G17" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I17" s="76">
         <v>298</v>
@@ -3819,10 +3852,10 @@
         <v>33</v>
       </c>
       <c r="M17" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N17" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O17" s="37"/>
       <c r="P17" s="37"/>
@@ -3834,25 +3867,25 @@
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="38"/>
       <c r="B18" s="72" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D18" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G18" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I18" s="76">
         <v>298</v>
@@ -3865,10 +3898,10 @@
         <v>33</v>
       </c>
       <c r="M18" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N18" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O18" s="37"/>
       <c r="P18" s="37"/>
@@ -3880,25 +3913,25 @@
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="38"/>
       <c r="B19" s="72" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C19" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D19" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G19" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I19" s="76">
         <v>298</v>
@@ -3911,10 +3944,10 @@
         <v>33</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N19" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
@@ -3926,25 +3959,25 @@
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="38"/>
       <c r="B20" s="72" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C20" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D20" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G20" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I20" s="76">
         <v>298</v>
@@ -3957,10 +3990,10 @@
         <v>33</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N20" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
@@ -3972,25 +4005,25 @@
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="38"/>
       <c r="B21" s="72" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C21" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D21" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G21" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I21" s="76">
         <v>298</v>
@@ -4000,13 +4033,13 @@
       </c>
       <c r="K21" s="38"/>
       <c r="L21" s="74" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N21" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O21" s="37"/>
       <c r="P21" s="37"/>
@@ -4018,25 +4051,25 @@
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="38"/>
       <c r="B22" s="72" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C22" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D22" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G22" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I22" s="76">
         <v>298</v>
@@ -4046,13 +4079,13 @@
       </c>
       <c r="K22" s="35"/>
       <c r="L22" s="74" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N22" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O22" s="37"/>
       <c r="P22" s="37"/>
@@ -4064,25 +4097,25 @@
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="30"/>
       <c r="B23" s="72" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C23" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D23" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G23" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I23" s="76">
         <v>298</v>
@@ -4092,13 +4125,13 @@
       </c>
       <c r="K23" s="62"/>
       <c r="L23" s="74" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M23" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N23" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O23" s="37"/>
       <c r="P23" s="37"/>
@@ -4110,25 +4143,25 @@
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="30"/>
       <c r="B24" s="72" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C24" s="73" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D24" s="73" t="s">
         <v>63</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G24" s="74" t="s">
         <v>29</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I24" s="76">
         <v>298</v>
@@ -4138,13 +4171,13 @@
       </c>
       <c r="K24" s="62"/>
       <c r="L24" s="74" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N24" s="78" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O24" s="37"/>
       <c r="P24" s="37"/>
@@ -4155,22 +4188,22 @@
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
       <c r="A25" s="139" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="140" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="140" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>103</v>
-      </c>
       <c r="F25" s="32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G25" s="32" t="s">
         <v>29</v>
@@ -4182,13 +4215,13 @@
       </c>
       <c r="K25" s="62"/>
       <c r="L25" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M25" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N25" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O25" s="37"/>
       <c r="P25" s="38"/>
@@ -4199,22 +4232,22 @@
     </row>
     <row r="26" spans="1:20" ht="18.75" customHeight="1">
       <c r="A26" s="30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G26" s="32" t="s">
         <v>29</v>
@@ -4226,13 +4259,13 @@
       </c>
       <c r="K26" s="62"/>
       <c r="L26" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M26" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N26" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O26" s="37"/>
       <c r="P26" s="43"/>
@@ -4243,22 +4276,22 @@
     </row>
     <row r="27" spans="1:20" ht="18.75" customHeight="1">
       <c r="A27" s="30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G27" s="32" t="s">
         <v>29</v>
@@ -4270,13 +4303,13 @@
       </c>
       <c r="K27" s="62"/>
       <c r="L27" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M27" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N27" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O27" s="37"/>
       <c r="P27" s="43"/>
@@ -4287,22 +4320,22 @@
     </row>
     <row r="28" spans="1:20" ht="18.75" customHeight="1">
       <c r="A28" s="30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>29</v>
@@ -4314,13 +4347,13 @@
       </c>
       <c r="K28" s="62"/>
       <c r="L28" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M28" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O28" s="37"/>
       <c r="P28" s="43"/>
@@ -4331,22 +4364,22 @@
     </row>
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
       <c r="A29" s="139" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="140" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="140" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>103</v>
-      </c>
       <c r="F29" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>29</v>
@@ -4358,13 +4391,13 @@
       </c>
       <c r="K29" s="62"/>
       <c r="L29" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M29" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N29" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O29" s="37"/>
       <c r="P29" s="43"/>
@@ -4375,22 +4408,22 @@
     </row>
     <row r="30" spans="1:20" ht="18.75" customHeight="1">
       <c r="A30" s="30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G30" s="32" t="s">
         <v>29</v>
@@ -4402,13 +4435,13 @@
       </c>
       <c r="K30" s="62"/>
       <c r="L30" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M30" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N30" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O30" s="37"/>
       <c r="P30" s="43"/>
@@ -4419,22 +4452,22 @@
     </row>
     <row r="31" spans="1:20" ht="18.75" customHeight="1">
       <c r="A31" s="30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G31" s="32" t="s">
         <v>29</v>
@@ -4446,13 +4479,13 @@
       </c>
       <c r="K31" s="62"/>
       <c r="L31" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M31" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N31" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O31" s="37"/>
       <c r="P31" s="43"/>
@@ -4463,22 +4496,22 @@
     </row>
     <row r="32" spans="1:20" ht="18.75" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G32" s="32" t="s">
         <v>29</v>
@@ -4490,13 +4523,13 @@
       </c>
       <c r="K32" s="62"/>
       <c r="L32" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M32" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N32" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O32" s="37"/>
       <c r="P32" s="43"/>
@@ -4507,28 +4540,28 @@
     </row>
     <row r="33" spans="1:20" ht="18.75" customHeight="1">
       <c r="A33" s="30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H33" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I33" s="34"/>
       <c r="J33" s="62">
@@ -4536,13 +4569,13 @@
       </c>
       <c r="K33" s="62"/>
       <c r="L33" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M33" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N33" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O33" s="37"/>
       <c r="P33" s="43"/>
@@ -4553,28 +4586,28 @@
     </row>
     <row r="34" spans="1:20" ht="18.75" customHeight="1">
       <c r="A34" s="30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G34" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H34" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I34" s="34"/>
       <c r="J34" s="62">
@@ -4582,13 +4615,13 @@
       </c>
       <c r="K34" s="62"/>
       <c r="L34" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M34" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N34" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O34" s="37"/>
       <c r="P34" s="38"/>
@@ -4599,28 +4632,28 @@
     </row>
     <row r="35" spans="1:20" ht="18.75" customHeight="1">
       <c r="A35" s="30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G35" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I35" s="34"/>
       <c r="J35" s="38">
@@ -4628,13 +4661,13 @@
       </c>
       <c r="K35" s="38"/>
       <c r="L35" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M35" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N35" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O35" s="37"/>
       <c r="P35" s="38"/>
@@ -4645,28 +4678,28 @@
     </row>
     <row r="36" spans="1:20" ht="18.75" customHeight="1">
       <c r="A36" s="30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G36" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="38">
@@ -4674,13 +4707,13 @@
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M36" s="40" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N36" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O36" s="37"/>
       <c r="P36" s="38"/>
@@ -4691,28 +4724,28 @@
     </row>
     <row r="37" spans="1:20" ht="18.75" customHeight="1">
       <c r="A37" s="30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G37" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H37" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I37" s="34"/>
       <c r="J37" s="38">
@@ -4720,13 +4753,13 @@
       </c>
       <c r="K37" s="35"/>
       <c r="L37" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M37" s="40" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N37" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O37" s="37"/>
       <c r="P37" s="38"/>
@@ -4737,28 +4770,28 @@
     </row>
     <row r="38" spans="1:20" ht="18.75" customHeight="1">
       <c r="A38" s="30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G38" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="38">
@@ -4766,13 +4799,13 @@
       </c>
       <c r="K38" s="35"/>
       <c r="L38" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M38" s="40" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N38" s="36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O38" s="46"/>
       <c r="P38" s="39"/>
@@ -4784,25 +4817,25 @@
     <row r="39" spans="1:20" ht="18.75" customHeight="1">
       <c r="A39" s="30"/>
       <c r="B39" s="41" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G39" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I39" s="34"/>
       <c r="J39" s="38">
@@ -4810,13 +4843,13 @@
       </c>
       <c r="K39" s="35"/>
       <c r="L39" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M39" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N39" s="36" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="O39" s="46"/>
       <c r="P39" s="39"/>
@@ -4828,23 +4861,23 @@
     <row r="40" spans="1:20" ht="18.75" customHeight="1">
       <c r="A40" s="30"/>
       <c r="B40" s="41" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G40" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H40" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="46">
@@ -4852,11 +4885,11 @@
       </c>
       <c r="K40" s="47"/>
       <c r="L40" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M40" s="40"/>
       <c r="N40" s="36" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O40" s="46"/>
       <c r="P40" s="39"/>
@@ -4868,23 +4901,23 @@
     <row r="41" spans="1:20" ht="18.75" customHeight="1">
       <c r="A41" s="30"/>
       <c r="B41" s="41" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G41" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I41" s="34"/>
       <c r="J41" s="94">
@@ -4892,11 +4925,11 @@
       </c>
       <c r="K41" s="47"/>
       <c r="L41" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M41" s="40"/>
       <c r="N41" s="36" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O41" s="46"/>
       <c r="P41" s="39"/>
@@ -4908,23 +4941,23 @@
     <row r="42" spans="1:20" ht="18.75" customHeight="1">
       <c r="A42" s="30"/>
       <c r="B42" s="41" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G42" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H42" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I42" s="34"/>
       <c r="J42" s="94">
@@ -4932,11 +4965,11 @@
       </c>
       <c r="K42" s="47"/>
       <c r="L42" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M42" s="40"/>
       <c r="N42" s="36" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="O42" s="46"/>
       <c r="P42" s="47"/>
@@ -4948,23 +4981,23 @@
     <row r="43" spans="1:20" ht="18" customHeight="1">
       <c r="A43" s="30"/>
       <c r="B43" s="41" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G43" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H43" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="94">
@@ -4972,11 +5005,11 @@
       </c>
       <c r="K43" s="47"/>
       <c r="L43" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M43" s="40"/>
       <c r="N43" s="36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O43" s="46"/>
       <c r="P43" s="47"/>
@@ -4988,23 +5021,23 @@
     <row r="44" spans="1:20" ht="18" customHeight="1">
       <c r="A44" s="30"/>
       <c r="B44" s="41" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G44" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I44" s="34"/>
       <c r="J44" s="94">
@@ -5012,11 +5045,11 @@
       </c>
       <c r="K44" s="49"/>
       <c r="L44" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M44" s="40"/>
       <c r="N44" s="141" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="O44" s="46"/>
       <c r="P44" s="46"/>
@@ -5028,23 +5061,23 @@
     <row r="45" spans="1:20" ht="18" customHeight="1">
       <c r="A45" s="30"/>
       <c r="B45" s="41" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G45" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="46">
@@ -5052,11 +5085,11 @@
       </c>
       <c r="K45" s="49"/>
       <c r="L45" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M45" s="40"/>
       <c r="N45" s="141" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="O45" s="46"/>
       <c r="P45" s="46"/>
@@ -5068,25 +5101,25 @@
     <row r="46" spans="1:20" ht="18" customHeight="1">
       <c r="A46" s="30"/>
       <c r="B46" s="41" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G46" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H46" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I46" s="34"/>
       <c r="J46" s="38">
@@ -5094,13 +5127,13 @@
       </c>
       <c r="K46" s="35"/>
       <c r="L46" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M46" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N46" s="36" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="O46" s="46"/>
       <c r="P46" s="46"/>
@@ -5112,23 +5145,23 @@
     <row r="47" spans="1:20" ht="18" customHeight="1">
       <c r="A47" s="30"/>
       <c r="B47" s="41" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G47" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H47" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I47" s="34"/>
       <c r="J47" s="46">
@@ -5136,11 +5169,11 @@
       </c>
       <c r="K47" s="47"/>
       <c r="L47" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M47" s="40"/>
       <c r="N47" s="36" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O47" s="46"/>
       <c r="P47" s="46"/>
@@ -5152,23 +5185,23 @@
     <row r="48" spans="1:20" ht="18" customHeight="1">
       <c r="A48" s="30"/>
       <c r="B48" s="41" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G48" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I48" s="34"/>
       <c r="J48" s="94">
@@ -5176,11 +5209,11 @@
       </c>
       <c r="K48" s="47"/>
       <c r="L48" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M48" s="40"/>
       <c r="N48" s="36" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O48" s="46"/>
       <c r="P48" s="46"/>
@@ -5192,23 +5225,23 @@
     <row r="49" spans="1:20" ht="18" customHeight="1">
       <c r="A49" s="30"/>
       <c r="B49" s="41" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G49" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="94">
@@ -5216,11 +5249,11 @@
       </c>
       <c r="K49" s="47"/>
       <c r="L49" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M49" s="40"/>
       <c r="N49" s="36" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="O49" s="46"/>
       <c r="P49" s="46"/>
@@ -5232,23 +5265,23 @@
     <row r="50" spans="1:20" ht="18" customHeight="1">
       <c r="A50" s="30"/>
       <c r="B50" s="41" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G50" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I50" s="34"/>
       <c r="J50" s="94">
@@ -5256,11 +5289,11 @@
       </c>
       <c r="K50" s="47"/>
       <c r="L50" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M50" s="40"/>
       <c r="N50" s="36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O50" s="46"/>
       <c r="P50" s="46"/>
@@ -5272,23 +5305,23 @@
     <row r="51" spans="1:20" ht="18" customHeight="1">
       <c r="A51" s="30"/>
       <c r="B51" s="41" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G51" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I51" s="34"/>
       <c r="J51" s="94">
@@ -5296,11 +5329,11 @@
       </c>
       <c r="K51" s="49"/>
       <c r="L51" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M51" s="40"/>
       <c r="N51" s="141" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="O51" s="46"/>
       <c r="P51" s="46"/>
@@ -5312,23 +5345,23 @@
     <row r="52" spans="1:20" ht="18" customHeight="1">
       <c r="A52" s="30"/>
       <c r="B52" s="41" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F52" s="32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G52" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I52" s="34"/>
       <c r="J52" s="46">
@@ -5336,11 +5369,11 @@
       </c>
       <c r="K52" s="49"/>
       <c r="L52" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M52" s="40"/>
       <c r="N52" s="141" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="O52" s="46"/>
       <c r="P52" s="47"/>
@@ -5352,25 +5385,25 @@
     <row r="53" spans="1:20" ht="18" customHeight="1">
       <c r="A53" s="30"/>
       <c r="B53" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C53" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D53" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E53" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F53" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G53" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H53" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I53" s="34"/>
       <c r="J53" s="49">
@@ -5378,13 +5411,13 @@
       </c>
       <c r="K53" s="49"/>
       <c r="L53" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M53" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N53" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O53" s="46"/>
       <c r="P53" s="47"/>
@@ -5396,25 +5429,25 @@
     <row r="54" spans="1:20" ht="18" customHeight="1">
       <c r="A54" s="30"/>
       <c r="B54" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C54" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D54" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E54" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F54" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G54" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H54" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I54" s="34"/>
       <c r="J54" s="49">
@@ -5422,13 +5455,13 @@
       </c>
       <c r="K54" s="49"/>
       <c r="L54" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M54" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N54" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O54" s="46"/>
       <c r="P54" s="47"/>
@@ -5440,25 +5473,25 @@
     <row r="55" spans="1:20" ht="18" customHeight="1">
       <c r="A55" s="30"/>
       <c r="B55" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C55" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D55" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E55" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F55" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G55" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="49">
@@ -5466,13 +5499,13 @@
       </c>
       <c r="K55" s="49"/>
       <c r="L55" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M55" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N55" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O55" s="46"/>
       <c r="P55" s="47"/>
@@ -5484,25 +5517,25 @@
     <row r="56" spans="1:20" ht="18" customHeight="1">
       <c r="A56" s="30"/>
       <c r="B56" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C56" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D56" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E56" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F56" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G56" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I56" s="34"/>
       <c r="J56" s="49">
@@ -5510,13 +5543,13 @@
       </c>
       <c r="K56" s="49"/>
       <c r="L56" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M56" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N56" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O56" s="46"/>
       <c r="P56" s="46"/>
@@ -5528,25 +5561,25 @@
     <row r="57" spans="1:20" ht="18" customHeight="1">
       <c r="A57" s="30"/>
       <c r="B57" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F57" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G57" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H57" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I57" s="34"/>
       <c r="J57" s="49">
@@ -5554,13 +5587,13 @@
       </c>
       <c r="K57" s="49"/>
       <c r="L57" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M57" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N57" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O57" s="46"/>
       <c r="P57" s="46"/>
@@ -5572,25 +5605,25 @@
     <row r="58" spans="1:20" ht="18" customHeight="1">
       <c r="A58" s="30"/>
       <c r="B58" s="31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F58" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G58" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H58" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="49">
@@ -5598,13 +5631,13 @@
       </c>
       <c r="K58" s="49"/>
       <c r="L58" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M58" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N58" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O58" s="46"/>
       <c r="P58" s="46"/>
@@ -5616,25 +5649,25 @@
     <row r="59" spans="1:20" ht="18" customHeight="1">
       <c r="A59" s="30"/>
       <c r="B59" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C59" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D59" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E59" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F59" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G59" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I59" s="34"/>
       <c r="J59" s="49">
@@ -5642,13 +5675,13 @@
       </c>
       <c r="K59" s="49"/>
       <c r="L59" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M59" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N59" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O59" s="46"/>
       <c r="P59" s="46"/>
@@ -5660,25 +5693,25 @@
     <row r="60" spans="1:20" ht="18" customHeight="1">
       <c r="A60" s="30"/>
       <c r="B60" s="31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C60" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D60" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D60" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E60" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F60" s="48" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G60" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H60" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I60" s="34"/>
       <c r="J60" s="49">
@@ -5686,13 +5719,13 @@
       </c>
       <c r="K60" s="49"/>
       <c r="L60" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M60" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N60" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O60" s="46"/>
       <c r="P60" s="46"/>
@@ -5704,25 +5737,25 @@
     <row r="61" spans="1:20" ht="18" customHeight="1">
       <c r="A61" s="30"/>
       <c r="B61" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C61" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D61" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E61" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F61" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G61" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H61" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I61" s="34"/>
       <c r="J61" s="49">
@@ -5730,13 +5763,13 @@
       </c>
       <c r="K61" s="49"/>
       <c r="L61" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M61" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N61" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O61" s="46"/>
       <c r="P61" s="46"/>
@@ -5748,25 +5781,25 @@
     <row r="62" spans="1:20" ht="18" customHeight="1">
       <c r="A62" s="30"/>
       <c r="B62" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C62" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D62" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E62" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F62" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G62" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H62" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="49">
@@ -5774,13 +5807,13 @@
       </c>
       <c r="K62" s="49"/>
       <c r="L62" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M62" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N62" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O62" s="46"/>
       <c r="P62" s="46"/>
@@ -5792,25 +5825,25 @@
     <row r="63" spans="1:20" ht="18" customHeight="1">
       <c r="A63" s="30"/>
       <c r="B63" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C63" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D63" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D63" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E63" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F63" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G63" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H63" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I63" s="34"/>
       <c r="J63" s="49">
@@ -5818,13 +5851,13 @@
       </c>
       <c r="K63" s="49"/>
       <c r="L63" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M63" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N63" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O63" s="46"/>
       <c r="P63" s="46"/>
@@ -5836,25 +5869,25 @@
     <row r="64" spans="1:20" ht="18" customHeight="1">
       <c r="A64" s="30"/>
       <c r="B64" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C64" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D64" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E64" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F64" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G64" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H64" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I64" s="34"/>
       <c r="J64" s="49">
@@ -5862,13 +5895,13 @@
       </c>
       <c r="K64" s="49"/>
       <c r="L64" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M64" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N64" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O64" s="46"/>
       <c r="P64" s="46"/>
@@ -5880,25 +5913,25 @@
     <row r="65" spans="1:20" ht="18" customHeight="1">
       <c r="A65" s="30"/>
       <c r="B65" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E65" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F65" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G65" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H65" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I65" s="34"/>
       <c r="J65" s="49">
@@ -5906,13 +5939,13 @@
       </c>
       <c r="K65" s="49"/>
       <c r="L65" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M65" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N65" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O65" s="46"/>
       <c r="P65" s="46"/>
@@ -5924,25 +5957,25 @@
     <row r="66" spans="1:20" ht="18" customHeight="1">
       <c r="A66" s="30"/>
       <c r="B66" s="31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D66" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F66" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G66" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H66" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I66" s="34"/>
       <c r="J66" s="94">
@@ -5950,13 +5983,13 @@
       </c>
       <c r="K66" s="47"/>
       <c r="L66" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M66" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N66" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O66" s="46"/>
       <c r="P66" s="46"/>
@@ -5968,25 +6001,25 @@
     <row r="67" spans="1:20" ht="18" customHeight="1">
       <c r="A67" s="30"/>
       <c r="B67" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C67" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D67" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D67" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E67" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F67" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G67" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H67" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I67" s="34"/>
       <c r="J67" s="46">
@@ -5994,13 +6027,13 @@
       </c>
       <c r="K67" s="47"/>
       <c r="L67" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M67" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N67" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O67" s="46"/>
       <c r="P67" s="46"/>
@@ -6012,25 +6045,25 @@
     <row r="68" spans="1:20" ht="18" customHeight="1">
       <c r="A68" s="30"/>
       <c r="B68" s="31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C68" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D68" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E68" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F68" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G68" s="32" t="s">
         <v>29</v>
       </c>
       <c r="H68" s="34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="46">
@@ -6038,13 +6071,13 @@
       </c>
       <c r="K68" s="47"/>
       <c r="L68" s="50" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M68" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N68" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O68" s="46"/>
       <c r="P68" s="46"/>
@@ -6056,16 +6089,16 @@
     <row r="69" spans="1:20" ht="18" customHeight="1">
       <c r="A69" s="30"/>
       <c r="B69" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C69" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D69" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E69" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F69" s="48" t="s">
         <v>62</v>
@@ -6089,10 +6122,10 @@
         <v>33</v>
       </c>
       <c r="M69" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N69" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O69" s="46"/>
       <c r="P69" s="46">
@@ -6108,16 +6141,16 @@
     <row r="70" spans="1:20" ht="18" customHeight="1">
       <c r="A70" s="30"/>
       <c r="B70" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C70" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D70" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D70" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E70" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F70" s="48" t="s">
         <v>62</v>
@@ -6141,10 +6174,10 @@
         <v>33</v>
       </c>
       <c r="M70" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N70" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O70" s="46"/>
       <c r="P70" s="46">
@@ -6160,16 +6193,16 @@
     <row r="71" spans="1:20" ht="18" customHeight="1">
       <c r="A71" s="30"/>
       <c r="B71" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C71" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D71" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D71" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E71" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F71" s="48" t="s">
         <v>62</v>
@@ -6193,10 +6226,10 @@
         <v>33</v>
       </c>
       <c r="M71" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N71" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O71" s="46"/>
       <c r="P71" s="1">
@@ -6212,16 +6245,16 @@
     <row r="72" spans="1:20" ht="18" customHeight="1">
       <c r="A72" s="30"/>
       <c r="B72" s="31" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C72" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D72" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D72" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E72" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F72" s="48" t="s">
         <v>62</v>
@@ -6245,10 +6278,10 @@
         <v>33</v>
       </c>
       <c r="M72" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N72" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O72" s="46"/>
       <c r="P72" s="47">
@@ -6264,16 +6297,16 @@
     <row r="73" spans="1:20" ht="18" customHeight="1">
       <c r="A73" s="30"/>
       <c r="B73" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E73" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F73" s="48" t="s">
         <v>62</v>
@@ -6297,10 +6330,10 @@
         <v>33</v>
       </c>
       <c r="M73" s="50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N73" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O73" s="46"/>
       <c r="P73" s="46">
@@ -6316,16 +6349,16 @@
     <row r="74" spans="1:20" ht="18" customHeight="1">
       <c r="A74" s="30"/>
       <c r="B74" s="31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E74" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F74" s="48" t="s">
         <v>62</v>
@@ -6349,10 +6382,10 @@
         <v>33</v>
       </c>
       <c r="M74" s="50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N74" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O74" s="46"/>
       <c r="P74" s="46">
@@ -6368,16 +6401,16 @@
     <row r="75" spans="1:20" ht="18" customHeight="1">
       <c r="A75" s="30"/>
       <c r="B75" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C75" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D75" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D75" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E75" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F75" s="48" t="s">
         <v>62</v>
@@ -6401,10 +6434,10 @@
         <v>33</v>
       </c>
       <c r="M75" s="50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N75" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O75" s="46"/>
       <c r="P75" s="46">
@@ -6420,16 +6453,16 @@
     <row r="76" spans="1:20" ht="18" customHeight="1">
       <c r="A76" s="30"/>
       <c r="B76" s="31" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C76" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D76" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D76" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E76" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F76" s="48" t="s">
         <v>62</v>
@@ -6453,10 +6486,10 @@
         <v>33</v>
       </c>
       <c r="M76" s="50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N76" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O76" s="46"/>
       <c r="P76" s="46">
@@ -6472,19 +6505,19 @@
     <row r="77" spans="1:20" ht="18" customHeight="1">
       <c r="A77" s="30"/>
       <c r="B77" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C77" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D77" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D77" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E77" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F77" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G77" s="32" t="s">
         <v>29</v>
@@ -6501,10 +6534,10 @@
         <v>33</v>
       </c>
       <c r="M77" s="50" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N77" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O77" s="46"/>
       <c r="P77" s="49"/>
@@ -6516,19 +6549,19 @@
     <row r="78" spans="1:20" ht="18" customHeight="1">
       <c r="A78" s="30"/>
       <c r="B78" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C78" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D78" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D78" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E78" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F78" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G78" s="32" t="s">
         <v>29</v>
@@ -6545,10 +6578,10 @@
         <v>33</v>
       </c>
       <c r="M78" s="50" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N78" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O78" s="46"/>
       <c r="P78" s="49"/>
@@ -6560,19 +6593,19 @@
     <row r="79" spans="1:20" ht="18" customHeight="1">
       <c r="A79" s="30"/>
       <c r="B79" s="31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E79" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F79" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G79" s="32" t="s">
         <v>29</v>
@@ -6589,10 +6622,10 @@
         <v>33</v>
       </c>
       <c r="M79" s="50" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N79" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O79" s="46"/>
       <c r="P79" s="46"/>
@@ -6604,19 +6637,19 @@
     <row r="80" spans="1:20" ht="18" customHeight="1">
       <c r="A80" s="30"/>
       <c r="B80" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C80" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D80" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D80" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E80" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F80" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G80" s="32" t="s">
         <v>29</v>
@@ -6630,13 +6663,13 @@
       </c>
       <c r="K80" s="35"/>
       <c r="L80" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M80" s="50" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N80" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O80" s="46"/>
       <c r="P80" s="39"/>
@@ -6648,19 +6681,19 @@
     <row r="81" spans="1:20" ht="18" customHeight="1">
       <c r="A81" s="30"/>
       <c r="B81" s="31" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C81" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D81" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="D81" s="30" t="s">
-        <v>139</v>
-      </c>
       <c r="E81" s="31" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F81" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G81" s="32" t="s">
         <v>29</v>
@@ -6674,13 +6707,13 @@
       </c>
       <c r="K81" s="35"/>
       <c r="L81" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M81" s="50" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N81" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O81" s="46"/>
       <c r="P81" s="39"/>
@@ -6692,19 +6725,19 @@
     <row r="82" spans="1:20" ht="18" customHeight="1">
       <c r="A82" s="30"/>
       <c r="B82" s="31" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D82" s="30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E82" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F82" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G82" s="32" t="s">
         <v>29</v>
@@ -6718,13 +6751,13 @@
       </c>
       <c r="K82" s="35"/>
       <c r="L82" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M82" s="50" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N82" s="30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="O82" s="46"/>
       <c r="P82" s="39"/>
@@ -6736,19 +6769,19 @@
     <row r="83" spans="1:20" ht="18" customHeight="1">
       <c r="A83" s="30"/>
       <c r="B83" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C83" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C83" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D83" s="30" t="s">
-        <v>148</v>
-      </c>
       <c r="E83" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F83" s="48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G83" s="32" t="s">
         <v>29</v>
@@ -6766,7 +6799,7 @@
       </c>
       <c r="M83" s="50"/>
       <c r="N83" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O83" s="46"/>
       <c r="P83" s="39"/>
@@ -6778,19 +6811,19 @@
     <row r="84" spans="1:20" ht="18" customHeight="1">
       <c r="A84" s="30"/>
       <c r="B84" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C84" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="C84" s="30" t="s">
-        <v>149</v>
-      </c>
       <c r="D84" s="30" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E84" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F84" s="48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G84" s="32" t="s">
         <v>29</v>
@@ -6808,7 +6841,7 @@
       </c>
       <c r="M84" s="50"/>
       <c r="N84" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O84" s="46"/>
       <c r="P84" s="39"/>
@@ -6820,19 +6853,19 @@
     <row r="85" spans="1:20" ht="18" customHeight="1">
       <c r="A85" s="30"/>
       <c r="B85" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D85" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C85" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D85" s="30" t="s">
-        <v>148</v>
-      </c>
       <c r="E85" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F85" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G85" s="32" t="s">
         <v>29</v>
@@ -6850,7 +6883,7 @@
       </c>
       <c r="M85" s="50"/>
       <c r="N85" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O85" s="46"/>
       <c r="P85" s="39"/>
@@ -6862,19 +6895,19 @@
     <row r="86" spans="1:20" ht="18" customHeight="1">
       <c r="A86" s="30"/>
       <c r="B86" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C86" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="C86" s="30" t="s">
-        <v>149</v>
-      </c>
       <c r="D86" s="30" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E86" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F86" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G86" s="32" t="s">
         <v>29</v>
@@ -6892,7 +6925,7 @@
       </c>
       <c r="M86" s="50"/>
       <c r="N86" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O86" s="46"/>
       <c r="P86" s="39"/>
@@ -6904,19 +6937,19 @@
     <row r="87" spans="1:20" ht="18" customHeight="1">
       <c r="A87" s="30"/>
       <c r="B87" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D87" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C87" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D87" s="30" t="s">
-        <v>148</v>
-      </c>
       <c r="E87" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F87" s="48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G87" s="32" t="s">
         <v>29</v>
@@ -6930,11 +6963,11 @@
       </c>
       <c r="K87" s="49"/>
       <c r="L87" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M87" s="50"/>
       <c r="N87" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O87" s="46"/>
       <c r="P87" s="39"/>
@@ -6946,19 +6979,19 @@
     <row r="88" spans="1:20" ht="18" customHeight="1">
       <c r="A88" s="30"/>
       <c r="B88" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C88" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="C88" s="30" t="s">
-        <v>149</v>
-      </c>
       <c r="D88" s="30" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E88" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F88" s="48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G88" s="32" t="s">
         <v>29</v>
@@ -6972,11 +7005,11 @@
       </c>
       <c r="K88" s="49"/>
       <c r="L88" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M88" s="50"/>
       <c r="N88" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O88" s="46"/>
       <c r="P88" s="39"/>
@@ -6988,17 +7021,17 @@
     <row r="89" spans="1:20" ht="18" customHeight="1">
       <c r="A89" s="30"/>
       <c r="B89" s="31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C89" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D89" s="30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E89" s="31"/>
       <c r="F89" s="48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G89" s="32" t="s">
         <v>29</v>
@@ -7016,7 +7049,7 @@
       </c>
       <c r="M89" s="50"/>
       <c r="N89" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O89" s="46"/>
       <c r="P89" s="39"/>
@@ -7028,17 +7061,17 @@
     <row r="90" spans="1:20" ht="18" customHeight="1">
       <c r="A90" s="30"/>
       <c r="B90" s="31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D90" s="30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E90" s="31"/>
       <c r="F90" s="32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G90" s="32" t="s">
         <v>29</v>
@@ -7056,7 +7089,7 @@
       </c>
       <c r="M90" s="50"/>
       <c r="N90" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O90" s="46"/>
       <c r="P90" s="39"/>
@@ -7068,17 +7101,17 @@
     <row r="91" spans="1:20" ht="18" customHeight="1">
       <c r="A91" s="30"/>
       <c r="B91" s="31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C91" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D91" s="30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E91" s="31"/>
       <c r="F91" s="32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G91" s="32" t="s">
         <v>29</v>
@@ -7092,11 +7125,11 @@
       </c>
       <c r="K91" s="49"/>
       <c r="L91" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M91" s="50"/>
       <c r="N91" s="30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O91" s="46"/>
       <c r="P91" s="47"/>
@@ -7108,13 +7141,13 @@
     <row r="92" spans="1:20" ht="18" customHeight="1">
       <c r="A92" s="30"/>
       <c r="B92" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C92" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D92" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E92" s="31"/>
       <c r="F92" s="32" t="s">
@@ -7136,10 +7169,10 @@
         <v>33</v>
       </c>
       <c r="M92" s="50" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N92" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O92" s="46"/>
       <c r="P92" s="47">
@@ -7153,17 +7186,17 @@
     <row r="93" spans="1:20" ht="18" customHeight="1">
       <c r="A93" s="30"/>
       <c r="B93" s="31" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C93" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D93" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E93" s="31"/>
       <c r="F93" s="32" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G93" s="32" t="s">
         <v>29</v>
@@ -7177,13 +7210,13 @@
       </c>
       <c r="K93" s="49"/>
       <c r="L93" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M93" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N93" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O93" s="46"/>
       <c r="P93" s="47"/>
@@ -7195,17 +7228,17 @@
     <row r="94" spans="1:20" ht="18" customHeight="1">
       <c r="A94" s="30"/>
       <c r="B94" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C94" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D94" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E94" s="31"/>
       <c r="F94" s="32" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G94" s="32" t="s">
         <v>29</v>
@@ -7219,13 +7252,13 @@
       </c>
       <c r="K94" s="49"/>
       <c r="L94" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M94" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N94" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O94" s="46"/>
       <c r="P94" s="47"/>
@@ -7237,17 +7270,17 @@
     <row r="95" spans="1:20" ht="18" customHeight="1">
       <c r="A95" s="30"/>
       <c r="B95" s="31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C95" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D95" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E95" s="31"/>
       <c r="F95" s="32" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G95" s="32" t="s">
         <v>29</v>
@@ -7261,13 +7294,13 @@
       </c>
       <c r="K95" s="49"/>
       <c r="L95" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M95" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N95" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O95" s="46"/>
       <c r="P95" s="47"/>
@@ -7279,17 +7312,17 @@
     <row r="96" spans="1:20" ht="18" customHeight="1">
       <c r="A96" s="30"/>
       <c r="B96" s="31" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C96" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D96" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E96" s="31"/>
       <c r="F96" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G96" s="32" t="s">
         <v>29</v>
@@ -7304,13 +7337,13 @@
       </c>
       <c r="K96" s="49"/>
       <c r="L96" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M96" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N96" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O96" s="46"/>
       <c r="P96" s="46">
@@ -7326,17 +7359,17 @@
     <row r="97" spans="1:20" ht="18" customHeight="1">
       <c r="A97" s="30"/>
       <c r="B97" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C97" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D97" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E97" s="31"/>
       <c r="F97" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G97" s="32" t="s">
         <v>29</v>
@@ -7351,13 +7384,13 @@
       </c>
       <c r="K97" s="49"/>
       <c r="L97" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M97" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N97" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O97" s="46"/>
       <c r="P97" s="46">
@@ -7373,17 +7406,17 @@
     <row r="98" spans="1:20" ht="18" customHeight="1">
       <c r="A98" s="30"/>
       <c r="B98" s="31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C98" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D98" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E98" s="31"/>
       <c r="F98" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G98" s="32" t="s">
         <v>29</v>
@@ -7398,13 +7431,13 @@
       </c>
       <c r="K98" s="49"/>
       <c r="L98" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M98" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N98" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O98" s="46"/>
       <c r="P98" s="46">
@@ -7420,17 +7453,17 @@
     <row r="99" spans="1:20" ht="18" customHeight="1">
       <c r="A99" s="30"/>
       <c r="B99" s="31" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C99" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E99" s="31"/>
       <c r="F99" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G99" s="32" t="s">
         <v>29</v>
@@ -7445,13 +7478,13 @@
       </c>
       <c r="K99" s="49"/>
       <c r="L99" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M99" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N99" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O99" s="46"/>
       <c r="P99" s="46">
@@ -7467,17 +7500,17 @@
     <row r="100" spans="1:20" ht="18" customHeight="1">
       <c r="A100" s="30"/>
       <c r="B100" s="31" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C100" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E100" s="31"/>
       <c r="F100" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G100" s="32" t="s">
         <v>29</v>
@@ -7492,13 +7525,13 @@
       </c>
       <c r="K100" s="49"/>
       <c r="L100" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M100" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N100" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O100" s="46"/>
       <c r="P100" s="46">
@@ -7514,17 +7547,17 @@
     <row r="101" spans="1:20" ht="18" customHeight="1">
       <c r="A101" s="30"/>
       <c r="B101" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C101" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E101" s="31"/>
       <c r="F101" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G101" s="32" t="s">
         <v>29</v>
@@ -7539,13 +7572,13 @@
       </c>
       <c r="K101" s="49"/>
       <c r="L101" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M101" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N101" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O101" s="46"/>
       <c r="P101" s="46">
@@ -7561,17 +7594,17 @@
     <row r="102" spans="1:20" ht="18" customHeight="1">
       <c r="A102" s="30"/>
       <c r="B102" s="31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C102" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E102" s="31"/>
       <c r="F102" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G102" s="32" t="s">
         <v>29</v>
@@ -7586,13 +7619,13 @@
       </c>
       <c r="K102" s="49"/>
       <c r="L102" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M102" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N102" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O102" s="46"/>
       <c r="P102" s="46">
@@ -7608,17 +7641,17 @@
     <row r="103" spans="1:20" ht="18" customHeight="1">
       <c r="A103" s="51"/>
       <c r="B103" s="31" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C103" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E103" s="31"/>
       <c r="F103" s="32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G103" s="32" t="s">
         <v>29</v>
@@ -7635,10 +7668,10 @@
         <v>33</v>
       </c>
       <c r="M103" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N103" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O103" s="46"/>
       <c r="P103" s="39"/>
@@ -7650,17 +7683,17 @@
     <row r="104" spans="1:20" ht="18" customHeight="1">
       <c r="A104" s="51"/>
       <c r="B104" s="31" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E104" s="31"/>
       <c r="F104" s="32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G104" s="32" t="s">
         <v>29</v>
@@ -7677,10 +7710,10 @@
         <v>33</v>
       </c>
       <c r="M104" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N104" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O104" s="46"/>
       <c r="P104" s="39"/>
@@ -7692,17 +7725,17 @@
     <row r="105" spans="1:20" ht="18" customHeight="1">
       <c r="A105" s="51"/>
       <c r="B105" s="31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D105" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E105" s="31"/>
       <c r="F105" s="32" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G105" s="32" t="s">
         <v>29</v>
@@ -7719,10 +7752,10 @@
         <v>33</v>
       </c>
       <c r="M105" s="50" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N105" s="30" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O105" s="46"/>
       <c r="P105" s="39"/>
@@ -7733,10 +7766,18 @@
     </row>
     <row r="106" spans="1:20" ht="18" customHeight="1">
       <c r="A106" s="51"/>
-      <c r="B106" s="31"/>
-      <c r="C106" s="30"/>
-      <c r="D106" s="30"/>
-      <c r="E106" s="31"/>
+      <c r="B106" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C106" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E106" s="31" t="s">
+        <v>172</v>
+      </c>
       <c r="F106" s="32"/>
       <c r="G106" s="32"/>
       <c r="H106" s="33"/>
@@ -7744,8 +7785,12 @@
       <c r="J106" s="52"/>
       <c r="K106" s="53"/>
       <c r="L106" s="32"/>
-      <c r="M106" s="32"/>
-      <c r="N106" s="30"/>
+      <c r="M106" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N106" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O106" s="46"/>
       <c r="P106" s="39"/>
       <c r="Q106" s="39"/>
@@ -7755,10 +7800,18 @@
     </row>
     <row r="107" spans="1:20" ht="18" customHeight="1">
       <c r="A107" s="51"/>
-      <c r="B107" s="31"/>
-      <c r="C107" s="30"/>
-      <c r="D107" s="30"/>
-      <c r="E107" s="31"/>
+      <c r="B107" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C107" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>172</v>
+      </c>
       <c r="F107" s="32"/>
       <c r="G107" s="32"/>
       <c r="H107" s="33"/>
@@ -7766,8 +7819,12 @@
       <c r="J107" s="53"/>
       <c r="K107" s="53"/>
       <c r="L107" s="32"/>
-      <c r="M107" s="32"/>
-      <c r="N107" s="30"/>
+      <c r="M107" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N107" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O107" s="46"/>
       <c r="P107" s="39"/>
       <c r="Q107" s="39"/>
@@ -7777,10 +7834,18 @@
     </row>
     <row r="108" spans="1:20" ht="18" customHeight="1">
       <c r="A108" s="51"/>
-      <c r="B108" s="31"/>
-      <c r="C108" s="30"/>
-      <c r="D108" s="30"/>
-      <c r="E108" s="31"/>
+      <c r="B108" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C108" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D108" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E108" s="31" t="s">
+        <v>172</v>
+      </c>
       <c r="F108" s="32"/>
       <c r="G108" s="32"/>
       <c r="H108" s="33"/>
@@ -7788,8 +7853,12 @@
       <c r="J108" s="53"/>
       <c r="K108" s="49"/>
       <c r="L108" s="32"/>
-      <c r="M108" s="32"/>
-      <c r="N108" s="30"/>
+      <c r="M108" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N108" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O108" s="46"/>
       <c r="P108" s="39"/>
       <c r="Q108" s="39"/>
@@ -7799,10 +7868,18 @@
     </row>
     <row r="109" spans="1:20" ht="18" customHeight="1">
       <c r="A109" s="51"/>
-      <c r="B109" s="31"/>
-      <c r="C109" s="30"/>
-      <c r="D109" s="30"/>
-      <c r="E109" s="31"/>
+      <c r="B109" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C109" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>172</v>
+      </c>
       <c r="F109" s="32"/>
       <c r="G109" s="32"/>
       <c r="H109" s="33"/>
@@ -7810,8 +7887,12 @@
       <c r="J109" s="52"/>
       <c r="K109" s="49"/>
       <c r="L109" s="32"/>
-      <c r="M109" s="32"/>
-      <c r="N109" s="30"/>
+      <c r="M109" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N109" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O109" s="37"/>
       <c r="P109" s="39"/>
       <c r="Q109" s="39"/>
@@ -7821,10 +7902,18 @@
     </row>
     <row r="110" spans="1:20" ht="18" customHeight="1">
       <c r="A110" s="51"/>
-      <c r="B110" s="31"/>
-      <c r="C110" s="30"/>
-      <c r="D110" s="30"/>
-      <c r="E110" s="31"/>
+      <c r="B110" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C110" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>175</v>
+      </c>
       <c r="F110" s="32"/>
       <c r="G110" s="32"/>
       <c r="H110" s="33"/>
@@ -7832,8 +7921,12 @@
       <c r="J110" s="52"/>
       <c r="K110" s="49"/>
       <c r="L110" s="50"/>
-      <c r="M110" s="32"/>
-      <c r="N110" s="30"/>
+      <c r="M110" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="N110" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O110" s="37"/>
       <c r="P110" s="39"/>
       <c r="Q110" s="39"/>
@@ -7843,10 +7936,18 @@
     </row>
     <row r="111" spans="1:20" ht="18" customHeight="1">
       <c r="A111" s="51"/>
-      <c r="B111" s="31"/>
-      <c r="C111" s="30"/>
-      <c r="D111" s="30"/>
-      <c r="E111" s="31"/>
+      <c r="B111" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C111" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E111" s="31" t="s">
+        <v>175</v>
+      </c>
       <c r="F111" s="32"/>
       <c r="G111" s="32"/>
       <c r="H111" s="33"/>
@@ -7854,8 +7955,12 @@
       <c r="J111" s="35"/>
       <c r="K111" s="49"/>
       <c r="L111" s="50"/>
-      <c r="M111" s="32"/>
-      <c r="N111" s="30"/>
+      <c r="M111" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="N111" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O111" s="46"/>
       <c r="P111" s="47"/>
       <c r="Q111" s="39"/>
@@ -7865,10 +7970,18 @@
     </row>
     <row r="112" spans="1:20" ht="18" customHeight="1">
       <c r="A112" s="51"/>
-      <c r="B112" s="31"/>
-      <c r="C112" s="30"/>
-      <c r="D112" s="30"/>
-      <c r="E112" s="31"/>
+      <c r="B112" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C112" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E112" s="31" t="s">
+        <v>175</v>
+      </c>
       <c r="F112" s="32"/>
       <c r="G112" s="32"/>
       <c r="H112" s="33"/>
@@ -7876,8 +7989,12 @@
       <c r="J112" s="35"/>
       <c r="K112" s="49"/>
       <c r="L112" s="50"/>
-      <c r="M112" s="32"/>
-      <c r="N112" s="30"/>
+      <c r="M112" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="N112" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O112" s="46"/>
       <c r="P112" s="47"/>
       <c r="Q112" s="39"/>
@@ -7887,10 +8004,18 @@
     </row>
     <row r="113" spans="1:20" ht="18" customHeight="1">
       <c r="A113" s="51"/>
-      <c r="B113" s="31"/>
-      <c r="C113" s="30"/>
-      <c r="D113" s="30"/>
-      <c r="E113" s="31"/>
+      <c r="B113" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C113" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>175</v>
+      </c>
       <c r="F113" s="32"/>
       <c r="G113" s="32"/>
       <c r="H113" s="33"/>
@@ -7898,8 +8023,12 @@
       <c r="J113" s="52"/>
       <c r="K113" s="49"/>
       <c r="L113" s="50"/>
-      <c r="M113" s="32"/>
-      <c r="N113" s="30"/>
+      <c r="M113" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="N113" s="30" t="s">
+        <v>167</v>
+      </c>
       <c r="O113" s="46"/>
       <c r="P113" s="47"/>
       <c r="Q113" s="38"/>

</xml_diff>

<commit_message>
- parsed `10.1016/j.matdes.2024.113396` and adjusted some data from last commit
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6174FB0-DEC2-4F4D-85BD-0DBB2D3A3EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32DC0A4-904C-CC42-9ED0-EC9A3BB087A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3414" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="308">
   <si>
     <r>
       <rPr>
@@ -1009,10 +1009,52 @@
     <t>SF2</t>
   </si>
   <si>
-    <t>magnetostriction</t>
+    <t>m/m</t>
   </si>
   <si>
-    <t>m/m</t>
+    <t>CoCrFe(GaNi)0.4</t>
+  </si>
+  <si>
+    <t>CoCrFe(GaNi)0.7</t>
+  </si>
+  <si>
+    <t>CoCrFe(GaNi)1.0</t>
+  </si>
+  <si>
+    <t>CoCrFe(GaNi)1.3</t>
+  </si>
+  <si>
+    <t>CoCrFe(GaNi)1.6</t>
+  </si>
+  <si>
+    <t>AIM</t>
+  </si>
+  <si>
+    <t>vacuum induction melting in argon-filled silica tube with alumina cruicible and slowly cooled</t>
+  </si>
+  <si>
+    <t>vacuum induction melting in argon-filled silica tube with alumina cruicible and slowly cooled; major FCC phase</t>
+  </si>
+  <si>
+    <t>vacuum induction melting in argon-filled silica tube with alumina cruicible and slowly cooled; major BCC phase</t>
+  </si>
+  <si>
+    <t>BCC+D03</t>
+  </si>
+  <si>
+    <t>vacuum induction melting in argon-filled silica tube with alumina cruicible and slowly cooled; minor D03 is Fe3Si-type ordered BCC 2x2x2 supercell</t>
+  </si>
+  <si>
+    <t>F13b</t>
+  </si>
+  <si>
+    <t>saturation magnetostriction</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
+  <si>
+    <t>10.1016/j.matdes.2024.113396</t>
   </si>
 </sst>
 </file>
@@ -2216,56 +2258,17 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2327,17 +2330,56 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3501,8 +3543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T962"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A318" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O332" sqref="O332"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A351" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N404" sqref="N404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3559,19 +3601,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="114" t="s">
+      <c r="D2" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="115"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="122"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="113"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3587,17 +3629,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="126"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="N3" s="117"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3638,43 +3680,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="127" t="s">
+      <c r="C5" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="129" t="s">
+      <c r="D5" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="129" t="s">
+      <c r="E5" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="129" t="s">
+      <c r="F5" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="129" t="s">
+      <c r="G5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="130" t="s">
+      <c r="H5" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="129" t="s">
+      <c r="I5" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="129" t="s">
+      <c r="J5" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="129" t="s">
+      <c r="K5" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="129" t="s">
+      <c r="L5" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="129" t="s">
+      <c r="M5" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="129" t="s">
+      <c r="N5" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="97" t="s">
+      <c r="O5" s="125" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3690,19 +3732,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="131"/>
-      <c r="I6" s="132"/>
-      <c r="J6" s="133"/>
-      <c r="K6" s="133"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="98"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="126"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3752,7 +3794,7 @@
       <c r="N7" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="99"/>
+      <c r="O7" s="127"/>
       <c r="P7" s="69" t="s">
         <v>77</v>
       </c>
@@ -3767,35 +3809,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="64"/>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103" t="s">
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="108" t="s">
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="109"/>
+      <c r="N8" s="137"/>
       <c r="O8" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="110" t="s">
+      <c r="P8" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="111"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="113"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="140"/>
+      <c r="S8" s="140"/>
+      <c r="T8" s="141"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="65" t="s">
@@ -4542,10 +4584,10 @@
       <c r="T24" s="37"/>
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A25" s="134" t="s">
+      <c r="A25" s="97" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="135" t="s">
+      <c r="B25" s="98" t="s">
         <v>121</v>
       </c>
       <c r="C25" s="30" t="s">
@@ -4718,10 +4760,10 @@
       <c r="T28" s="37"/>
     </row>
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A29" s="134" t="s">
+      <c r="A29" s="97" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="135" t="s">
+      <c r="B29" s="98" t="s">
         <v>121</v>
       </c>
       <c r="C29" s="30" t="s">
@@ -5403,7 +5445,7 @@
         <v>125</v>
       </c>
       <c r="M44" s="40"/>
-      <c r="N44" s="136" t="s">
+      <c r="N44" s="99" t="s">
         <v>144</v>
       </c>
       <c r="O44" s="46"/>
@@ -5443,7 +5485,7 @@
         <v>125</v>
       </c>
       <c r="M45" s="40"/>
-      <c r="N45" s="136" t="s">
+      <c r="N45" s="99" t="s">
         <v>145</v>
       </c>
       <c r="O45" s="46"/>
@@ -5687,7 +5729,7 @@
         <v>128</v>
       </c>
       <c r="M51" s="40"/>
-      <c r="N51" s="136" t="s">
+      <c r="N51" s="99" t="s">
         <v>144</v>
       </c>
       <c r="O51" s="46"/>
@@ -5727,7 +5769,7 @@
         <v>128</v>
       </c>
       <c r="M52" s="40"/>
-      <c r="N52" s="136" t="s">
+      <c r="N52" s="99" t="s">
         <v>145</v>
       </c>
       <c r="O52" s="46"/>
@@ -6465,11 +6507,11 @@
       <c r="I69" s="34">
         <v>298</v>
       </c>
-      <c r="J69" s="137">
+      <c r="J69" s="100">
         <f t="shared" ref="J69:J76" si="0">P69*9807000</f>
         <v>5122230164.5338182</v>
       </c>
-      <c r="K69" s="137">
+      <c r="K69" s="100">
         <f>(Q69-P69)*9807000</f>
         <v>338852468.0073154</v>
       </c>
@@ -6517,11 +6559,11 @@
       <c r="I70" s="34">
         <v>298</v>
       </c>
-      <c r="J70" s="137">
+      <c r="J70" s="100">
         <f t="shared" si="0"/>
         <v>6038386837.2943306</v>
       </c>
-      <c r="K70" s="137">
+      <c r="K70" s="100">
         <f t="shared" ref="K70:K76" si="1">(Q70-P70)*9807000</f>
         <v>338852468.0073154</v>
       </c>
@@ -6569,11 +6611,11 @@
       <c r="I71" s="34">
         <v>298</v>
       </c>
-      <c r="J71" s="137">
+      <c r="J71" s="100">
         <f t="shared" si="0"/>
         <v>6690991590.4935989</v>
       </c>
-      <c r="K71" s="137">
+      <c r="K71" s="100">
         <f t="shared" si="1"/>
         <v>288652102.37659782</v>
       </c>
@@ -6621,11 +6663,11 @@
       <c r="I72" s="34">
         <v>298</v>
       </c>
-      <c r="J72" s="137">
+      <c r="J72" s="100">
         <f t="shared" si="0"/>
         <v>6929443327.2394876</v>
       </c>
-      <c r="K72" s="137">
+      <c r="K72" s="100">
         <f t="shared" si="1"/>
         <v>376502742.23034215</v>
       </c>
@@ -6673,11 +6715,11 @@
       <c r="I73" s="34">
         <v>298</v>
       </c>
-      <c r="J73" s="137">
+      <c r="J73" s="100">
         <f t="shared" si="0"/>
         <v>4370646088.794919</v>
       </c>
-      <c r="K73" s="137">
+      <c r="K73" s="100">
         <f t="shared" si="1"/>
         <v>362838266.38477683</v>
       </c>
@@ -6725,11 +6767,11 @@
       <c r="I74" s="34">
         <v>298</v>
       </c>
-      <c r="J74" s="137">
+      <c r="J74" s="100">
         <f t="shared" si="0"/>
         <v>5417693657.5052862</v>
       </c>
-      <c r="K74" s="137">
+      <c r="K74" s="100">
         <f t="shared" si="1"/>
         <v>269536997.88582945</v>
       </c>
@@ -6777,11 +6819,11 @@
       <c r="I75" s="34">
         <v>298</v>
       </c>
-      <c r="J75" s="137">
+      <c r="J75" s="100">
         <f t="shared" si="0"/>
         <v>5127423044.3974543</v>
       </c>
-      <c r="K75" s="137">
+      <c r="K75" s="100">
         <f t="shared" si="1"/>
         <v>342104651.16279542</v>
       </c>
@@ -6829,11 +6871,11 @@
       <c r="I76" s="34">
         <v>298</v>
       </c>
-      <c r="J76" s="137">
+      <c r="J76" s="100">
         <f t="shared" si="0"/>
         <v>5013388160.6765261</v>
       </c>
-      <c r="K76" s="137">
+      <c r="K76" s="100">
         <f t="shared" si="1"/>
         <v>238436575.05285701</v>
       </c>
@@ -7515,7 +7557,7 @@
       <c r="I92" s="34">
         <v>298</v>
       </c>
-      <c r="J92" s="137">
+      <c r="J92" s="100">
         <f t="shared" ref="J92" si="2">P92*9807000</f>
         <v>1765260000</v>
       </c>
@@ -8417,11 +8459,11 @@
       <c r="I114" s="38">
         <v>298</v>
       </c>
-      <c r="J114" s="137">
+      <c r="J114" s="100">
         <f t="shared" ref="J114:K116" si="4">P114*9807000</f>
         <v>4776009000</v>
       </c>
-      <c r="K114" s="137">
+      <c r="K114" s="100">
         <f t="shared" si="4"/>
         <v>176526000</v>
       </c>
@@ -8471,11 +8513,11 @@
       <c r="I115" s="38">
         <v>298</v>
       </c>
-      <c r="J115" s="137">
+      <c r="J115" s="100">
         <f t="shared" si="4"/>
         <v>5511534000</v>
       </c>
-      <c r="K115" s="137">
+      <c r="K115" s="100">
         <f t="shared" si="4"/>
         <v>196140000</v>
       </c>
@@ -8525,11 +8567,11 @@
       <c r="I116" s="38">
         <v>298</v>
       </c>
-      <c r="J116" s="137">
+      <c r="J116" s="100">
         <f t="shared" si="4"/>
         <v>6619725000</v>
       </c>
-      <c r="K116" s="137">
+      <c r="K116" s="100">
         <f t="shared" si="4"/>
         <v>460929000</v>
       </c>
@@ -8978,7 +9020,7 @@
       <c r="B127" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="C127" s="138" t="s">
+      <c r="C127" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D127" s="30" t="s">
@@ -9022,7 +9064,7 @@
       <c r="B128" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="C128" s="139" t="s">
+      <c r="C128" s="102" t="s">
         <v>74</v>
       </c>
       <c r="D128" s="30" t="s">
@@ -9066,7 +9108,7 @@
       <c r="B129" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="C129" s="139" t="s">
+      <c r="C129" s="102" t="s">
         <v>74</v>
       </c>
       <c r="D129" s="30" t="s">
@@ -9110,7 +9152,7 @@
       <c r="B130" s="96" t="s">
         <v>207</v>
       </c>
-      <c r="C130" s="139" t="s">
+      <c r="C130" s="102" t="s">
         <v>75</v>
       </c>
       <c r="D130" s="30" t="s">
@@ -9154,7 +9196,7 @@
       <c r="B131" s="96" t="s">
         <v>208</v>
       </c>
-      <c r="C131" s="139" t="s">
+      <c r="C131" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D131" s="30" t="s">
@@ -9198,7 +9240,7 @@
       <c r="B132" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="C132" s="138" t="s">
+      <c r="C132" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D132" s="30" t="s">
@@ -9242,7 +9284,7 @@
       <c r="B133" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="C133" s="139" t="s">
+      <c r="C133" s="102" t="s">
         <v>74</v>
       </c>
       <c r="D133" s="30" t="s">
@@ -9286,7 +9328,7 @@
       <c r="B134" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="C134" s="139" t="s">
+      <c r="C134" s="102" t="s">
         <v>74</v>
       </c>
       <c r="D134" s="30" t="s">
@@ -9330,7 +9372,7 @@
       <c r="B135" s="96" t="s">
         <v>207</v>
       </c>
-      <c r="C135" s="139" t="s">
+      <c r="C135" s="102" t="s">
         <v>75</v>
       </c>
       <c r="D135" s="30" t="s">
@@ -9374,7 +9416,7 @@
       <c r="B136" s="96" t="s">
         <v>208</v>
       </c>
-      <c r="C136" s="139" t="s">
+      <c r="C136" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D136" s="30" t="s">
@@ -9418,7 +9460,7 @@
       <c r="B137" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="C137" s="138" t="s">
+      <c r="C137" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D137" s="30" t="s">
@@ -9462,7 +9504,7 @@
       <c r="B138" s="96" t="s">
         <v>205</v>
       </c>
-      <c r="C138" s="139" t="s">
+      <c r="C138" s="102" t="s">
         <v>74</v>
       </c>
       <c r="D138" s="30" t="s">
@@ -9506,7 +9548,7 @@
       <c r="B139" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="C139" s="139" t="s">
+      <c r="C139" s="102" t="s">
         <v>74</v>
       </c>
       <c r="D139" s="30" t="s">
@@ -9550,7 +9592,7 @@
       <c r="B140" s="96" t="s">
         <v>207</v>
       </c>
-      <c r="C140" s="139" t="s">
+      <c r="C140" s="102" t="s">
         <v>75</v>
       </c>
       <c r="D140" s="30" t="s">
@@ -9594,7 +9636,7 @@
       <c r="B141" s="96" t="s">
         <v>208</v>
       </c>
-      <c r="C141" s="139" t="s">
+      <c r="C141" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D141" s="30" t="s">
@@ -9638,7 +9680,7 @@
       <c r="B142" s="96" t="s">
         <v>208</v>
       </c>
-      <c r="C142" s="139" t="s">
+      <c r="C142" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D142" s="30" t="s">
@@ -13072,7 +13114,7 @@
       <c r="I215" s="38">
         <v>298</v>
       </c>
-      <c r="J215" s="137">
+      <c r="J215" s="100">
         <f t="shared" ref="J215:J221" si="9">P215*9807000</f>
         <v>1372652006.6889586</v>
       </c>
@@ -13121,7 +13163,7 @@
       <c r="I216" s="38">
         <v>298</v>
       </c>
-      <c r="J216" s="137">
+      <c r="J216" s="100">
         <f t="shared" si="9"/>
         <v>2986379096.9899654</v>
       </c>
@@ -13170,7 +13212,7 @@
       <c r="I217" s="38">
         <v>298</v>
       </c>
-      <c r="J217" s="137">
+      <c r="J217" s="100">
         <f t="shared" si="9"/>
         <v>5033057357.8595304</v>
       </c>
@@ -13219,7 +13261,7 @@
       <c r="I218" s="38">
         <v>298</v>
       </c>
-      <c r="J218" s="137">
+      <c r="J218" s="100">
         <f t="shared" si="9"/>
         <v>4993698160.5351105</v>
       </c>
@@ -13268,7 +13310,7 @@
       <c r="I219" s="38">
         <v>298</v>
       </c>
-      <c r="J219" s="137">
+      <c r="J219" s="100">
         <f t="shared" si="9"/>
         <v>5859600501.6722345</v>
       </c>
@@ -13317,7 +13359,7 @@
       <c r="I220" s="38">
         <v>298</v>
       </c>
-      <c r="J220" s="137">
+      <c r="J220" s="100">
         <f t="shared" si="9"/>
         <v>5879280100.334445</v>
       </c>
@@ -13366,7 +13408,7 @@
       <c r="I221" s="38">
         <v>298</v>
       </c>
-      <c r="J221" s="137">
+      <c r="J221" s="100">
         <f t="shared" si="9"/>
         <v>8024356354.5150414</v>
       </c>
@@ -14396,7 +14438,7 @@
       <c r="B243" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C243" s="140" t="s">
+      <c r="C243" s="103" t="s">
         <v>93</v>
       </c>
       <c r="D243" s="61" t="s">
@@ -14444,7 +14486,7 @@
       <c r="B244" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C244" s="140" t="s">
+      <c r="C244" s="103" t="s">
         <v>248</v>
       </c>
       <c r="D244" s="61" t="s">
@@ -14492,7 +14534,7 @@
       <c r="B245" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C245" s="140" t="s">
+      <c r="C245" s="103" t="s">
         <v>93</v>
       </c>
       <c r="D245" s="61" t="s">
@@ -14540,7 +14582,7 @@
       <c r="B246" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C246" s="140" t="s">
+      <c r="C246" s="103" t="s">
         <v>248</v>
       </c>
       <c r="D246" s="61" t="s">
@@ -14588,7 +14630,7 @@
       <c r="B247" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C247" s="140" t="s">
+      <c r="C247" s="103" t="s">
         <v>93</v>
       </c>
       <c r="D247" s="61" t="s">
@@ -14636,7 +14678,7 @@
       <c r="B248" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C248" s="140" t="s">
+      <c r="C248" s="103" t="s">
         <v>248</v>
       </c>
       <c r="D248" s="61" t="s">
@@ -14682,7 +14724,7 @@
       <c r="B249" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C249" s="140" t="s">
+      <c r="C249" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D249" s="61" t="s">
@@ -14726,7 +14768,7 @@
       <c r="B250" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C250" s="140" t="s">
+      <c r="C250" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D250" s="61"/>
@@ -14766,7 +14808,7 @@
       <c r="B251" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C251" s="140" t="s">
+      <c r="C251" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D251" s="61" t="s">
@@ -14810,7 +14852,7 @@
       <c r="B252" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C252" s="140" t="s">
+      <c r="C252" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D252" s="61"/>
@@ -14850,7 +14892,7 @@
       <c r="B253" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C253" s="140" t="s">
+      <c r="C253" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D253" s="61" t="s">
@@ -14894,7 +14936,7 @@
       <c r="B254" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C254" s="140" t="s">
+      <c r="C254" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D254" s="61"/>
@@ -14934,7 +14976,7 @@
       <c r="B255" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C255" s="140" t="s">
+      <c r="C255" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D255" s="61" t="s">
@@ -14976,7 +15018,7 @@
       <c r="B256" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C256" s="140" t="s">
+      <c r="C256" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D256" s="61"/>
@@ -15014,7 +15056,7 @@
       <c r="B257" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C257" s="140" t="s">
+      <c r="C257" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D257" s="61" t="s">
@@ -15055,7 +15097,7 @@
       <c r="B258" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C258" s="140" t="s">
+      <c r="C258" s="103" t="s">
         <v>64</v>
       </c>
       <c r="D258" s="61"/>
@@ -15163,7 +15205,7 @@
         <v>300</v>
       </c>
       <c r="J260" s="53">
-        <f t="shared" ref="J260:J277" si="10">P260*0.000001</f>
+        <f t="shared" ref="J260:J276" si="10">P260*0.000001</f>
         <v>1.5438777075873399E-5</v>
       </c>
       <c r="K260" s="38"/>
@@ -15960,7 +16002,7 @@
       <c r="N276" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="O276" s="141"/>
+      <c r="O276" s="104"/>
       <c r="P276" s="45">
         <v>164.444444444444</v>
       </c>
@@ -19881,7 +19923,7 @@
         <v>288</v>
       </c>
       <c r="F361" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G361" s="32" t="s">
         <v>29</v>
@@ -19896,7 +19938,7 @@
       </c>
       <c r="K361" s="49"/>
       <c r="L361" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M361" s="61" t="s">
         <v>182</v>
@@ -19928,7 +19970,7 @@
         <v>288</v>
       </c>
       <c r="F362" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G362" s="32" t="s">
         <v>29</v>
@@ -19943,7 +19985,7 @@
       </c>
       <c r="K362" s="49"/>
       <c r="L362" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M362" s="61" t="s">
         <v>182</v>
@@ -19975,7 +20017,7 @@
         <v>288</v>
       </c>
       <c r="F363" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G363" s="32" t="s">
         <v>29</v>
@@ -19990,7 +20032,7 @@
       </c>
       <c r="K363" s="49"/>
       <c r="L363" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M363" s="61" t="s">
         <v>182</v>
@@ -20022,7 +20064,7 @@
         <v>288</v>
       </c>
       <c r="F364" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G364" s="32" t="s">
         <v>29</v>
@@ -20037,7 +20079,7 @@
       </c>
       <c r="K364" s="45"/>
       <c r="L364" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M364" s="61" t="s">
         <v>182</v>
@@ -20069,7 +20111,7 @@
         <v>288</v>
       </c>
       <c r="F365" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G365" s="32" t="s">
         <v>29</v>
@@ -20084,7 +20126,7 @@
       </c>
       <c r="K365" s="45"/>
       <c r="L365" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M365" s="61" t="s">
         <v>182</v>
@@ -20116,7 +20158,7 @@
         <v>288</v>
       </c>
       <c r="F366" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G366" s="32" t="s">
         <v>29</v>
@@ -20131,7 +20173,7 @@
       </c>
       <c r="K366" s="45"/>
       <c r="L366" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M366" s="61" t="s">
         <v>182</v>
@@ -20163,7 +20205,7 @@
         <v>288</v>
       </c>
       <c r="F367" s="61" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="G367" s="32" t="s">
         <v>29</v>
@@ -20178,7 +20220,7 @@
       </c>
       <c r="K367" s="45"/>
       <c r="L367" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M367" s="61" t="s">
         <v>182</v>
@@ -20197,19 +20239,41 @@
     </row>
     <row r="368" spans="1:20" ht="18" customHeight="1">
       <c r="A368" s="45"/>
-      <c r="B368" s="61"/>
-      <c r="C368" s="61"/>
-      <c r="D368" s="61"/>
-      <c r="E368" s="61"/>
-      <c r="F368" s="45"/>
-      <c r="G368" s="45"/>
+      <c r="B368" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C368" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D368" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E368" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F368" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G368" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H368" s="45"/>
-      <c r="I368" s="45"/>
-      <c r="J368" s="45"/>
+      <c r="I368" s="45">
+        <v>300</v>
+      </c>
+      <c r="J368" s="45">
+        <v>0.101503759398496</v>
+      </c>
       <c r="K368" s="45"/>
-      <c r="L368" s="61"/>
-      <c r="M368" s="45"/>
-      <c r="N368" s="61"/>
+      <c r="L368" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="M368" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="N368" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O368" s="45"/>
       <c r="P368" s="45"/>
       <c r="Q368" s="45"/>
@@ -20219,19 +20283,41 @@
     </row>
     <row r="369" spans="1:20" ht="18" customHeight="1">
       <c r="A369" s="45"/>
-      <c r="B369" s="61"/>
-      <c r="C369" s="61"/>
-      <c r="D369" s="61"/>
-      <c r="E369" s="61"/>
-      <c r="F369" s="61"/>
-      <c r="G369" s="61"/>
+      <c r="B369" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C369" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D369" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E369" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F369" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G369" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H369" s="45"/>
-      <c r="I369" s="45"/>
-      <c r="J369" s="45"/>
+      <c r="I369" s="45">
+        <v>300</v>
+      </c>
+      <c r="J369" s="45">
+        <v>-0.29699248120300697</v>
+      </c>
       <c r="K369" s="45"/>
-      <c r="L369" s="61"/>
-      <c r="M369" s="61"/>
-      <c r="N369" s="61"/>
+      <c r="L369" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="M369" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="N369" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O369" s="45"/>
       <c r="P369" s="45"/>
       <c r="Q369" s="45"/>
@@ -20241,19 +20327,41 @@
     </row>
     <row r="370" spans="1:20" ht="18" customHeight="1">
       <c r="A370" s="45"/>
-      <c r="B370" s="61"/>
-      <c r="C370" s="61"/>
-      <c r="D370" s="61"/>
-      <c r="E370" s="61"/>
-      <c r="F370" s="61"/>
-      <c r="G370" s="61"/>
+      <c r="B370" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C370" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D370" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E370" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F370" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G370" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H370" s="45"/>
-      <c r="I370" s="45"/>
-      <c r="J370" s="45"/>
+      <c r="I370" s="45">
+        <v>300</v>
+      </c>
+      <c r="J370" s="45">
+        <v>-0.84962406015037595</v>
+      </c>
       <c r="K370" s="45"/>
-      <c r="L370" s="61"/>
-      <c r="M370" s="61"/>
-      <c r="N370" s="61"/>
+      <c r="L370" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="M370" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="N370" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O370" s="45"/>
       <c r="P370" s="45"/>
       <c r="Q370" s="45"/>
@@ -20263,19 +20371,41 @@
     </row>
     <row r="371" spans="1:20" ht="18" customHeight="1">
       <c r="A371" s="45"/>
-      <c r="B371" s="61"/>
-      <c r="C371" s="61"/>
-      <c r="D371" s="61"/>
-      <c r="E371" s="61"/>
-      <c r="F371" s="61"/>
-      <c r="G371" s="61"/>
+      <c r="B371" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C371" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D371" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E371" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F371" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G371" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H371" s="45"/>
-      <c r="I371" s="45"/>
-      <c r="J371" s="45"/>
+      <c r="I371" s="45">
+        <v>300</v>
+      </c>
+      <c r="J371" s="45">
+        <v>-1.4473684210526301</v>
+      </c>
       <c r="K371" s="45"/>
-      <c r="L371" s="61"/>
-      <c r="M371" s="61"/>
-      <c r="N371" s="61"/>
+      <c r="L371" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="M371" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="N371" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O371" s="45"/>
       <c r="P371" s="45"/>
       <c r="Q371" s="45"/>
@@ -20285,19 +20415,41 @@
     </row>
     <row r="372" spans="1:20" ht="18" customHeight="1">
       <c r="A372" s="45"/>
-      <c r="B372" s="61"/>
-      <c r="C372" s="61"/>
-      <c r="D372" s="61"/>
-      <c r="E372" s="61"/>
-      <c r="F372" s="61"/>
-      <c r="G372" s="61"/>
+      <c r="B372" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C372" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D372" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E372" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F372" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G372" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H372" s="45"/>
-      <c r="I372" s="45"/>
-      <c r="J372" s="45"/>
+      <c r="I372" s="45">
+        <v>300</v>
+      </c>
+      <c r="J372" s="45">
+        <v>-3.0263157894736801</v>
+      </c>
       <c r="K372" s="45"/>
-      <c r="L372" s="61"/>
-      <c r="M372" s="61"/>
-      <c r="N372" s="61"/>
+      <c r="L372" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="M372" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="N372" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O372" s="45"/>
       <c r="P372" s="45"/>
       <c r="Q372" s="45"/>
@@ -20307,19 +20459,39 @@
     </row>
     <row r="373" spans="1:20" ht="18" customHeight="1">
       <c r="A373" s="45"/>
-      <c r="B373" s="61"/>
-      <c r="C373" s="61"/>
-      <c r="D373" s="61"/>
-      <c r="E373" s="61"/>
-      <c r="F373" s="61"/>
-      <c r="G373" s="61"/>
+      <c r="B373" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C373" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D373" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E373" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F373" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G373" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H373" s="45"/>
       <c r="I373" s="45"/>
-      <c r="J373" s="45"/>
-      <c r="K373" s="45"/>
-      <c r="L373" s="61"/>
+      <c r="J373" s="45">
+        <v>750</v>
+      </c>
+      <c r="K373" s="45">
+        <v>10</v>
+      </c>
+      <c r="L373" s="61" t="s">
+        <v>125</v>
+      </c>
       <c r="M373" s="61"/>
-      <c r="N373" s="61"/>
+      <c r="N373" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O373" s="45"/>
       <c r="P373" s="45"/>
       <c r="Q373" s="45"/>
@@ -20329,19 +20501,39 @@
     </row>
     <row r="374" spans="1:20" ht="18" customHeight="1">
       <c r="A374" s="45"/>
-      <c r="B374" s="61"/>
-      <c r="C374" s="61"/>
-      <c r="D374" s="61"/>
-      <c r="E374" s="61"/>
-      <c r="F374" s="61"/>
-      <c r="G374" s="61"/>
+      <c r="B374" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C374" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D374" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E374" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F374" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G374" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H374" s="45"/>
       <c r="I374" s="45"/>
-      <c r="J374" s="45"/>
-      <c r="K374" s="45"/>
-      <c r="L374" s="61"/>
+      <c r="J374" s="45">
+        <v>725</v>
+      </c>
+      <c r="K374" s="45">
+        <v>10</v>
+      </c>
+      <c r="L374" s="61" t="s">
+        <v>125</v>
+      </c>
       <c r="M374" s="61"/>
-      <c r="N374" s="61"/>
+      <c r="N374" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O374" s="45"/>
       <c r="P374" s="45"/>
       <c r="Q374" s="45"/>
@@ -20351,19 +20543,39 @@
     </row>
     <row r="375" spans="1:20" ht="18" customHeight="1">
       <c r="A375" s="45"/>
-      <c r="B375" s="61"/>
-      <c r="C375" s="61"/>
-      <c r="D375" s="61"/>
-      <c r="E375" s="61"/>
-      <c r="F375" s="61"/>
-      <c r="G375" s="61"/>
+      <c r="B375" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C375" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D375" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E375" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F375" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G375" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H375" s="45"/>
       <c r="I375" s="45"/>
-      <c r="J375" s="45"/>
-      <c r="K375" s="45"/>
-      <c r="L375" s="61"/>
+      <c r="J375" s="45">
+        <v>715</v>
+      </c>
+      <c r="K375" s="45">
+        <v>10</v>
+      </c>
+      <c r="L375" s="61" t="s">
+        <v>125</v>
+      </c>
       <c r="M375" s="61"/>
-      <c r="N375" s="61"/>
+      <c r="N375" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O375" s="45"/>
       <c r="P375" s="45"/>
       <c r="Q375" s="45"/>
@@ -20373,19 +20585,39 @@
     </row>
     <row r="376" spans="1:20" ht="18" customHeight="1">
       <c r="A376" s="45"/>
-      <c r="B376" s="61"/>
-      <c r="C376" s="61"/>
-      <c r="D376" s="61"/>
-      <c r="E376" s="61"/>
-      <c r="F376" s="61"/>
-      <c r="G376" s="61"/>
+      <c r="B376" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C376" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D376" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E376" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F376" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G376" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H376" s="45"/>
       <c r="I376" s="45"/>
-      <c r="J376" s="45"/>
-      <c r="K376" s="45"/>
-      <c r="L376" s="61"/>
+      <c r="J376" s="45">
+        <v>700</v>
+      </c>
+      <c r="K376" s="45">
+        <v>10</v>
+      </c>
+      <c r="L376" s="61" t="s">
+        <v>125</v>
+      </c>
       <c r="M376" s="61"/>
-      <c r="N376" s="61"/>
+      <c r="N376" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O376" s="45"/>
       <c r="P376" s="45"/>
       <c r="Q376" s="45"/>
@@ -20395,19 +20627,41 @@
     </row>
     <row r="377" spans="1:20" ht="18" customHeight="1">
       <c r="A377" s="45"/>
-      <c r="B377" s="61"/>
-      <c r="C377" s="61"/>
-      <c r="D377" s="61"/>
-      <c r="E377" s="61"/>
-      <c r="F377" s="61"/>
-      <c r="G377" s="61"/>
+      <c r="B377" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C377" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D377" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E377" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F377" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G377" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H377" s="45"/>
-      <c r="I377" s="45"/>
-      <c r="J377" s="45"/>
+      <c r="I377" s="45">
+        <v>5</v>
+      </c>
+      <c r="J377" s="45">
+        <v>1163.2653061224401</v>
+      </c>
       <c r="K377" s="45"/>
-      <c r="L377" s="61"/>
-      <c r="M377" s="61"/>
-      <c r="N377" s="61"/>
+      <c r="L377" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M377" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N377" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O377" s="45"/>
       <c r="P377" s="45"/>
       <c r="Q377" s="45"/>
@@ -20417,19 +20671,41 @@
     </row>
     <row r="378" spans="1:20" ht="18" customHeight="1">
       <c r="A378" s="45"/>
-      <c r="B378" s="61"/>
-      <c r="C378" s="61"/>
-      <c r="D378" s="61"/>
-      <c r="E378" s="45"/>
-      <c r="F378" s="61"/>
-      <c r="G378" s="61"/>
+      <c r="B378" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C378" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D378" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E378" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F378" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G378" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H378" s="45"/>
-      <c r="I378" s="45"/>
-      <c r="J378" s="45"/>
+      <c r="I378" s="45">
+        <v>100</v>
+      </c>
+      <c r="J378" s="45">
+        <v>911.56462585034001</v>
+      </c>
       <c r="K378" s="45"/>
-      <c r="L378" s="61"/>
-      <c r="M378" s="61"/>
-      <c r="N378" s="61"/>
+      <c r="L378" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M378" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N378" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O378" s="45"/>
       <c r="P378" s="45"/>
       <c r="Q378" s="45"/>
@@ -20439,19 +20715,41 @@
     </row>
     <row r="379" spans="1:20" ht="18" customHeight="1">
       <c r="A379" s="45"/>
-      <c r="B379" s="61"/>
-      <c r="C379" s="61"/>
-      <c r="D379" s="61"/>
-      <c r="E379" s="45"/>
-      <c r="F379" s="61"/>
-      <c r="G379" s="61"/>
+      <c r="B379" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C379" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D379" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E379" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F379" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G379" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H379" s="45"/>
-      <c r="I379" s="45"/>
-      <c r="J379" s="45"/>
+      <c r="I379" s="45">
+        <v>200</v>
+      </c>
+      <c r="J379" s="45">
+        <v>687.07482993197198</v>
+      </c>
       <c r="K379" s="45"/>
-      <c r="L379" s="61"/>
-      <c r="M379" s="61"/>
-      <c r="N379" s="61"/>
+      <c r="L379" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M379" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N379" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O379" s="45"/>
       <c r="P379" s="45"/>
       <c r="Q379" s="45"/>
@@ -20461,19 +20759,41 @@
     </row>
     <row r="380" spans="1:20" ht="18" customHeight="1">
       <c r="A380" s="45"/>
-      <c r="B380" s="61"/>
-      <c r="C380" s="61"/>
-      <c r="D380" s="61"/>
-      <c r="E380" s="45"/>
-      <c r="F380" s="61"/>
-      <c r="G380" s="61"/>
+      <c r="B380" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C380" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D380" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E380" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F380" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G380" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H380" s="45"/>
-      <c r="I380" s="45"/>
-      <c r="J380" s="45"/>
+      <c r="I380" s="45">
+        <v>300</v>
+      </c>
+      <c r="J380" s="45">
+        <v>341.83673469387702</v>
+      </c>
       <c r="K380" s="45"/>
-      <c r="L380" s="61"/>
-      <c r="M380" s="61"/>
-      <c r="N380" s="61"/>
+      <c r="L380" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M380" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N380" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O380" s="45"/>
       <c r="P380" s="45"/>
       <c r="Q380" s="45"/>
@@ -20483,19 +20803,41 @@
     </row>
     <row r="381" spans="1:20" ht="18" customHeight="1">
       <c r="A381" s="45"/>
-      <c r="B381" s="61"/>
-      <c r="C381" s="61"/>
-      <c r="D381" s="61"/>
-      <c r="E381" s="45"/>
-      <c r="F381" s="61"/>
-      <c r="G381" s="61"/>
+      <c r="B381" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C381" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D381" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E381" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F381" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G381" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H381" s="45"/>
-      <c r="I381" s="45"/>
-      <c r="J381" s="45"/>
+      <c r="I381" s="45">
+        <v>400</v>
+      </c>
+      <c r="J381" s="45">
+        <v>176.87074829931899</v>
+      </c>
       <c r="K381" s="45"/>
-      <c r="L381" s="61"/>
-      <c r="M381" s="61"/>
-      <c r="N381" s="61"/>
+      <c r="L381" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M381" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N381" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O381" s="45"/>
       <c r="P381" s="45"/>
       <c r="Q381" s="45"/>
@@ -20505,21 +20847,46 @@
     </row>
     <row r="382" spans="1:20" ht="18" customHeight="1">
       <c r="A382" s="45"/>
-      <c r="B382" s="61"/>
-      <c r="C382" s="61"/>
-      <c r="D382" s="61"/>
-      <c r="E382" s="45"/>
-      <c r="F382" s="61"/>
-      <c r="G382" s="61"/>
+      <c r="B382" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C382" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D382" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E382" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F382" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G382" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H382" s="45"/>
-      <c r="I382" s="45"/>
-      <c r="J382" s="49"/>
+      <c r="I382" s="61">
+        <v>2</v>
+      </c>
+      <c r="J382" s="49">
+        <f>P382*0.00000001</f>
+        <v>1.0272829763246899E-6</v>
+      </c>
       <c r="K382" s="45"/>
-      <c r="L382" s="61"/>
-      <c r="M382" s="61"/>
-      <c r="N382" s="61"/>
+      <c r="L382" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M382" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N382" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O382" s="45"/>
-      <c r="P382" s="45"/>
+      <c r="P382" s="45">
+        <v>102.72829763246899</v>
+      </c>
       <c r="Q382" s="45"/>
       <c r="R382" s="45"/>
       <c r="S382" s="37"/>
@@ -20527,21 +20894,46 @@
     </row>
     <row r="383" spans="1:20" ht="18" customHeight="1">
       <c r="A383" s="45"/>
-      <c r="B383" s="61"/>
-      <c r="C383" s="61"/>
-      <c r="D383" s="61"/>
-      <c r="E383" s="45"/>
-      <c r="F383" s="61"/>
-      <c r="G383" s="61"/>
+      <c r="B383" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C383" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D383" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E383" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F383" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G383" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H383" s="45"/>
-      <c r="I383" s="45"/>
-      <c r="J383" s="49"/>
+      <c r="I383" s="61">
+        <v>2</v>
+      </c>
+      <c r="J383" s="49">
+        <f t="shared" ref="J383:J401" si="14">P383*0.00000001</f>
+        <v>1.2126268320180301E-6</v>
+      </c>
       <c r="K383" s="45"/>
-      <c r="L383" s="61"/>
-      <c r="M383" s="61"/>
-      <c r="N383" s="61"/>
+      <c r="L383" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M383" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N383" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O383" s="45"/>
-      <c r="P383" s="45"/>
+      <c r="P383" s="45">
+        <v>121.262683201803</v>
+      </c>
       <c r="Q383" s="45"/>
       <c r="R383" s="45"/>
       <c r="S383" s="37"/>
@@ -20549,21 +20941,46 @@
     </row>
     <row r="384" spans="1:20" ht="18" customHeight="1">
       <c r="A384" s="45"/>
-      <c r="B384" s="61"/>
-      <c r="C384" s="61"/>
-      <c r="D384" s="61"/>
-      <c r="E384" s="45"/>
-      <c r="F384" s="61"/>
-      <c r="G384" s="61"/>
+      <c r="B384" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C384" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D384" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E384" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F384" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G384" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H384" s="45"/>
-      <c r="I384" s="45"/>
-      <c r="J384" s="49"/>
+      <c r="I384" s="61">
+        <v>2</v>
+      </c>
+      <c r="J384" s="49">
+        <f t="shared" si="14"/>
+        <v>1.12468996617812E-6</v>
+      </c>
       <c r="K384" s="45"/>
-      <c r="L384" s="61"/>
-      <c r="M384" s="61"/>
-      <c r="N384" s="61"/>
+      <c r="L384" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M384" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N384" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O384" s="45"/>
-      <c r="P384" s="45"/>
+      <c r="P384" s="45">
+        <v>112.468996617812</v>
+      </c>
       <c r="Q384" s="45"/>
       <c r="R384" s="45"/>
       <c r="S384" s="37"/>
@@ -20571,21 +20988,46 @@
     </row>
     <row r="385" spans="1:20" ht="18" customHeight="1">
       <c r="A385" s="45"/>
-      <c r="B385" s="61"/>
-      <c r="C385" s="61"/>
-      <c r="D385" s="61"/>
-      <c r="E385" s="45"/>
-      <c r="F385" s="61"/>
-      <c r="G385" s="61"/>
+      <c r="B385" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C385" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D385" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E385" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F385" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G385" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H385" s="45"/>
-      <c r="I385" s="45"/>
-      <c r="J385" s="49"/>
+      <c r="I385" s="61">
+        <v>2</v>
+      </c>
+      <c r="J385" s="49">
+        <f t="shared" si="14"/>
+        <v>9.9210822998872598E-7</v>
+      </c>
       <c r="K385" s="45"/>
-      <c r="L385" s="61"/>
-      <c r="M385" s="61"/>
-      <c r="N385" s="61"/>
+      <c r="L385" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M385" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N385" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O385" s="45"/>
-      <c r="P385" s="45"/>
+      <c r="P385" s="45">
+        <v>99.210822998872601</v>
+      </c>
       <c r="Q385" s="45"/>
       <c r="R385" s="45"/>
       <c r="S385" s="37"/>
@@ -20593,21 +21035,46 @@
     </row>
     <row r="386" spans="1:20" ht="18" customHeight="1">
       <c r="A386" s="45"/>
-      <c r="B386" s="61"/>
-      <c r="C386" s="61"/>
-      <c r="D386" s="61"/>
-      <c r="E386" s="45"/>
-      <c r="F386" s="61"/>
-      <c r="G386" s="61"/>
+      <c r="B386" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C386" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D386" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E386" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F386" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G386" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H386" s="45"/>
-      <c r="I386" s="45"/>
-      <c r="J386" s="49"/>
+      <c r="I386" s="61">
+        <v>2</v>
+      </c>
+      <c r="J386" s="49">
+        <f t="shared" si="14"/>
+        <v>9.4475760992108206E-7</v>
+      </c>
       <c r="K386" s="45"/>
-      <c r="L386" s="61"/>
-      <c r="M386" s="61"/>
-      <c r="N386" s="61"/>
+      <c r="L386" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M386" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N386" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O386" s="45"/>
-      <c r="P386" s="45"/>
+      <c r="P386" s="45">
+        <v>94.475760992108206</v>
+      </c>
       <c r="Q386" s="45"/>
       <c r="R386" s="45"/>
       <c r="S386" s="37"/>
@@ -20615,21 +21082,46 @@
     </row>
     <row r="387" spans="1:20" ht="18" customHeight="1">
       <c r="A387" s="45"/>
-      <c r="B387" s="61"/>
-      <c r="C387" s="61"/>
-      <c r="D387" s="61"/>
-      <c r="E387" s="45"/>
-      <c r="F387" s="61"/>
-      <c r="G387" s="61"/>
+      <c r="B387" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C387" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D387" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E387" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F387" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G387" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H387" s="45"/>
-      <c r="I387" s="45"/>
-      <c r="J387" s="49"/>
+      <c r="I387" s="61">
+        <v>50</v>
+      </c>
+      <c r="J387" s="49">
+        <f t="shared" si="14"/>
+        <v>1.0381059751972901E-6</v>
+      </c>
       <c r="K387" s="45"/>
-      <c r="L387" s="61"/>
-      <c r="M387" s="61"/>
-      <c r="N387" s="61"/>
+      <c r="L387" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M387" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N387" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O387" s="45"/>
-      <c r="P387" s="45"/>
+      <c r="P387" s="45">
+        <v>103.810597519729</v>
+      </c>
       <c r="Q387" s="45"/>
       <c r="R387" s="45"/>
       <c r="S387" s="37"/>
@@ -20637,21 +21129,46 @@
     </row>
     <row r="388" spans="1:20" ht="18" customHeight="1">
       <c r="A388" s="45"/>
-      <c r="B388" s="61"/>
-      <c r="C388" s="61"/>
-      <c r="D388" s="61"/>
-      <c r="E388" s="45"/>
-      <c r="F388" s="61"/>
-      <c r="G388" s="61"/>
+      <c r="B388" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C388" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D388" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E388" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F388" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G388" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H388" s="45"/>
-      <c r="I388" s="45"/>
-      <c r="J388" s="45"/>
+      <c r="I388" s="61">
+        <v>50</v>
+      </c>
+      <c r="J388" s="49">
+        <f t="shared" si="14"/>
+        <v>1.2133032694475701E-6</v>
+      </c>
       <c r="K388" s="45"/>
-      <c r="L388" s="61"/>
-      <c r="M388" s="61"/>
-      <c r="N388" s="61"/>
+      <c r="L388" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M388" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N388" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O388" s="45"/>
-      <c r="P388" s="45"/>
+      <c r="P388" s="45">
+        <v>121.330326944757</v>
+      </c>
       <c r="Q388" s="45"/>
       <c r="R388" s="45"/>
       <c r="S388" s="37"/>
@@ -20659,21 +21176,46 @@
     </row>
     <row r="389" spans="1:20" ht="18" customHeight="1">
       <c r="A389" s="45"/>
-      <c r="B389" s="61"/>
-      <c r="C389" s="61"/>
-      <c r="D389" s="61"/>
-      <c r="E389" s="45"/>
-      <c r="F389" s="61"/>
-      <c r="G389" s="61"/>
+      <c r="B389" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C389" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D389" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E389" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F389" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G389" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H389" s="45"/>
-      <c r="I389" s="45"/>
-      <c r="J389" s="45"/>
+      <c r="I389" s="61">
+        <v>50</v>
+      </c>
+      <c r="J389" s="49">
+        <f t="shared" si="14"/>
+        <v>1.1287485907553501E-6</v>
+      </c>
       <c r="K389" s="45"/>
-      <c r="L389" s="61"/>
-      <c r="M389" s="61"/>
-      <c r="N389" s="61"/>
+      <c r="L389" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M389" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N389" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O389" s="45"/>
-      <c r="P389" s="45"/>
+      <c r="P389" s="45">
+        <v>112.874859075535</v>
+      </c>
       <c r="Q389" s="45"/>
       <c r="R389" s="45"/>
       <c r="S389" s="37"/>
@@ -20681,21 +21223,46 @@
     </row>
     <row r="390" spans="1:20" ht="18" customHeight="1">
       <c r="A390" s="45"/>
-      <c r="B390" s="61"/>
-      <c r="C390" s="61"/>
-      <c r="D390" s="61"/>
-      <c r="E390" s="45"/>
-      <c r="F390" s="61"/>
-      <c r="G390" s="61"/>
+      <c r="B390" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C390" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D390" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E390" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F390" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G390" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H390" s="45"/>
-      <c r="I390" s="45"/>
-      <c r="J390" s="45"/>
+      <c r="I390" s="61">
+        <v>50</v>
+      </c>
+      <c r="J390" s="49">
+        <f t="shared" si="14"/>
+        <v>1.0002254791431701E-6</v>
+      </c>
       <c r="K390" s="45"/>
-      <c r="L390" s="61"/>
-      <c r="M390" s="61"/>
-      <c r="N390" s="61"/>
+      <c r="L390" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M390" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N390" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O390" s="45"/>
-      <c r="P390" s="45"/>
+      <c r="P390" s="45">
+        <v>100.022547914317</v>
+      </c>
       <c r="Q390" s="45"/>
       <c r="R390" s="45"/>
       <c r="S390" s="37"/>
@@ -20703,21 +21270,46 @@
     </row>
     <row r="391" spans="1:20" ht="18" customHeight="1">
       <c r="A391" s="45"/>
-      <c r="B391" s="61"/>
-      <c r="C391" s="61"/>
-      <c r="D391" s="61"/>
-      <c r="E391" s="45"/>
-      <c r="F391" s="61"/>
-      <c r="G391" s="61"/>
+      <c r="B391" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C391" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D391" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E391" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F391" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G391" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H391" s="45"/>
-      <c r="I391" s="45"/>
-      <c r="J391" s="45"/>
+      <c r="I391" s="61">
+        <v>50</v>
+      </c>
+      <c r="J391" s="49">
+        <f t="shared" si="14"/>
+        <v>9.5625704622322398E-7</v>
+      </c>
       <c r="K391" s="45"/>
-      <c r="L391" s="61"/>
-      <c r="M391" s="61"/>
-      <c r="N391" s="61"/>
+      <c r="L391" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M391" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N391" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O391" s="45"/>
-      <c r="P391" s="45"/>
+      <c r="P391" s="45">
+        <v>95.625704622322402</v>
+      </c>
       <c r="Q391" s="45"/>
       <c r="R391" s="45"/>
       <c r="S391" s="37"/>
@@ -20725,21 +21317,46 @@
     </row>
     <row r="392" spans="1:20" ht="18" customHeight="1">
       <c r="A392" s="45"/>
-      <c r="B392" s="61"/>
-      <c r="C392" s="61"/>
-      <c r="D392" s="61"/>
-      <c r="E392" s="45"/>
-      <c r="F392" s="61"/>
-      <c r="G392" s="61"/>
+      <c r="B392" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C392" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D392" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E392" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F392" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G392" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H392" s="45"/>
-      <c r="I392" s="45"/>
-      <c r="J392" s="45"/>
+      <c r="I392" s="61">
+        <v>100</v>
+      </c>
+      <c r="J392" s="49">
+        <f t="shared" si="14"/>
+        <v>1.0617812852311101E-6</v>
+      </c>
       <c r="K392" s="45"/>
-      <c r="L392" s="61"/>
-      <c r="M392" s="61"/>
-      <c r="N392" s="61"/>
+      <c r="L392" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M392" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N392" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O392" s="45"/>
-      <c r="P392" s="45"/>
+      <c r="P392" s="45">
+        <v>106.178128523111</v>
+      </c>
       <c r="Q392" s="45"/>
       <c r="R392" s="45"/>
       <c r="S392" s="37"/>
@@ -20747,21 +21364,46 @@
     </row>
     <row r="393" spans="1:20" ht="18" customHeight="1">
       <c r="A393" s="45"/>
-      <c r="B393" s="61"/>
-      <c r="C393" s="61"/>
-      <c r="D393" s="61"/>
-      <c r="E393" s="45"/>
-      <c r="F393" s="61"/>
-      <c r="G393" s="61"/>
+      <c r="B393" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C393" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D393" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E393" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F393" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G393" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H393" s="45"/>
-      <c r="I393" s="45"/>
-      <c r="J393" s="45"/>
+      <c r="I393" s="61">
+        <v>100</v>
+      </c>
+      <c r="J393" s="49">
+        <f t="shared" si="14"/>
+        <v>1.2315670800450901E-6</v>
+      </c>
       <c r="K393" s="45"/>
-      <c r="L393" s="61"/>
-      <c r="M393" s="61"/>
-      <c r="N393" s="61"/>
+      <c r="L393" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M393" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N393" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O393" s="45"/>
-      <c r="P393" s="45"/>
+      <c r="P393" s="45">
+        <v>123.156708004509</v>
+      </c>
       <c r="Q393" s="45"/>
       <c r="R393" s="45"/>
       <c r="S393" s="37"/>
@@ -20769,21 +21411,46 @@
     </row>
     <row r="394" spans="1:20" ht="18" customHeight="1">
       <c r="A394" s="45"/>
-      <c r="B394" s="61"/>
-      <c r="C394" s="61"/>
-      <c r="D394" s="61"/>
-      <c r="E394" s="45"/>
-      <c r="F394" s="61"/>
-      <c r="G394" s="61"/>
+      <c r="B394" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C394" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D394" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E394" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F394" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G394" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H394" s="45"/>
-      <c r="I394" s="45"/>
-      <c r="J394" s="45"/>
+      <c r="I394" s="61">
+        <v>100</v>
+      </c>
+      <c r="J394" s="49">
+        <f t="shared" si="14"/>
+        <v>1.14904171364148E-6</v>
+      </c>
       <c r="K394" s="45"/>
-      <c r="L394" s="61"/>
-      <c r="M394" s="61"/>
-      <c r="N394" s="61"/>
+      <c r="L394" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M394" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N394" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O394" s="45"/>
-      <c r="P394" s="45"/>
+      <c r="P394" s="45">
+        <v>114.904171364148</v>
+      </c>
       <c r="Q394" s="45"/>
       <c r="R394" s="45"/>
       <c r="S394" s="37"/>
@@ -20791,21 +21458,46 @@
     </row>
     <row r="395" spans="1:20" ht="18" customHeight="1">
       <c r="A395" s="45"/>
-      <c r="B395" s="61"/>
-      <c r="C395" s="61"/>
-      <c r="D395" s="61"/>
-      <c r="E395" s="45"/>
-      <c r="F395" s="61"/>
-      <c r="G395" s="61"/>
+      <c r="B395" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C395" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D395" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E395" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F395" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G395" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H395" s="45"/>
-      <c r="I395" s="45"/>
-      <c r="J395" s="45"/>
+      <c r="I395" s="61">
+        <v>100</v>
+      </c>
+      <c r="J395" s="49">
+        <f t="shared" si="14"/>
+        <v>1.02660653889515E-6</v>
+      </c>
       <c r="K395" s="45"/>
-      <c r="L395" s="61"/>
-      <c r="M395" s="61"/>
-      <c r="N395" s="61"/>
+      <c r="L395" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M395" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N395" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O395" s="45"/>
-      <c r="P395" s="45"/>
+      <c r="P395" s="45">
+        <v>102.660653889515</v>
+      </c>
       <c r="Q395" s="45"/>
       <c r="R395" s="45"/>
       <c r="S395" s="37"/>
@@ -20813,21 +21505,46 @@
     </row>
     <row r="396" spans="1:20" ht="18" customHeight="1">
       <c r="A396" s="45"/>
-      <c r="B396" s="61"/>
-      <c r="C396" s="61"/>
-      <c r="D396" s="61"/>
-      <c r="E396" s="45"/>
-      <c r="F396" s="61"/>
-      <c r="G396" s="61"/>
+      <c r="B396" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C396" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D396" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E396" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F396" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G396" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H396" s="45"/>
-      <c r="I396" s="45"/>
-      <c r="J396" s="45"/>
+      <c r="I396" s="61">
+        <v>100</v>
+      </c>
+      <c r="J396" s="49">
+        <f t="shared" si="14"/>
+        <v>9.8872604284103699E-7</v>
+      </c>
       <c r="K396" s="45"/>
-      <c r="L396" s="61"/>
-      <c r="M396" s="61"/>
-      <c r="N396" s="61"/>
+      <c r="L396" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M396" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N396" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O396" s="45"/>
-      <c r="P396" s="45"/>
+      <c r="P396" s="45">
+        <v>98.872604284103701</v>
+      </c>
       <c r="Q396" s="45"/>
       <c r="R396" s="45"/>
       <c r="S396" s="37"/>
@@ -20835,21 +21552,46 @@
     </row>
     <row r="397" spans="1:20" ht="18" customHeight="1">
       <c r="A397" s="45"/>
-      <c r="B397" s="61"/>
-      <c r="C397" s="61"/>
-      <c r="D397" s="61"/>
-      <c r="E397" s="45"/>
-      <c r="F397" s="61"/>
-      <c r="G397" s="61"/>
+      <c r="B397" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C397" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D397" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E397" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F397" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G397" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H397" s="45"/>
-      <c r="I397" s="45"/>
-      <c r="J397" s="45"/>
+      <c r="I397" s="61">
+        <v>300</v>
+      </c>
+      <c r="J397" s="49">
+        <f t="shared" si="14"/>
+        <v>1.14768883878241E-6</v>
+      </c>
       <c r="K397" s="45"/>
-      <c r="L397" s="61"/>
-      <c r="M397" s="61"/>
-      <c r="N397" s="61"/>
+      <c r="L397" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M397" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N397" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O397" s="45"/>
-      <c r="P397" s="45"/>
+      <c r="P397" s="45">
+        <v>114.768883878241</v>
+      </c>
       <c r="Q397" s="45"/>
       <c r="R397" s="45"/>
       <c r="S397" s="37"/>
@@ -20857,21 +21599,46 @@
     </row>
     <row r="398" spans="1:20" ht="18" customHeight="1">
       <c r="A398" s="45"/>
-      <c r="B398" s="61"/>
-      <c r="C398" s="61"/>
-      <c r="D398" s="61"/>
-      <c r="E398" s="45"/>
-      <c r="F398" s="61"/>
-      <c r="G398" s="61"/>
+      <c r="B398" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C398" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D398" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E398" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F398" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G398" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H398" s="45"/>
-      <c r="I398" s="45"/>
-      <c r="J398" s="45"/>
+      <c r="I398" s="61">
+        <v>300</v>
+      </c>
+      <c r="J398" s="49">
+        <f t="shared" si="14"/>
+        <v>1.3032694475760901E-6</v>
+      </c>
       <c r="K398" s="45"/>
-      <c r="L398" s="61"/>
-      <c r="M398" s="61"/>
-      <c r="N398" s="61"/>
+      <c r="L398" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M398" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N398" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O398" s="45"/>
-      <c r="P398" s="45"/>
+      <c r="P398" s="45">
+        <v>130.326944757609</v>
+      </c>
       <c r="Q398" s="45"/>
       <c r="R398" s="45"/>
       <c r="S398" s="37"/>
@@ -20879,21 +21646,46 @@
     </row>
     <row r="399" spans="1:20" ht="18" customHeight="1">
       <c r="A399" s="45"/>
-      <c r="B399" s="61"/>
-      <c r="C399" s="61"/>
-      <c r="D399" s="61"/>
-      <c r="E399" s="45"/>
-      <c r="F399" s="61"/>
-      <c r="G399" s="61"/>
+      <c r="B399" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C399" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D399" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E399" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F399" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G399" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H399" s="45"/>
-      <c r="I399" s="45"/>
-      <c r="J399" s="45"/>
+      <c r="I399" s="61">
+        <v>300</v>
+      </c>
+      <c r="J399" s="49">
+        <f t="shared" si="14"/>
+        <v>1.2369785794813901E-6</v>
+      </c>
       <c r="K399" s="45"/>
-      <c r="L399" s="61"/>
-      <c r="M399" s="61"/>
-      <c r="N399" s="61"/>
+      <c r="L399" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M399" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N399" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O399" s="45"/>
-      <c r="P399" s="45"/>
+      <c r="P399" s="45">
+        <v>123.697857948139</v>
+      </c>
       <c r="Q399" s="45"/>
       <c r="R399" s="45"/>
       <c r="S399" s="37"/>
@@ -20901,21 +21693,46 @@
     </row>
     <row r="400" spans="1:20" ht="18" customHeight="1">
       <c r="A400" s="45"/>
-      <c r="B400" s="61"/>
-      <c r="C400" s="61"/>
-      <c r="D400" s="61"/>
-      <c r="E400" s="45"/>
-      <c r="F400" s="61"/>
-      <c r="G400" s="61"/>
+      <c r="B400" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C400" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D400" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E400" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F400" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G400" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H400" s="45"/>
-      <c r="I400" s="45"/>
-      <c r="J400" s="45"/>
+      <c r="I400" s="61">
+        <v>300</v>
+      </c>
+      <c r="J400" s="49">
+        <f t="shared" si="14"/>
+        <v>1.14024802705749E-6</v>
+      </c>
       <c r="K400" s="45"/>
-      <c r="L400" s="61"/>
-      <c r="M400" s="61"/>
-      <c r="N400" s="61"/>
+      <c r="L400" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M400" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N400" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O400" s="45"/>
-      <c r="P400" s="45"/>
+      <c r="P400" s="45">
+        <v>114.024802705749</v>
+      </c>
       <c r="Q400" s="45"/>
       <c r="R400" s="45"/>
       <c r="S400" s="37"/>
@@ -20923,21 +21740,46 @@
     </row>
     <row r="401" spans="1:20" ht="18" customHeight="1">
       <c r="A401" s="45"/>
-      <c r="B401" s="61"/>
-      <c r="C401" s="61"/>
-      <c r="D401" s="61"/>
-      <c r="E401" s="45"/>
-      <c r="F401" s="61"/>
-      <c r="G401" s="61"/>
+      <c r="B401" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C401" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D401" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E401" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F401" s="61" t="s">
+        <v>305</v>
+      </c>
+      <c r="G401" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H401" s="45"/>
-      <c r="I401" s="45"/>
-      <c r="J401" s="45"/>
+      <c r="I401" s="61">
+        <v>300</v>
+      </c>
+      <c r="J401" s="49">
+        <f t="shared" si="14"/>
+        <v>1.12130777903043E-6</v>
+      </c>
       <c r="K401" s="62"/>
-      <c r="L401" s="61"/>
-      <c r="M401" s="61"/>
-      <c r="N401" s="61"/>
+      <c r="L401" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="M401" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="N401" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O401" s="45"/>
-      <c r="P401" s="45"/>
+      <c r="P401" s="45">
+        <v>112.130777903043</v>
+      </c>
       <c r="Q401" s="45"/>
       <c r="R401" s="45"/>
       <c r="S401" s="37"/>
@@ -33215,6 +34057,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -33229,11 +34076,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- parsed `10.1016/j.matchemphys.2005.01.001` and adjusted data from previous commit
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C20162-90F7-9D4F-B3DE-FD959AF055C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF19851-58DD-874B-AD5D-75D609785CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3756" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="327">
   <si>
     <r>
       <rPr>
@@ -1075,9 +1075,6 @@
     <t>homogenized in Ar at 1473K for 2h cold rolled to 70% reduction and annealed at 1273K for 1h followed by water quench</t>
   </si>
   <si>
-    <t>pit nucleation resistance</t>
-  </si>
-  <si>
     <t>10.1016/j.jallcom.2022.164641</t>
   </si>
   <si>
@@ -1085,6 +1082,36 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>FeCoNiCr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeCoNiCrCu0.5 </t>
+  </si>
+  <si>
+    <t>FeCoNiCrCu1</t>
+  </si>
+  <si>
+    <t>passive current density</t>
+  </si>
+  <si>
+    <t>A/m^2</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>corrosion potential</t>
+  </si>
+  <si>
+    <t>pitting potential</t>
+  </si>
+  <si>
+    <t>corrosion current density</t>
+  </si>
+  <si>
+    <t>10.1016/j.matchemphys.2005.01.001</t>
   </si>
 </sst>
 </file>
@@ -2106,7 +2133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2411,6 +2438,10 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3573,8 +3604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T962"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A388" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F411" sqref="F411"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A394" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N431" sqref="N431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -21830,35 +21861,41 @@
         <v>313</v>
       </c>
       <c r="F402" s="61" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="G402" s="61" t="s">
         <v>29</v>
       </c>
       <c r="H402" s="61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I402" s="45">
         <v>298</v>
       </c>
-      <c r="J402" s="45">
-        <v>0.112</v>
+      <c r="J402" s="62">
+        <f>P402*0.0001</f>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="K402" s="62">
-        <v>1.6E-2</v>
+        <f>Q402*0.0001</f>
+        <v>6.0000000000000006E-4</v>
       </c>
       <c r="L402" s="61" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="M402" s="61" t="s">
         <v>86</v>
       </c>
       <c r="N402" s="61" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O402" s="45"/>
-      <c r="P402" s="45"/>
-      <c r="Q402" s="45"/>
+      <c r="P402" s="45">
+        <v>44</v>
+      </c>
+      <c r="Q402" s="45">
+        <v>6</v>
+      </c>
       <c r="R402" s="45"/>
       <c r="S402" s="37"/>
       <c r="T402" s="37"/>
@@ -21878,35 +21915,41 @@
         <v>313</v>
       </c>
       <c r="F403" s="61" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="G403" s="61" t="s">
         <v>29</v>
       </c>
       <c r="H403" s="61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I403" s="45">
         <v>298</v>
       </c>
-      <c r="J403" s="45">
-        <v>0.185</v>
+      <c r="J403" s="62">
+        <f t="shared" ref="J403:J406" si="15">P403*0.0001</f>
+        <v>3.4000000000000002E-3</v>
       </c>
       <c r="K403" s="62">
-        <v>2.1000000000000001E-2</v>
+        <f>Q403*0.0001</f>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="L403" s="61" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="M403" s="61" t="s">
         <v>86</v>
       </c>
       <c r="N403" s="61" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O403" s="45"/>
-      <c r="P403" s="45"/>
-      <c r="Q403" s="45"/>
+      <c r="P403" s="45">
+        <v>34</v>
+      </c>
+      <c r="Q403" s="45">
+        <v>4</v>
+      </c>
       <c r="R403" s="45"/>
       <c r="S403" s="37"/>
       <c r="T403" s="37"/>
@@ -21926,35 +21969,41 @@
         <v>313</v>
       </c>
       <c r="F404" s="61" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="G404" s="61" t="s">
         <v>29</v>
       </c>
       <c r="H404" s="61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I404" s="45">
         <v>298</v>
       </c>
       <c r="J404" s="62">
-        <v>0.32400000000000001</v>
+        <f t="shared" si="15"/>
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="K404" s="62">
-        <v>1.7999999999999999E-2</v>
+        <f>Q404*0.0001</f>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="L404" s="61" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="M404" s="61" t="s">
         <v>86</v>
       </c>
       <c r="N404" s="61" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O404" s="45"/>
-      <c r="P404" s="45"/>
-      <c r="Q404" s="45"/>
+      <c r="P404" s="45">
+        <v>47</v>
+      </c>
+      <c r="Q404" s="45">
+        <v>8</v>
+      </c>
       <c r="R404" s="45"/>
       <c r="S404" s="37"/>
       <c r="T404" s="37"/>
@@ -21974,230 +22023,514 @@
         <v>313</v>
       </c>
       <c r="F405" s="61" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="G405" s="61" t="s">
         <v>29</v>
       </c>
       <c r="H405" s="61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I405" s="45">
         <v>298</v>
       </c>
       <c r="J405" s="62">
-        <v>0.56799999999999995</v>
+        <f t="shared" si="15"/>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="K405" s="62">
-        <v>3.3000000000000002E-2</v>
+        <f>Q405*0.0001</f>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="L405" s="61" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="M405" s="61" t="s">
         <v>86</v>
       </c>
       <c r="N405" s="61" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O405" s="45"/>
-      <c r="P405" s="45"/>
-      <c r="Q405" s="45"/>
+      <c r="P405" s="45">
+        <v>56</v>
+      </c>
+      <c r="Q405" s="45">
+        <v>7</v>
+      </c>
       <c r="R405" s="45"/>
       <c r="S405" s="37"/>
       <c r="T405" s="37"/>
     </row>
     <row r="406" spans="1:20" ht="18" customHeight="1">
       <c r="A406" s="45"/>
-      <c r="B406" s="61"/>
-      <c r="C406" s="61"/>
-      <c r="D406" s="61"/>
-      <c r="E406" s="45"/>
-      <c r="F406" s="61"/>
-      <c r="G406" s="61"/>
-      <c r="H406" s="45"/>
-      <c r="I406" s="45"/>
-      <c r="J406" s="62"/>
-      <c r="K406" s="62"/>
-      <c r="L406" s="61"/>
-      <c r="M406" s="61"/>
-      <c r="N406" s="61"/>
+      <c r="B406" s="61" t="s">
+        <v>308</v>
+      </c>
+      <c r="C406" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D406" s="61" t="s">
+        <v>312</v>
+      </c>
+      <c r="E406" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="F406" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G406" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H406" s="61" t="s">
+        <v>315</v>
+      </c>
+      <c r="I406" s="45">
+        <v>298</v>
+      </c>
+      <c r="J406" s="45">
+        <f>P406*0.001</f>
+        <v>-0.17</v>
+      </c>
+      <c r="K406" s="49">
+        <f>Q406*0.0001</f>
+        <v>1.8000000000000002E-3</v>
+      </c>
+      <c r="L406" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M406" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N406" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O406" s="45"/>
-      <c r="P406" s="45"/>
-      <c r="Q406" s="45"/>
+      <c r="P406" s="45">
+        <v>-170</v>
+      </c>
+      <c r="Q406" s="45">
+        <v>18</v>
+      </c>
       <c r="R406" s="45"/>
       <c r="S406" s="37"/>
       <c r="T406" s="37"/>
     </row>
     <row r="407" spans="1:20" ht="18" customHeight="1">
       <c r="A407" s="45"/>
-      <c r="B407" s="61"/>
-      <c r="C407" s="61"/>
-      <c r="D407" s="61"/>
-      <c r="E407" s="45"/>
-      <c r="F407" s="61"/>
-      <c r="G407" s="61"/>
-      <c r="H407" s="45"/>
-      <c r="I407" s="45"/>
-      <c r="J407" s="62"/>
-      <c r="K407" s="45"/>
-      <c r="L407" s="61"/>
-      <c r="M407" s="61"/>
-      <c r="N407" s="61"/>
+      <c r="B407" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="C407" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D407" s="61" t="s">
+        <v>312</v>
+      </c>
+      <c r="E407" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="F407" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G407" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H407" s="61" t="s">
+        <v>315</v>
+      </c>
+      <c r="I407" s="45">
+        <v>298</v>
+      </c>
+      <c r="J407" s="45">
+        <f>P407*0.001</f>
+        <v>-0.156</v>
+      </c>
+      <c r="K407" s="49">
+        <f>Q407*0.0001</f>
+        <v>2.6000000000000003E-3</v>
+      </c>
+      <c r="L407" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M407" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N407" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O407" s="45"/>
-      <c r="P407" s="45"/>
-      <c r="Q407" s="45"/>
+      <c r="P407" s="45">
+        <v>-156</v>
+      </c>
+      <c r="Q407" s="45">
+        <v>26</v>
+      </c>
       <c r="R407" s="45"/>
       <c r="S407" s="37"/>
       <c r="T407" s="37"/>
     </row>
     <row r="408" spans="1:20" ht="18" customHeight="1">
       <c r="A408" s="45"/>
-      <c r="B408" s="61"/>
-      <c r="C408" s="61"/>
-      <c r="D408" s="61"/>
-      <c r="E408" s="45"/>
-      <c r="F408" s="61"/>
-      <c r="G408" s="61"/>
-      <c r="H408" s="45"/>
-      <c r="I408" s="45"/>
-      <c r="J408" s="62"/>
-      <c r="K408" s="45"/>
-      <c r="L408" s="61"/>
-      <c r="M408" s="61"/>
-      <c r="N408" s="61"/>
+      <c r="B408" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="C408" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D408" s="61" t="s">
+        <v>312</v>
+      </c>
+      <c r="E408" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="F408" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G408" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H408" s="61" t="s">
+        <v>315</v>
+      </c>
+      <c r="I408" s="45">
+        <v>298</v>
+      </c>
+      <c r="J408" s="45">
+        <f t="shared" ref="J408:J413" si="16">P408*0.001</f>
+        <v>-0.27</v>
+      </c>
+      <c r="K408" s="49">
+        <f>Q408*0.0001</f>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="L408" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M408" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N408" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O408" s="45"/>
-      <c r="P408" s="45"/>
-      <c r="Q408" s="45"/>
+      <c r="P408" s="45">
+        <v>-270</v>
+      </c>
+      <c r="Q408" s="45">
+        <v>17</v>
+      </c>
       <c r="R408" s="45"/>
       <c r="S408" s="37"/>
       <c r="T408" s="37"/>
     </row>
     <row r="409" spans="1:20" ht="18" customHeight="1">
       <c r="A409" s="45"/>
-      <c r="B409" s="61"/>
-      <c r="C409" s="61"/>
-      <c r="D409" s="61"/>
-      <c r="E409" s="45"/>
-      <c r="F409" s="61"/>
-      <c r="G409" s="61"/>
-      <c r="H409" s="45"/>
-      <c r="I409" s="45"/>
-      <c r="J409" s="62"/>
-      <c r="K409" s="45"/>
-      <c r="L409" s="61"/>
-      <c r="M409" s="61"/>
-      <c r="N409" s="61"/>
+      <c r="B409" s="61" t="s">
+        <v>311</v>
+      </c>
+      <c r="C409" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D409" s="61" t="s">
+        <v>312</v>
+      </c>
+      <c r="E409" s="61" t="s">
+        <v>313</v>
+      </c>
+      <c r="F409" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G409" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="H409" s="61" t="s">
+        <v>315</v>
+      </c>
+      <c r="I409" s="45">
+        <v>298</v>
+      </c>
+      <c r="J409" s="45">
+        <f t="shared" si="16"/>
+        <v>-0.30299999999999999</v>
+      </c>
+      <c r="K409" s="49">
+        <f>Q409*0.0001</f>
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="L409" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M409" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N409" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O409" s="45"/>
-      <c r="P409" s="45"/>
-      <c r="Q409" s="45"/>
+      <c r="P409" s="45">
+        <v>-303</v>
+      </c>
+      <c r="Q409" s="45">
+        <v>41</v>
+      </c>
       <c r="R409" s="45"/>
       <c r="S409" s="37"/>
       <c r="T409" s="37"/>
     </row>
     <row r="410" spans="1:20" ht="18" customHeight="1">
       <c r="A410" s="45"/>
-      <c r="B410" s="61"/>
-      <c r="C410" s="61"/>
-      <c r="D410" s="61"/>
-      <c r="E410" s="45"/>
-      <c r="F410" s="61"/>
-      <c r="G410" s="61"/>
-      <c r="H410" s="45"/>
-      <c r="I410" s="45"/>
-      <c r="J410" s="45"/>
-      <c r="K410" s="49"/>
-      <c r="L410" s="61"/>
-      <c r="M410" s="61"/>
-      <c r="N410" s="61"/>
+      <c r="B410" s="142" t="s">
+        <v>308</v>
+      </c>
+      <c r="C410" s="143" t="s">
+        <v>74</v>
+      </c>
+      <c r="D410" s="143" t="s">
+        <v>312</v>
+      </c>
+      <c r="E410" s="143" t="s">
+        <v>313</v>
+      </c>
+      <c r="F410" s="143" t="s">
+        <v>324</v>
+      </c>
+      <c r="G410" s="143" t="s">
+        <v>29</v>
+      </c>
+      <c r="H410" s="143" t="s">
+        <v>315</v>
+      </c>
+      <c r="I410" s="143">
+        <v>298</v>
+      </c>
+      <c r="J410" s="45">
+        <f t="shared" si="16"/>
+        <v>-5.8000000000000003E-2</v>
+      </c>
+      <c r="K410" s="49">
+        <f>Q410*0.0001</f>
+        <v>2.1000000000000003E-3</v>
+      </c>
+      <c r="L410" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M410" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N410" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O410" s="45"/>
-      <c r="P410" s="45"/>
-      <c r="Q410" s="45"/>
+      <c r="P410" s="45">
+        <v>-58</v>
+      </c>
+      <c r="Q410" s="45">
+        <v>21</v>
+      </c>
       <c r="R410" s="45"/>
       <c r="S410" s="37"/>
       <c r="T410" s="37"/>
     </row>
     <row r="411" spans="1:20" ht="18" customHeight="1">
       <c r="A411" s="45"/>
-      <c r="B411" s="61"/>
-      <c r="C411" s="61"/>
-      <c r="D411" s="61"/>
-      <c r="E411" s="45"/>
-      <c r="F411" s="61"/>
-      <c r="G411" s="61"/>
-      <c r="H411" s="45"/>
-      <c r="I411" s="45"/>
-      <c r="J411" s="45"/>
-      <c r="K411" s="49"/>
-      <c r="L411" s="61"/>
-      <c r="M411" s="61"/>
-      <c r="N411" s="61"/>
+      <c r="B411" s="144" t="s">
+        <v>309</v>
+      </c>
+      <c r="C411" s="145" t="s">
+        <v>74</v>
+      </c>
+      <c r="D411" s="145" t="s">
+        <v>312</v>
+      </c>
+      <c r="E411" s="145" t="s">
+        <v>313</v>
+      </c>
+      <c r="F411" s="143" t="s">
+        <v>324</v>
+      </c>
+      <c r="G411" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H411" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I411" s="145">
+        <v>298</v>
+      </c>
+      <c r="J411" s="45">
+        <f t="shared" si="16"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="K411" s="45">
+        <f>Q411*0.0001</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L411" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M411" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N411" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O411" s="45"/>
-      <c r="P411" s="45"/>
-      <c r="Q411" s="45"/>
+      <c r="P411" s="45">
+        <v>29</v>
+      </c>
+      <c r="Q411" s="45">
+        <v>30</v>
+      </c>
       <c r="R411" s="45"/>
       <c r="S411" s="37"/>
       <c r="T411" s="37"/>
     </row>
     <row r="412" spans="1:20" ht="18" customHeight="1">
       <c r="A412" s="45"/>
-      <c r="B412" s="61"/>
-      <c r="C412" s="63"/>
-      <c r="D412" s="61"/>
-      <c r="E412" s="45"/>
-      <c r="F412" s="61"/>
-      <c r="G412" s="61"/>
-      <c r="H412" s="45"/>
-      <c r="I412" s="45"/>
-      <c r="J412" s="45"/>
-      <c r="K412" s="49"/>
-      <c r="L412" s="61"/>
-      <c r="M412" s="61"/>
-      <c r="N412" s="61"/>
+      <c r="B412" s="144" t="s">
+        <v>310</v>
+      </c>
+      <c r="C412" s="145" t="s">
+        <v>74</v>
+      </c>
+      <c r="D412" s="145" t="s">
+        <v>312</v>
+      </c>
+      <c r="E412" s="145" t="s">
+        <v>313</v>
+      </c>
+      <c r="F412" s="143" t="s">
+        <v>324</v>
+      </c>
+      <c r="G412" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H412" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I412" s="145">
+        <v>298</v>
+      </c>
+      <c r="J412" s="45">
+        <f t="shared" si="16"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K412" s="45">
+        <f>Q412*0.0001</f>
+        <v>1.7000000000000001E-3</v>
+      </c>
+      <c r="L412" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M412" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N412" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O412" s="45"/>
-      <c r="P412" s="45"/>
-      <c r="Q412" s="45"/>
+      <c r="P412" s="45">
+        <v>54</v>
+      </c>
+      <c r="Q412" s="45">
+        <v>17</v>
+      </c>
       <c r="R412" s="45"/>
       <c r="S412" s="37"/>
       <c r="T412" s="37"/>
     </row>
     <row r="413" spans="1:20" ht="18" customHeight="1">
       <c r="A413" s="45"/>
-      <c r="B413" s="61"/>
-      <c r="C413" s="61"/>
-      <c r="D413" s="61"/>
-      <c r="E413" s="45"/>
-      <c r="F413" s="61"/>
-      <c r="G413" s="61"/>
-      <c r="H413" s="45"/>
-      <c r="I413" s="45"/>
-      <c r="J413" s="49"/>
-      <c r="K413" s="49"/>
-      <c r="L413" s="61"/>
-      <c r="M413" s="61"/>
-      <c r="N413" s="61"/>
+      <c r="B413" s="144" t="s">
+        <v>311</v>
+      </c>
+      <c r="C413" s="145" t="s">
+        <v>74</v>
+      </c>
+      <c r="D413" s="145" t="s">
+        <v>312</v>
+      </c>
+      <c r="E413" s="145" t="s">
+        <v>313</v>
+      </c>
+      <c r="F413" s="143" t="s">
+        <v>324</v>
+      </c>
+      <c r="G413" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H413" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I413" s="145">
+        <v>298</v>
+      </c>
+      <c r="J413" s="45">
+        <f t="shared" si="16"/>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="K413" s="45">
+        <f>Q413*0.0001</f>
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="L413" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M413" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="N413" s="61" t="s">
+        <v>314</v>
+      </c>
       <c r="O413" s="45"/>
-      <c r="P413" s="45"/>
-      <c r="Q413" s="45"/>
+      <c r="P413" s="45">
+        <v>265</v>
+      </c>
+      <c r="Q413" s="45">
+        <v>49</v>
+      </c>
       <c r="R413" s="45"/>
       <c r="S413" s="37"/>
       <c r="T413" s="37"/>
     </row>
     <row r="414" spans="1:20" ht="18" customHeight="1">
       <c r="A414" s="45"/>
-      <c r="B414" s="61"/>
-      <c r="C414" s="61"/>
-      <c r="D414" s="61"/>
-      <c r="E414" s="45"/>
-      <c r="F414" s="61"/>
-      <c r="G414" s="61"/>
-      <c r="H414" s="45"/>
-      <c r="I414" s="45"/>
-      <c r="J414" s="49"/>
-      <c r="K414" s="49"/>
-      <c r="L414" s="61"/>
-      <c r="M414" s="61"/>
-      <c r="N414" s="61"/>
+      <c r="B414" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="C414" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D414" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E414" s="61"/>
+      <c r="F414" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G414" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H414" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I414" s="145">
+        <v>298</v>
+      </c>
+      <c r="J414" s="62">
+        <v>-0.26</v>
+      </c>
+      <c r="K414" s="45"/>
+      <c r="L414" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M414" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N414" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O414" s="45"/>
       <c r="P414" s="45"/>
       <c r="Q414" s="45"/>
@@ -22207,19 +22540,41 @@
     </row>
     <row r="415" spans="1:20" ht="18" customHeight="1">
       <c r="A415" s="45"/>
-      <c r="B415" s="61"/>
-      <c r="C415" s="61"/>
-      <c r="D415" s="61"/>
+      <c r="B415" s="61" t="s">
+        <v>318</v>
+      </c>
+      <c r="C415" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D415" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E415" s="61"/>
-      <c r="F415" s="61"/>
-      <c r="G415" s="61"/>
-      <c r="H415" s="45"/>
-      <c r="I415" s="45"/>
-      <c r="J415" s="49"/>
-      <c r="K415" s="45"/>
-      <c r="L415" s="61"/>
-      <c r="M415" s="61"/>
-      <c r="N415" s="61"/>
+      <c r="F415" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G415" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H415" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I415" s="145">
+        <v>298</v>
+      </c>
+      <c r="J415" s="62">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="K415" s="62"/>
+      <c r="L415" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M415" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N415" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O415" s="45"/>
       <c r="P415" s="45"/>
       <c r="Q415" s="45"/>
@@ -22229,19 +22584,41 @@
     </row>
     <row r="416" spans="1:20" ht="18" customHeight="1">
       <c r="A416" s="45"/>
-      <c r="B416" s="61"/>
-      <c r="C416" s="61"/>
-      <c r="D416" s="61"/>
+      <c r="B416" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="C416" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D416" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E416" s="61"/>
-      <c r="F416" s="61"/>
-      <c r="G416" s="61"/>
-      <c r="H416" s="45"/>
-      <c r="I416" s="45"/>
-      <c r="J416" s="49"/>
-      <c r="K416" s="45"/>
-      <c r="L416" s="61"/>
-      <c r="M416" s="61"/>
-      <c r="N416" s="61"/>
+      <c r="F416" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G416" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H416" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I416" s="145">
+        <v>298</v>
+      </c>
+      <c r="J416" s="62">
+        <v>-0.33</v>
+      </c>
+      <c r="K416" s="62"/>
+      <c r="L416" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M416" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N416" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O416" s="45"/>
       <c r="P416" s="45"/>
       <c r="Q416" s="45"/>
@@ -22251,19 +22628,41 @@
     </row>
     <row r="417" spans="1:20" ht="18" customHeight="1">
       <c r="A417" s="45"/>
-      <c r="B417" s="61"/>
-      <c r="C417" s="63"/>
-      <c r="D417" s="61"/>
+      <c r="B417" s="61" t="s">
+        <v>317</v>
+      </c>
+      <c r="C417" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D417" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E417" s="61"/>
-      <c r="F417" s="61"/>
-      <c r="G417" s="61"/>
-      <c r="H417" s="45"/>
-      <c r="I417" s="45"/>
-      <c r="J417" s="49"/>
-      <c r="K417" s="45"/>
-      <c r="L417" s="61"/>
-      <c r="M417" s="61"/>
-      <c r="N417" s="61"/>
+      <c r="F417" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="G417" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H417" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I417" s="145">
+        <v>298</v>
+      </c>
+      <c r="J417" s="62">
+        <v>0.31</v>
+      </c>
+      <c r="K417" s="62"/>
+      <c r="L417" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M417" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N417" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O417" s="45"/>
       <c r="P417" s="45"/>
       <c r="Q417" s="45"/>
@@ -22273,19 +22672,41 @@
     </row>
     <row r="418" spans="1:20" ht="18" customHeight="1">
       <c r="A418" s="45"/>
-      <c r="B418" s="61"/>
-      <c r="C418" s="61"/>
-      <c r="D418" s="61"/>
+      <c r="B418" s="61" t="s">
+        <v>318</v>
+      </c>
+      <c r="C418" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D418" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E418" s="61"/>
-      <c r="F418" s="61"/>
-      <c r="G418" s="61"/>
-      <c r="H418" s="45"/>
-      <c r="I418" s="45"/>
-      <c r="J418" s="45"/>
-      <c r="K418" s="45"/>
-      <c r="L418" s="61"/>
-      <c r="M418" s="61"/>
-      <c r="N418" s="61"/>
+      <c r="F418" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="G418" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H418" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I418" s="145">
+        <v>298</v>
+      </c>
+      <c r="J418" s="62">
+        <v>0.09</v>
+      </c>
+      <c r="K418" s="62"/>
+      <c r="L418" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M418" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N418" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O418" s="45"/>
       <c r="P418" s="45"/>
       <c r="Q418" s="45"/>
@@ -22295,19 +22716,41 @@
     </row>
     <row r="419" spans="1:20" ht="18" customHeight="1">
       <c r="A419" s="45"/>
-      <c r="B419" s="61"/>
-      <c r="C419" s="63"/>
-      <c r="D419" s="61"/>
+      <c r="B419" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="C419" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D419" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E419" s="61"/>
-      <c r="F419" s="61"/>
-      <c r="G419" s="61"/>
-      <c r="H419" s="45"/>
-      <c r="I419" s="45"/>
-      <c r="J419" s="45"/>
+      <c r="F419" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="G419" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H419" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I419" s="145">
+        <v>298</v>
+      </c>
+      <c r="J419" s="62">
+        <v>0.08</v>
+      </c>
       <c r="K419" s="62"/>
-      <c r="L419" s="61"/>
-      <c r="M419" s="61"/>
-      <c r="N419" s="61"/>
+      <c r="L419" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M419" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N419" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O419" s="45"/>
       <c r="P419" s="45"/>
       <c r="Q419" s="45"/>
@@ -22316,20 +22759,42 @@
       <c r="T419" s="37"/>
     </row>
     <row r="420" spans="1:20" ht="18" customHeight="1">
-      <c r="A420" s="45"/>
-      <c r="B420" s="61"/>
-      <c r="C420" s="61"/>
-      <c r="D420" s="61"/>
+      <c r="A420" s="61"/>
+      <c r="B420" s="142" t="s">
+        <v>317</v>
+      </c>
+      <c r="C420" s="143" t="s">
+        <v>74</v>
+      </c>
+      <c r="D420" s="143" t="s">
+        <v>63</v>
+      </c>
       <c r="E420" s="61"/>
-      <c r="F420" s="61"/>
-      <c r="G420" s="61"/>
-      <c r="H420" s="45"/>
-      <c r="I420" s="45"/>
-      <c r="J420" s="45"/>
+      <c r="F420" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="G420" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H420" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I420" s="145">
+        <v>298</v>
+      </c>
+      <c r="J420" s="62">
+        <v>3.1500000000000001E-4</v>
+      </c>
       <c r="K420" s="62"/>
-      <c r="L420" s="61"/>
-      <c r="M420" s="61"/>
-      <c r="N420" s="61"/>
+      <c r="L420" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="M420" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N420" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O420" s="45"/>
       <c r="P420" s="45"/>
       <c r="Q420" s="45"/>
@@ -22338,20 +22803,42 @@
       <c r="T420" s="37"/>
     </row>
     <row r="421" spans="1:20" ht="18" customHeight="1">
-      <c r="A421" s="45"/>
-      <c r="B421" s="61"/>
-      <c r="C421" s="63"/>
-      <c r="D421" s="61"/>
+      <c r="A421" s="61"/>
+      <c r="B421" s="144" t="s">
+        <v>318</v>
+      </c>
+      <c r="C421" s="145" t="s">
+        <v>93</v>
+      </c>
+      <c r="D421" s="145" t="s">
+        <v>63</v>
+      </c>
       <c r="E421" s="61"/>
-      <c r="F421" s="61"/>
-      <c r="G421" s="61"/>
-      <c r="H421" s="45"/>
-      <c r="I421" s="45"/>
-      <c r="J421" s="45"/>
+      <c r="F421" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="G421" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H421" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I421" s="145">
+        <v>298</v>
+      </c>
+      <c r="J421" s="62">
+        <v>7.2300000000000003E-3</v>
+      </c>
       <c r="K421" s="62"/>
-      <c r="L421" s="61"/>
-      <c r="M421" s="61"/>
-      <c r="N421" s="61"/>
+      <c r="L421" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="M421" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N421" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O421" s="45"/>
       <c r="P421" s="45"/>
       <c r="Q421" s="45"/>
@@ -22360,20 +22847,42 @@
       <c r="T421" s="37"/>
     </row>
     <row r="422" spans="1:20" ht="18" customHeight="1">
-      <c r="A422" s="45"/>
-      <c r="B422" s="61"/>
-      <c r="C422" s="61"/>
-      <c r="D422" s="61"/>
+      <c r="A422" s="61"/>
+      <c r="B422" s="144" t="s">
+        <v>319</v>
+      </c>
+      <c r="C422" s="145" t="s">
+        <v>93</v>
+      </c>
+      <c r="D422" s="145" t="s">
+        <v>63</v>
+      </c>
       <c r="E422" s="61"/>
-      <c r="F422" s="61"/>
-      <c r="G422" s="61"/>
-      <c r="H422" s="45"/>
-      <c r="I422" s="45"/>
-      <c r="J422" s="62"/>
+      <c r="F422" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="G422" s="145" t="s">
+        <v>29</v>
+      </c>
+      <c r="H422" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="I422" s="145">
+        <v>298</v>
+      </c>
+      <c r="J422" s="62">
+        <v>1.32E-2</v>
+      </c>
       <c r="K422" s="62"/>
-      <c r="L422" s="61"/>
-      <c r="M422" s="61"/>
-      <c r="N422" s="61"/>
+      <c r="L422" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="M422" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="N422" s="61" t="s">
+        <v>326</v>
+      </c>
       <c r="O422" s="45"/>
       <c r="P422" s="45"/>
       <c r="Q422" s="45"/>
@@ -22382,7 +22891,7 @@
       <c r="T422" s="37"/>
     </row>
     <row r="423" spans="1:20" ht="15" customHeight="1">
-      <c r="A423" s="45"/>
+      <c r="A423" s="61"/>
       <c r="B423" s="61"/>
       <c r="C423" s="61"/>
       <c r="D423" s="61"/>
@@ -22392,7 +22901,7 @@
       <c r="H423" s="45"/>
       <c r="I423" s="45"/>
       <c r="J423" s="62"/>
-      <c r="K423" s="62"/>
+      <c r="K423" s="45"/>
       <c r="L423" s="61"/>
       <c r="M423" s="61"/>
       <c r="N423" s="61"/>
@@ -22405,7 +22914,7 @@
     </row>
     <row r="424" spans="1:20" ht="15" customHeight="1">
       <c r="A424" s="61"/>
-      <c r="B424" s="61"/>
+      <c r="B424" s="45"/>
       <c r="C424" s="61"/>
       <c r="D424" s="61"/>
       <c r="E424" s="61"/>
@@ -22414,7 +22923,7 @@
       <c r="H424" s="45"/>
       <c r="I424" s="45"/>
       <c r="J424" s="62"/>
-      <c r="K424" s="62"/>
+      <c r="K424" s="45"/>
       <c r="L424" s="61"/>
       <c r="M424" s="61"/>
       <c r="N424" s="61"/>
@@ -22427,8 +22936,8 @@
     </row>
     <row r="425" spans="1:20" ht="15" customHeight="1">
       <c r="A425" s="61"/>
-      <c r="B425" s="61"/>
-      <c r="C425" s="61"/>
+      <c r="B425" s="45"/>
+      <c r="C425" s="63"/>
       <c r="D425" s="61"/>
       <c r="E425" s="61"/>
       <c r="F425" s="61"/>
@@ -22436,7 +22945,7 @@
       <c r="H425" s="45"/>
       <c r="I425" s="45"/>
       <c r="J425" s="62"/>
-      <c r="K425" s="62"/>
+      <c r="K425" s="45"/>
       <c r="L425" s="61"/>
       <c r="M425" s="61"/>
       <c r="N425" s="61"/>
@@ -22449,7 +22958,7 @@
     </row>
     <row r="426" spans="1:20" ht="15" customHeight="1">
       <c r="A426" s="61"/>
-      <c r="B426" s="61"/>
+      <c r="B426" s="45"/>
       <c r="C426" s="61"/>
       <c r="D426" s="61"/>
       <c r="E426" s="61"/>
@@ -22457,8 +22966,8 @@
       <c r="G426" s="61"/>
       <c r="H426" s="45"/>
       <c r="I426" s="45"/>
-      <c r="J426" s="62"/>
-      <c r="K426" s="62"/>
+      <c r="J426" s="45"/>
+      <c r="K426" s="45"/>
       <c r="L426" s="61"/>
       <c r="M426" s="61"/>
       <c r="N426" s="61"/>
@@ -22471,7 +22980,7 @@
     </row>
     <row r="427" spans="1:20" ht="15" customHeight="1">
       <c r="A427" s="61"/>
-      <c r="B427" s="61"/>
+      <c r="B427" s="45"/>
       <c r="C427" s="61"/>
       <c r="D427" s="61"/>
       <c r="E427" s="61"/>
@@ -22479,7 +22988,7 @@
       <c r="G427" s="61"/>
       <c r="H427" s="45"/>
       <c r="I427" s="45"/>
-      <c r="J427" s="62"/>
+      <c r="J427" s="45"/>
       <c r="K427" s="45"/>
       <c r="L427" s="61"/>
       <c r="M427" s="61"/>
@@ -22501,7 +23010,7 @@
       <c r="G428" s="61"/>
       <c r="H428" s="45"/>
       <c r="I428" s="45"/>
-      <c r="J428" s="62"/>
+      <c r="J428" s="45"/>
       <c r="K428" s="45"/>
       <c r="L428" s="61"/>
       <c r="M428" s="61"/>
@@ -22516,14 +23025,14 @@
     <row r="429" spans="1:20" ht="15" customHeight="1">
       <c r="A429" s="61"/>
       <c r="B429" s="45"/>
-      <c r="C429" s="63"/>
+      <c r="C429" s="61"/>
       <c r="D429" s="61"/>
       <c r="E429" s="61"/>
       <c r="F429" s="61"/>
       <c r="G429" s="61"/>
       <c r="H429" s="45"/>
       <c r="I429" s="45"/>
-      <c r="J429" s="62"/>
+      <c r="J429" s="45"/>
       <c r="K429" s="45"/>
       <c r="L429" s="61"/>
       <c r="M429" s="61"/>
@@ -22538,7 +23047,7 @@
     <row r="430" spans="1:20" ht="15" customHeight="1">
       <c r="A430" s="61"/>
       <c r="B430" s="45"/>
-      <c r="C430" s="61"/>
+      <c r="C430" s="45"/>
       <c r="D430" s="61"/>
       <c r="E430" s="61"/>
       <c r="F430" s="61"/>
@@ -22560,7 +23069,7 @@
     <row r="431" spans="1:20" ht="15" customHeight="1">
       <c r="A431" s="61"/>
       <c r="B431" s="45"/>
-      <c r="C431" s="61"/>
+      <c r="C431" s="45"/>
       <c r="D431" s="61"/>
       <c r="E431" s="61"/>
       <c r="F431" s="61"/>
@@ -22582,7 +23091,7 @@
     <row r="432" spans="1:20" ht="15" customHeight="1">
       <c r="A432" s="61"/>
       <c r="B432" s="45"/>
-      <c r="C432" s="61"/>
+      <c r="C432" s="45"/>
       <c r="D432" s="61"/>
       <c r="E432" s="61"/>
       <c r="F432" s="61"/>
@@ -22604,7 +23113,7 @@
     <row r="433" spans="1:20" ht="15" customHeight="1">
       <c r="A433" s="61"/>
       <c r="B433" s="45"/>
-      <c r="C433" s="61"/>
+      <c r="C433" s="45"/>
       <c r="D433" s="61"/>
       <c r="E433" s="61"/>
       <c r="F433" s="61"/>
@@ -22635,7 +23144,7 @@
       <c r="I434" s="45"/>
       <c r="J434" s="45"/>
       <c r="K434" s="45"/>
-      <c r="L434" s="61"/>
+      <c r="L434" s="45"/>
       <c r="M434" s="61"/>
       <c r="N434" s="61"/>
       <c r="O434" s="45"/>
@@ -22657,7 +23166,7 @@
       <c r="I435" s="45"/>
       <c r="J435" s="45"/>
       <c r="K435" s="45"/>
-      <c r="L435" s="61"/>
+      <c r="L435" s="45"/>
       <c r="M435" s="61"/>
       <c r="N435" s="61"/>
       <c r="O435" s="45"/>
@@ -22679,7 +23188,7 @@
       <c r="I436" s="45"/>
       <c r="J436" s="45"/>
       <c r="K436" s="45"/>
-      <c r="L436" s="61"/>
+      <c r="L436" s="45"/>
       <c r="M436" s="61"/>
       <c r="N436" s="61"/>
       <c r="O436" s="45"/>
@@ -22701,7 +23210,7 @@
       <c r="I437" s="45"/>
       <c r="J437" s="45"/>
       <c r="K437" s="45"/>
-      <c r="L437" s="61"/>
+      <c r="L437" s="45"/>
       <c r="M437" s="61"/>
       <c r="N437" s="61"/>
       <c r="O437" s="45"/>
@@ -22800,20 +23309,20 @@
       <c r="T441" s="37"/>
     </row>
     <row r="442" spans="1:20" ht="15" customHeight="1">
-      <c r="A442" s="61"/>
+      <c r="A442" s="45"/>
       <c r="B442" s="45"/>
       <c r="C442" s="45"/>
-      <c r="D442" s="61"/>
-      <c r="E442" s="61"/>
-      <c r="F442" s="61"/>
-      <c r="G442" s="61"/>
+      <c r="D442" s="45"/>
+      <c r="E442" s="45"/>
+      <c r="F442" s="45"/>
+      <c r="G442" s="45"/>
       <c r="H442" s="45"/>
       <c r="I442" s="45"/>
       <c r="J442" s="45"/>
       <c r="K442" s="45"/>
       <c r="L442" s="45"/>
-      <c r="M442" s="61"/>
-      <c r="N442" s="61"/>
+      <c r="M442" s="45"/>
+      <c r="N442" s="45"/>
       <c r="O442" s="45"/>
       <c r="P442" s="45"/>
       <c r="Q442" s="45"/>
@@ -22822,20 +23331,20 @@
       <c r="T442" s="37"/>
     </row>
     <row r="443" spans="1:20" ht="15" customHeight="1">
-      <c r="A443" s="61"/>
+      <c r="A443" s="45"/>
       <c r="B443" s="45"/>
       <c r="C443" s="45"/>
-      <c r="D443" s="61"/>
-      <c r="E443" s="61"/>
-      <c r="F443" s="61"/>
-      <c r="G443" s="61"/>
+      <c r="D443" s="45"/>
+      <c r="E443" s="45"/>
+      <c r="F443" s="45"/>
+      <c r="G443" s="45"/>
       <c r="H443" s="45"/>
       <c r="I443" s="45"/>
       <c r="J443" s="45"/>
       <c r="K443" s="45"/>
       <c r="L443" s="45"/>
-      <c r="M443" s="61"/>
-      <c r="N443" s="61"/>
+      <c r="M443" s="45"/>
+      <c r="N443" s="45"/>
       <c r="O443" s="45"/>
       <c r="P443" s="45"/>
       <c r="Q443" s="45"/>
@@ -22844,20 +23353,20 @@
       <c r="T443" s="37"/>
     </row>
     <row r="444" spans="1:20" ht="15" customHeight="1">
-      <c r="A444" s="61"/>
+      <c r="A444" s="45"/>
       <c r="B444" s="45"/>
       <c r="C444" s="45"/>
-      <c r="D444" s="61"/>
-      <c r="E444" s="61"/>
-      <c r="F444" s="61"/>
-      <c r="G444" s="61"/>
+      <c r="D444" s="45"/>
+      <c r="E444" s="45"/>
+      <c r="F444" s="45"/>
+      <c r="G444" s="45"/>
       <c r="H444" s="45"/>
       <c r="I444" s="45"/>
       <c r="J444" s="45"/>
       <c r="K444" s="45"/>
       <c r="L444" s="45"/>
-      <c r="M444" s="61"/>
-      <c r="N444" s="61"/>
+      <c r="M444" s="45"/>
+      <c r="N444" s="45"/>
       <c r="O444" s="45"/>
       <c r="P444" s="45"/>
       <c r="Q444" s="45"/>
@@ -22866,20 +23375,20 @@
       <c r="T444" s="37"/>
     </row>
     <row r="445" spans="1:20" ht="15" customHeight="1">
-      <c r="A445" s="61"/>
+      <c r="A445" s="45"/>
       <c r="B445" s="45"/>
       <c r="C445" s="45"/>
-      <c r="D445" s="61"/>
-      <c r="E445" s="61"/>
-      <c r="F445" s="61"/>
-      <c r="G445" s="61"/>
+      <c r="D445" s="45"/>
+      <c r="E445" s="45"/>
+      <c r="F445" s="45"/>
+      <c r="G445" s="45"/>
       <c r="H445" s="45"/>
       <c r="I445" s="45"/>
       <c r="J445" s="45"/>
       <c r="K445" s="45"/>
       <c r="L445" s="45"/>
-      <c r="M445" s="61"/>
-      <c r="N445" s="61"/>
+      <c r="M445" s="45"/>
+      <c r="N445" s="45"/>
       <c r="O445" s="45"/>
       <c r="P445" s="45"/>
       <c r="Q445" s="45"/>
@@ -33779,7 +34288,6 @@
     </row>
     <row r="941" spans="1:20" ht="15" customHeight="1">
       <c r="A941" s="45"/>
-      <c r="B941" s="45"/>
       <c r="C941" s="45"/>
       <c r="D941" s="45"/>
       <c r="E941" s="45"/>
@@ -33801,7 +34309,6 @@
     </row>
     <row r="942" spans="1:20" ht="15" customHeight="1">
       <c r="A942" s="45"/>
-      <c r="B942" s="45"/>
       <c r="C942" s="45"/>
       <c r="D942" s="45"/>
       <c r="E942" s="45"/>
@@ -33823,7 +34330,6 @@
     </row>
     <row r="943" spans="1:20" ht="15" customHeight="1">
       <c r="A943" s="45"/>
-      <c r="B943" s="45"/>
       <c r="C943" s="45"/>
       <c r="D943" s="45"/>
       <c r="E943" s="45"/>
@@ -33845,7 +34351,6 @@
     </row>
     <row r="944" spans="1:20" ht="15" customHeight="1">
       <c r="A944" s="45"/>
-      <c r="B944" s="45"/>
       <c r="C944" s="45"/>
       <c r="D944" s="45"/>
       <c r="E944" s="45"/>
@@ -33909,7 +34414,6 @@
     </row>
     <row r="947" spans="1:20" ht="15" customHeight="1">
       <c r="A947" s="45"/>
-      <c r="C947" s="45"/>
       <c r="D947" s="45"/>
       <c r="E947" s="45"/>
       <c r="F947" s="45"/>
@@ -33930,15 +34434,11 @@
     </row>
     <row r="948" spans="1:20" ht="15" customHeight="1">
       <c r="A948" s="45"/>
-      <c r="C948" s="45"/>
       <c r="D948" s="45"/>
       <c r="E948" s="45"/>
       <c r="F948" s="45"/>
       <c r="G948" s="45"/>
       <c r="H948" s="45"/>
-      <c r="I948" s="45"/>
-      <c r="J948" s="45"/>
-      <c r="K948" s="45"/>
       <c r="L948" s="45"/>
       <c r="M948" s="45"/>
       <c r="N948" s="45"/>
@@ -33951,15 +34451,11 @@
     </row>
     <row r="949" spans="1:20" ht="15" customHeight="1">
       <c r="A949" s="45"/>
-      <c r="C949" s="45"/>
       <c r="D949" s="45"/>
       <c r="E949" s="45"/>
       <c r="F949" s="45"/>
       <c r="G949" s="45"/>
       <c r="H949" s="45"/>
-      <c r="I949" s="45"/>
-      <c r="J949" s="45"/>
-      <c r="K949" s="45"/>
       <c r="L949" s="45"/>
       <c r="M949" s="45"/>
       <c r="N949" s="45"/>
@@ -33972,15 +34468,11 @@
     </row>
     <row r="950" spans="1:20" ht="15" customHeight="1">
       <c r="A950" s="45"/>
-      <c r="C950" s="45"/>
       <c r="D950" s="45"/>
       <c r="E950" s="45"/>
       <c r="F950" s="45"/>
       <c r="G950" s="45"/>
       <c r="H950" s="45"/>
-      <c r="I950" s="45"/>
-      <c r="J950" s="45"/>
-      <c r="K950" s="45"/>
       <c r="L950" s="45"/>
       <c r="M950" s="45"/>
       <c r="N950" s="45"/>
@@ -33998,10 +34490,6 @@
       <c r="F951" s="45"/>
       <c r="G951" s="45"/>
       <c r="H951" s="45"/>
-      <c r="I951" s="45"/>
-      <c r="J951" s="45"/>
-      <c r="K951" s="45"/>
-      <c r="L951" s="45"/>
       <c r="M951" s="45"/>
       <c r="N951" s="45"/>
       <c r="O951" s="45"/>
@@ -34018,7 +34506,6 @@
       <c r="F952" s="45"/>
       <c r="G952" s="45"/>
       <c r="H952" s="45"/>
-      <c r="L952" s="45"/>
       <c r="M952" s="45"/>
       <c r="N952" s="45"/>
       <c r="O952" s="45"/>
@@ -34035,7 +34522,6 @@
       <c r="F953" s="45"/>
       <c r="G953" s="45"/>
       <c r="H953" s="45"/>
-      <c r="L953" s="45"/>
       <c r="M953" s="45"/>
       <c r="N953" s="45"/>
       <c r="O953" s="45"/>
@@ -34052,7 +34538,6 @@
       <c r="F954" s="45"/>
       <c r="G954" s="45"/>
       <c r="H954" s="45"/>
-      <c r="L954" s="45"/>
       <c r="M954" s="45"/>
       <c r="N954" s="45"/>
       <c r="O954" s="45"/>
@@ -34120,71 +34605,27 @@
       <c r="M958" s="45"/>
       <c r="N958" s="45"/>
       <c r="O958" s="45"/>
-      <c r="P958" s="45"/>
       <c r="Q958" s="45"/>
       <c r="R958" s="45"/>
       <c r="S958" s="45"/>
       <c r="T958" s="45"/>
     </row>
     <row r="959" spans="1:20" ht="15" customHeight="1">
-      <c r="A959" s="45"/>
-      <c r="D959" s="45"/>
-      <c r="E959" s="45"/>
-      <c r="F959" s="45"/>
-      <c r="G959" s="45"/>
-      <c r="H959" s="45"/>
-      <c r="M959" s="45"/>
-      <c r="N959" s="45"/>
-      <c r="O959" s="45"/>
-      <c r="P959" s="45"/>
-      <c r="Q959" s="45"/>
       <c r="R959" s="45"/>
       <c r="S959" s="45"/>
       <c r="T959" s="45"/>
     </row>
     <row r="960" spans="1:20" ht="15" customHeight="1">
-      <c r="A960" s="45"/>
-      <c r="D960" s="45"/>
-      <c r="E960" s="45"/>
-      <c r="F960" s="45"/>
-      <c r="G960" s="45"/>
-      <c r="H960" s="45"/>
-      <c r="M960" s="45"/>
-      <c r="N960" s="45"/>
-      <c r="O960" s="45"/>
-      <c r="P960" s="45"/>
-      <c r="Q960" s="45"/>
       <c r="R960" s="45"/>
       <c r="S960" s="45"/>
       <c r="T960" s="45"/>
     </row>
-    <row r="961" spans="1:20" ht="15" customHeight="1">
-      <c r="A961" s="45"/>
-      <c r="D961" s="45"/>
-      <c r="E961" s="45"/>
-      <c r="F961" s="45"/>
-      <c r="G961" s="45"/>
-      <c r="H961" s="45"/>
-      <c r="M961" s="45"/>
-      <c r="N961" s="45"/>
-      <c r="O961" s="45"/>
-      <c r="P961" s="45"/>
-      <c r="Q961" s="45"/>
+    <row r="961" spans="18:20" ht="15" customHeight="1">
       <c r="R961" s="45"/>
       <c r="S961" s="45"/>
       <c r="T961" s="45"/>
     </row>
-    <row r="962" spans="1:20" ht="15" customHeight="1">
-      <c r="A962" s="45"/>
-      <c r="D962" s="45"/>
-      <c r="E962" s="45"/>
-      <c r="F962" s="45"/>
-      <c r="G962" s="45"/>
-      <c r="H962" s="45"/>
-      <c r="M962" s="45"/>
-      <c r="N962" s="45"/>
-      <c r="O962" s="45"/>
-      <c r="Q962" s="45"/>
+    <row r="962" spans="18:20" ht="15" customHeight="1">
       <c r="R962" s="45"/>
       <c r="S962" s="45"/>
       <c r="T962" s="45"/>

</xml_diff>

<commit_message>
- extracted extra data from `10.1016/j.intermet.2020.106778`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF19851-58DD-874B-AD5D-75D609785CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB7E7C4-F5E6-9D4E-892E-C361AF999FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3971" uniqueCount="330">
   <si>
     <r>
       <rPr>
@@ -1113,6 +1113,15 @@
   <si>
     <t>10.1016/j.matchemphys.2005.01.001</t>
   </si>
+  <si>
+    <t>FeCo Ni Al0.2 Si0.2</t>
+  </si>
+  <si>
+    <t>AAM+MS</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2020.106778</t>
+  </si>
 </sst>
 </file>
 
@@ -2133,7 +2142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2239,7 +2248,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3605,7 +3613,7 @@
   <dimension ref="A1:T962"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A394" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N431" sqref="N431"/>
+      <selection activeCell="N433" sqref="N433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -3662,19 +3670,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="106"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="113"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="112"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -3690,17 +3698,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="117"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="115"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="113"/>
+      <c r="N3" s="116"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -3741,43 +3749,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="120" t="s">
+      <c r="E5" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="120" t="s">
+      <c r="F5" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="120" t="s">
+      <c r="G5" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="120" t="s">
+      <c r="I5" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="120" t="s">
+      <c r="J5" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="120" t="s">
+      <c r="K5" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="120" t="s">
+      <c r="L5" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="120" t="s">
+      <c r="M5" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="120" t="s">
+      <c r="N5" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="125" t="s">
+      <c r="O5" s="124" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -3793,19 +3801,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="126"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="118"/>
+      <c r="N6" s="118"/>
+      <c r="O6" s="125"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -3816,216 +3824,216 @@
       <c r="A7" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="67" t="s">
+      <c r="G7" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="67">
         <v>298</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="67" t="s">
+      <c r="K7" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="67" t="s">
+      <c r="L7" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="67" t="s">
+      <c r="M7" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="67" t="s">
+      <c r="N7" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="127"/>
-      <c r="P7" s="69" t="s">
+      <c r="O7" s="126"/>
+      <c r="P7" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="69" t="s">
+      <c r="Q7" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="70" t="s">
+      <c r="R7" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="71"/>
+      <c r="S7" s="70"/>
       <c r="T7" s="29"/>
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="128" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="127" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131" t="s">
+      <c r="C8" s="128"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="133"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="134"/>
-      <c r="L8" s="135"/>
-      <c r="M8" s="136" t="s">
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="134"/>
+      <c r="M8" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="137"/>
-      <c r="O8" s="81" t="s">
+      <c r="N8" s="136"/>
+      <c r="O8" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="138" t="s">
+      <c r="P8" s="137" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="139"/>
-      <c r="R8" s="140"/>
-      <c r="S8" s="140"/>
-      <c r="T8" s="141"/>
+      <c r="Q8" s="138"/>
+      <c r="R8" s="139"/>
+      <c r="S8" s="139"/>
+      <c r="T8" s="140"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="E9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="86" t="s">
+      <c r="H9" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="86" t="s">
+      <c r="I9" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="86" t="s">
+      <c r="J9" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="87" t="s">
+      <c r="L9" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="88" t="s">
+      <c r="M9" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="N9" s="89" t="s">
+      <c r="N9" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="O9" s="90"/>
-      <c r="P9" s="91" t="s">
+      <c r="O9" s="89"/>
+      <c r="P9" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="Q9" s="92" t="s">
+      <c r="Q9" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="R9" s="92" t="s">
+      <c r="R9" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="S9" s="92" t="s">
+      <c r="S9" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="T9" s="93" t="s">
+      <c r="T9" s="92" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1">
       <c r="A10" s="30"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="74" t="s">
+      <c r="E10" s="71"/>
+      <c r="F10" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="75" t="s">
+      <c r="G10" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="I10" s="76">
+      <c r="I10" s="75">
         <v>298</v>
       </c>
-      <c r="J10" s="77">
+      <c r="J10" s="76">
         <v>571000000</v>
       </c>
-      <c r="K10" s="77">
+      <c r="K10" s="76">
         <v>15000000</v>
       </c>
-      <c r="L10" s="74" t="s">
+      <c r="L10" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="74"/>
-      <c r="N10" s="78" t="s">
+      <c r="M10" s="73"/>
+      <c r="N10" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="O10" s="79"/>
-      <c r="P10" s="80"/>
-      <c r="Q10" s="80"/>
-      <c r="R10" s="80"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="79"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="78"/>
+      <c r="T10" s="78"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1">
       <c r="A11" s="30"/>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="72"/>
+      <c r="E11" s="71"/>
       <c r="F11" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="75" t="s">
+      <c r="G11" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="76">
+      <c r="I11" s="75">
         <v>298</v>
       </c>
       <c r="J11" s="35">
@@ -4034,11 +4042,11 @@
       <c r="K11" s="35">
         <v>5000000</v>
       </c>
-      <c r="L11" s="74" t="s">
+      <c r="L11" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M11" s="32"/>
-      <c r="N11" s="78" t="s">
+      <c r="N11" s="77" t="s">
         <v>101</v>
       </c>
       <c r="O11" s="37"/>
@@ -4050,26 +4058,26 @@
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1">
       <c r="A12" s="30"/>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="72"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="75" t="s">
+      <c r="G12" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="I12" s="76">
+      <c r="I12" s="75">
         <v>298</v>
       </c>
       <c r="J12" s="35">
@@ -4078,11 +4086,11 @@
       <c r="K12" s="35">
         <v>0.3</v>
       </c>
-      <c r="L12" s="74" t="s">
+      <c r="L12" s="73" t="s">
         <v>67</v>
       </c>
       <c r="M12" s="32"/>
-      <c r="N12" s="78" t="s">
+      <c r="N12" s="77" t="s">
         <v>101</v>
       </c>
       <c r="O12" s="37"/>
@@ -4094,13 +4102,13 @@
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1">
       <c r="A13" s="30"/>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="31" t="s">
@@ -4109,26 +4117,26 @@
       <c r="F13" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="74" t="s">
+      <c r="G13" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="76">
+      <c r="I13" s="75">
         <v>298</v>
       </c>
       <c r="J13" s="35">
         <v>1678000000</v>
       </c>
       <c r="K13" s="35"/>
-      <c r="L13" s="74" t="s">
+      <c r="L13" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M13" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N13" s="78" t="s">
+      <c r="N13" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O13" s="37"/>
@@ -4140,13 +4148,13 @@
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1">
       <c r="A14" s="30"/>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="73" t="s">
+      <c r="D14" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="31" t="s">
@@ -4155,26 +4163,26 @@
       <c r="F14" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="74" t="s">
+      <c r="G14" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H14" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="76">
+      <c r="I14" s="75">
         <v>298</v>
       </c>
       <c r="J14" s="35">
         <v>1397000000</v>
       </c>
       <c r="K14" s="35"/>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M14" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N14" s="78" t="s">
+      <c r="N14" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O14" s="37"/>
@@ -4186,13 +4194,13 @@
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1">
       <c r="A15" s="30"/>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="31" t="s">
@@ -4201,26 +4209,26 @@
       <c r="F15" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="74" t="s">
+      <c r="G15" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I15" s="76">
+      <c r="I15" s="75">
         <v>298</v>
       </c>
       <c r="J15" s="62">
         <v>1248000000</v>
       </c>
       <c r="K15" s="35"/>
-      <c r="L15" s="74" t="s">
+      <c r="L15" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M15" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N15" s="78" t="s">
+      <c r="N15" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O15" s="37"/>
@@ -4232,13 +4240,13 @@
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1">
       <c r="A16" s="30"/>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="73" t="s">
+      <c r="D16" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="31" t="s">
@@ -4247,26 +4255,26 @@
       <c r="F16" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="74" t="s">
+      <c r="G16" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I16" s="76">
+      <c r="I16" s="75">
         <v>298</v>
       </c>
       <c r="J16" s="62">
         <v>1168000000</v>
       </c>
       <c r="K16" s="38"/>
-      <c r="L16" s="74" t="s">
+      <c r="L16" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M16" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N16" s="78" t="s">
+      <c r="N16" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O16" s="37"/>
@@ -4278,13 +4286,13 @@
     </row>
     <row r="17" spans="1:20" ht="18.75" customHeight="1">
       <c r="A17" s="38"/>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="31" t="s">
@@ -4293,26 +4301,26 @@
       <c r="F17" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="74" t="s">
+      <c r="G17" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I17" s="76">
+      <c r="I17" s="75">
         <v>298</v>
       </c>
       <c r="J17" s="62">
         <v>2963000000</v>
       </c>
       <c r="K17" s="38"/>
-      <c r="L17" s="74" t="s">
+      <c r="L17" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M17" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N17" s="78" t="s">
+      <c r="N17" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O17" s="37"/>
@@ -4324,13 +4332,13 @@
     </row>
     <row r="18" spans="1:20" ht="18.75" customHeight="1">
       <c r="A18" s="38"/>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="31" t="s">
@@ -4339,26 +4347,26 @@
       <c r="F18" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="74" t="s">
+      <c r="G18" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H18" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="76">
+      <c r="I18" s="75">
         <v>298</v>
       </c>
       <c r="J18" s="62">
         <v>3281000000</v>
       </c>
       <c r="K18" s="38"/>
-      <c r="L18" s="74" t="s">
+      <c r="L18" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M18" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N18" s="78" t="s">
+      <c r="N18" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O18" s="37"/>
@@ -4370,13 +4378,13 @@
     </row>
     <row r="19" spans="1:20" ht="18.75" customHeight="1">
       <c r="A19" s="38"/>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="31" t="s">
@@ -4385,26 +4393,26 @@
       <c r="F19" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="74" t="s">
+      <c r="G19" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H19" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I19" s="76">
+      <c r="I19" s="75">
         <v>298</v>
       </c>
       <c r="J19" s="62">
         <v>3000000000</v>
       </c>
       <c r="K19" s="38"/>
-      <c r="L19" s="74" t="s">
+      <c r="L19" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M19" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N19" s="78" t="s">
+      <c r="N19" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O19" s="37"/>
@@ -4416,13 +4424,13 @@
     </row>
     <row r="20" spans="1:20" ht="18.75" customHeight="1">
       <c r="A20" s="38"/>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E20" s="31" t="s">
@@ -4431,26 +4439,26 @@
       <c r="F20" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="74" t="s">
+      <c r="G20" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="76">
+      <c r="I20" s="75">
         <v>298</v>
       </c>
       <c r="J20" s="62">
         <v>2846000000</v>
       </c>
       <c r="K20" s="38"/>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="73" t="s">
         <v>33</v>
       </c>
       <c r="M20" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N20" s="78" t="s">
+      <c r="N20" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O20" s="37"/>
@@ -4462,13 +4470,13 @@
     </row>
     <row r="21" spans="1:20" ht="18.75" customHeight="1">
       <c r="A21" s="38"/>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E21" s="31" t="s">
@@ -4477,26 +4485,26 @@
       <c r="F21" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="74" t="s">
+      <c r="G21" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H21" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="76">
+      <c r="I21" s="75">
         <v>298</v>
       </c>
       <c r="J21" s="62">
         <v>23.5</v>
       </c>
       <c r="K21" s="38"/>
-      <c r="L21" s="74" t="s">
+      <c r="L21" s="73" t="s">
         <v>67</v>
       </c>
       <c r="M21" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N21" s="78" t="s">
+      <c r="N21" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O21" s="37"/>
@@ -4508,13 +4516,13 @@
     </row>
     <row r="22" spans="1:20" ht="18.75" customHeight="1">
       <c r="A22" s="38"/>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="73" t="s">
+      <c r="D22" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E22" s="31" t="s">
@@ -4523,26 +4531,26 @@
       <c r="F22" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="74" t="s">
+      <c r="G22" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H22" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="76">
+      <c r="I22" s="75">
         <v>298</v>
       </c>
       <c r="J22" s="37">
         <v>31</v>
       </c>
       <c r="K22" s="35"/>
-      <c r="L22" s="74" t="s">
+      <c r="L22" s="73" t="s">
         <v>67</v>
       </c>
       <c r="M22" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N22" s="78" t="s">
+      <c r="N22" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O22" s="37"/>
@@ -4554,13 +4562,13 @@
     </row>
     <row r="23" spans="1:20" ht="18.75" customHeight="1">
       <c r="A23" s="30"/>
-      <c r="B23" s="72" t="s">
+      <c r="B23" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="D23" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="31" t="s">
@@ -4569,26 +4577,26 @@
       <c r="F23" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="74" t="s">
+      <c r="G23" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I23" s="76">
+      <c r="I23" s="75">
         <v>298</v>
       </c>
       <c r="J23" s="62">
         <v>32</v>
       </c>
       <c r="K23" s="62"/>
-      <c r="L23" s="74" t="s">
+      <c r="L23" s="73" t="s">
         <v>67</v>
       </c>
       <c r="M23" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N23" s="78" t="s">
+      <c r="N23" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O23" s="37"/>
@@ -4600,13 +4608,13 @@
     </row>
     <row r="24" spans="1:20" ht="18.75" customHeight="1">
       <c r="A24" s="30"/>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="73" t="s">
+      <c r="D24" s="72" t="s">
         <v>63</v>
       </c>
       <c r="E24" s="31" t="s">
@@ -4615,26 +4623,26 @@
       <c r="F24" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="74" t="s">
+      <c r="G24" s="73" t="s">
         <v>29</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="I24" s="76">
+      <c r="I24" s="75">
         <v>298</v>
       </c>
       <c r="J24" s="62">
         <v>34.5</v>
       </c>
       <c r="K24" s="62"/>
-      <c r="L24" s="74" t="s">
+      <c r="L24" s="73" t="s">
         <v>67</v>
       </c>
       <c r="M24" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="N24" s="78" t="s">
+      <c r="N24" s="77" t="s">
         <v>112</v>
       </c>
       <c r="O24" s="37"/>
@@ -4645,10 +4653,10 @@
       <c r="T24" s="37"/>
     </row>
     <row r="25" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="97" t="s">
         <v>121</v>
       </c>
       <c r="C25" s="30" t="s">
@@ -4821,10 +4829,10 @@
       <c r="T28" s="37"/>
     </row>
     <row r="29" spans="1:20" ht="18.75" customHeight="1">
-      <c r="A29" s="97" t="s">
+      <c r="A29" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="97" t="s">
         <v>121</v>
       </c>
       <c r="C29" s="30" t="s">
@@ -5378,7 +5386,7 @@
         <v>131</v>
       </c>
       <c r="I41" s="34"/>
-      <c r="J41" s="94">
+      <c r="J41" s="93">
         <v>120</v>
       </c>
       <c r="K41" s="47"/>
@@ -5418,7 +5426,7 @@
         <v>131</v>
       </c>
       <c r="I42" s="34"/>
-      <c r="J42" s="94">
+      <c r="J42" s="93">
         <v>12</v>
       </c>
       <c r="K42" s="47"/>
@@ -5458,7 +5466,7 @@
         <v>131</v>
       </c>
       <c r="I43" s="34"/>
-      <c r="J43" s="94">
+      <c r="J43" s="93">
         <v>33.6</v>
       </c>
       <c r="K43" s="47"/>
@@ -5498,7 +5506,7 @@
         <v>131</v>
       </c>
       <c r="I44" s="34"/>
-      <c r="J44" s="94">
+      <c r="J44" s="93">
         <v>55</v>
       </c>
       <c r="K44" s="49"/>
@@ -5506,7 +5514,7 @@
         <v>125</v>
       </c>
       <c r="M44" s="40"/>
-      <c r="N44" s="99" t="s">
+      <c r="N44" s="98" t="s">
         <v>144</v>
       </c>
       <c r="O44" s="46"/>
@@ -5546,7 +5554,7 @@
         <v>125</v>
       </c>
       <c r="M45" s="40"/>
-      <c r="N45" s="99" t="s">
+      <c r="N45" s="98" t="s">
         <v>145</v>
       </c>
       <c r="O45" s="46"/>
@@ -5662,7 +5670,7 @@
         <v>131</v>
       </c>
       <c r="I48" s="34"/>
-      <c r="J48" s="94">
+      <c r="J48" s="93">
         <v>5.9</v>
       </c>
       <c r="K48" s="47"/>
@@ -5702,7 +5710,7 @@
         <v>131</v>
       </c>
       <c r="I49" s="34"/>
-      <c r="J49" s="94">
+      <c r="J49" s="93">
         <v>11.9</v>
       </c>
       <c r="K49" s="47"/>
@@ -5742,7 +5750,7 @@
         <v>131</v>
       </c>
       <c r="I50" s="34"/>
-      <c r="J50" s="94">
+      <c r="J50" s="93">
         <v>8.6999999999999993</v>
       </c>
       <c r="K50" s="47"/>
@@ -5782,7 +5790,7 @@
         <v>131</v>
       </c>
       <c r="I51" s="34"/>
-      <c r="J51" s="94">
+      <c r="J51" s="93">
         <v>5.0999999999999996</v>
       </c>
       <c r="K51" s="49"/>
@@ -5790,7 +5798,7 @@
         <v>128</v>
       </c>
       <c r="M51" s="40"/>
-      <c r="N51" s="99" t="s">
+      <c r="N51" s="98" t="s">
         <v>144</v>
       </c>
       <c r="O51" s="46"/>
@@ -5830,7 +5838,7 @@
         <v>128</v>
       </c>
       <c r="M52" s="40"/>
-      <c r="N52" s="99" t="s">
+      <c r="N52" s="98" t="s">
         <v>145</v>
       </c>
       <c r="O52" s="46"/>
@@ -6436,7 +6444,7 @@
         <v>131</v>
       </c>
       <c r="I66" s="34"/>
-      <c r="J66" s="94">
+      <c r="J66" s="93">
         <v>48.5</v>
       </c>
       <c r="K66" s="47"/>
@@ -6568,11 +6576,11 @@
       <c r="I69" s="34">
         <v>298</v>
       </c>
-      <c r="J69" s="100">
+      <c r="J69" s="99">
         <f t="shared" ref="J69:J76" si="0">P69*9807000</f>
         <v>5122230164.5338182</v>
       </c>
-      <c r="K69" s="100">
+      <c r="K69" s="99">
         <f>(Q69-P69)*9807000</f>
         <v>338852468.0073154</v>
       </c>
@@ -6620,11 +6628,11 @@
       <c r="I70" s="34">
         <v>298</v>
       </c>
-      <c r="J70" s="100">
+      <c r="J70" s="99">
         <f t="shared" si="0"/>
         <v>6038386837.2943306</v>
       </c>
-      <c r="K70" s="100">
+      <c r="K70" s="99">
         <f t="shared" ref="K70:K76" si="1">(Q70-P70)*9807000</f>
         <v>338852468.0073154</v>
       </c>
@@ -6672,11 +6680,11 @@
       <c r="I71" s="34">
         <v>298</v>
       </c>
-      <c r="J71" s="100">
+      <c r="J71" s="99">
         <f t="shared" si="0"/>
         <v>6690991590.4935989</v>
       </c>
-      <c r="K71" s="100">
+      <c r="K71" s="99">
         <f t="shared" si="1"/>
         <v>288652102.37659782</v>
       </c>
@@ -6724,11 +6732,11 @@
       <c r="I72" s="34">
         <v>298</v>
       </c>
-      <c r="J72" s="100">
+      <c r="J72" s="99">
         <f t="shared" si="0"/>
         <v>6929443327.2394876</v>
       </c>
-      <c r="K72" s="100">
+      <c r="K72" s="99">
         <f t="shared" si="1"/>
         <v>376502742.23034215</v>
       </c>
@@ -6776,11 +6784,11 @@
       <c r="I73" s="34">
         <v>298</v>
       </c>
-      <c r="J73" s="100">
+      <c r="J73" s="99">
         <f t="shared" si="0"/>
         <v>4370646088.794919</v>
       </c>
-      <c r="K73" s="100">
+      <c r="K73" s="99">
         <f t="shared" si="1"/>
         <v>362838266.38477683</v>
       </c>
@@ -6828,11 +6836,11 @@
       <c r="I74" s="34">
         <v>298</v>
       </c>
-      <c r="J74" s="100">
+      <c r="J74" s="99">
         <f t="shared" si="0"/>
         <v>5417693657.5052862</v>
       </c>
-      <c r="K74" s="100">
+      <c r="K74" s="99">
         <f t="shared" si="1"/>
         <v>269536997.88582945</v>
       </c>
@@ -6880,11 +6888,11 @@
       <c r="I75" s="34">
         <v>298</v>
       </c>
-      <c r="J75" s="100">
+      <c r="J75" s="99">
         <f t="shared" si="0"/>
         <v>5127423044.3974543</v>
       </c>
-      <c r="K75" s="100">
+      <c r="K75" s="99">
         <f t="shared" si="1"/>
         <v>342104651.16279542</v>
       </c>
@@ -6932,11 +6940,11 @@
       <c r="I76" s="34">
         <v>298</v>
       </c>
-      <c r="J76" s="100">
+      <c r="J76" s="99">
         <f t="shared" si="0"/>
         <v>5013388160.6765261</v>
       </c>
-      <c r="K76" s="100">
+      <c r="K76" s="99">
         <f t="shared" si="1"/>
         <v>238436575.05285701</v>
       </c>
@@ -6984,7 +6992,7 @@
       <c r="I77" s="34">
         <v>298</v>
       </c>
-      <c r="J77" s="94">
+      <c r="J77" s="93">
         <v>383000000</v>
       </c>
       <c r="K77" s="47"/>
@@ -7028,7 +7036,7 @@
       <c r="I78" s="34">
         <v>298</v>
       </c>
-      <c r="J78" s="94">
+      <c r="J78" s="93">
         <v>321000000</v>
       </c>
       <c r="K78" s="47"/>
@@ -7498,7 +7506,7 @@
       <c r="I89" s="34">
         <v>298</v>
       </c>
-      <c r="J89" s="94">
+      <c r="J89" s="93">
         <v>356000000</v>
       </c>
       <c r="K89" s="49"/>
@@ -7538,7 +7546,7 @@
       <c r="I90" s="34">
         <v>298</v>
       </c>
-      <c r="J90" s="94">
+      <c r="J90" s="93">
         <v>536000000</v>
       </c>
       <c r="K90" s="49"/>
@@ -7578,7 +7586,7 @@
       <c r="I91" s="34">
         <v>298</v>
       </c>
-      <c r="J91" s="94">
+      <c r="J91" s="93">
         <v>29.1</v>
       </c>
       <c r="K91" s="49"/>
@@ -7618,7 +7626,7 @@
       <c r="I92" s="34">
         <v>298</v>
       </c>
-      <c r="J92" s="100">
+      <c r="J92" s="99">
         <f t="shared" ref="J92" si="2">P92*9807000</f>
         <v>1765260000</v>
       </c>
@@ -8520,11 +8528,11 @@
       <c r="I114" s="38">
         <v>298</v>
       </c>
-      <c r="J114" s="100">
+      <c r="J114" s="99">
         <f t="shared" ref="J114:K116" si="4">P114*9807000</f>
         <v>4776009000</v>
       </c>
-      <c r="K114" s="100">
+      <c r="K114" s="99">
         <f t="shared" si="4"/>
         <v>176526000</v>
       </c>
@@ -8574,11 +8582,11 @@
       <c r="I115" s="38">
         <v>298</v>
       </c>
-      <c r="J115" s="100">
+      <c r="J115" s="99">
         <f t="shared" si="4"/>
         <v>5511534000</v>
       </c>
-      <c r="K115" s="100">
+      <c r="K115" s="99">
         <f t="shared" si="4"/>
         <v>196140000</v>
       </c>
@@ -8628,11 +8636,11 @@
       <c r="I116" s="38">
         <v>298</v>
       </c>
-      <c r="J116" s="100">
+      <c r="J116" s="99">
         <f t="shared" si="4"/>
         <v>6619725000</v>
       </c>
-      <c r="K116" s="100">
+      <c r="K116" s="99">
         <f t="shared" si="4"/>
         <v>460929000</v>
       </c>
@@ -9078,10 +9086,10 @@
     </row>
     <row r="127" spans="1:20" ht="18" customHeight="1">
       <c r="A127" s="51"/>
-      <c r="B127" s="95" t="s">
+      <c r="B127" s="94" t="s">
         <v>204</v>
       </c>
-      <c r="C127" s="101" t="s">
+      <c r="C127" s="100" t="s">
         <v>74</v>
       </c>
       <c r="D127" s="30" t="s">
@@ -9122,10 +9130,10 @@
     </row>
     <row r="128" spans="1:20" ht="18" customHeight="1">
       <c r="A128" s="30"/>
-      <c r="B128" s="96" t="s">
+      <c r="B128" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="C128" s="102" t="s">
+      <c r="C128" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D128" s="30" t="s">
@@ -9166,10 +9174,10 @@
     </row>
     <row r="129" spans="1:20" ht="18" customHeight="1">
       <c r="A129" s="30"/>
-      <c r="B129" s="96" t="s">
+      <c r="B129" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="C129" s="102" t="s">
+      <c r="C129" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D129" s="30" t="s">
@@ -9210,10 +9218,10 @@
     </row>
     <row r="130" spans="1:20" ht="18" customHeight="1">
       <c r="A130" s="30"/>
-      <c r="B130" s="96" t="s">
+      <c r="B130" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="C130" s="102" t="s">
+      <c r="C130" s="101" t="s">
         <v>75</v>
       </c>
       <c r="D130" s="30" t="s">
@@ -9254,10 +9262,10 @@
     </row>
     <row r="131" spans="1:20" ht="18" customHeight="1">
       <c r="A131" s="30"/>
-      <c r="B131" s="96" t="s">
+      <c r="B131" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="C131" s="102" t="s">
+      <c r="C131" s="101" t="s">
         <v>64</v>
       </c>
       <c r="D131" s="30" t="s">
@@ -9298,10 +9306,10 @@
     </row>
     <row r="132" spans="1:20" ht="18" customHeight="1">
       <c r="A132" s="51"/>
-      <c r="B132" s="95" t="s">
+      <c r="B132" s="94" t="s">
         <v>204</v>
       </c>
-      <c r="C132" s="101" t="s">
+      <c r="C132" s="100" t="s">
         <v>74</v>
       </c>
       <c r="D132" s="30" t="s">
@@ -9342,10 +9350,10 @@
     </row>
     <row r="133" spans="1:20" ht="18" customHeight="1">
       <c r="A133" s="30"/>
-      <c r="B133" s="96" t="s">
+      <c r="B133" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="C133" s="102" t="s">
+      <c r="C133" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D133" s="30" t="s">
@@ -9386,10 +9394,10 @@
     </row>
     <row r="134" spans="1:20" ht="18" customHeight="1">
       <c r="A134" s="30"/>
-      <c r="B134" s="96" t="s">
+      <c r="B134" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="C134" s="102" t="s">
+      <c r="C134" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D134" s="30" t="s">
@@ -9430,10 +9438,10 @@
     </row>
     <row r="135" spans="1:20" ht="18" customHeight="1">
       <c r="A135" s="30"/>
-      <c r="B135" s="96" t="s">
+      <c r="B135" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="C135" s="102" t="s">
+      <c r="C135" s="101" t="s">
         <v>75</v>
       </c>
       <c r="D135" s="30" t="s">
@@ -9474,10 +9482,10 @@
     </row>
     <row r="136" spans="1:20" ht="18" customHeight="1">
       <c r="A136" s="30"/>
-      <c r="B136" s="96" t="s">
+      <c r="B136" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="C136" s="102" t="s">
+      <c r="C136" s="101" t="s">
         <v>64</v>
       </c>
       <c r="D136" s="30" t="s">
@@ -9518,10 +9526,10 @@
     </row>
     <row r="137" spans="1:20" ht="18" customHeight="1">
       <c r="A137" s="55"/>
-      <c r="B137" s="95" t="s">
+      <c r="B137" s="94" t="s">
         <v>204</v>
       </c>
-      <c r="C137" s="101" t="s">
+      <c r="C137" s="100" t="s">
         <v>74</v>
       </c>
       <c r="D137" s="30" t="s">
@@ -9562,10 +9570,10 @@
     </row>
     <row r="138" spans="1:20" ht="18" customHeight="1">
       <c r="A138" s="42"/>
-      <c r="B138" s="96" t="s">
+      <c r="B138" s="95" t="s">
         <v>205</v>
       </c>
-      <c r="C138" s="102" t="s">
+      <c r="C138" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D138" s="30" t="s">
@@ -9606,10 +9614,10 @@
     </row>
     <row r="139" spans="1:20" ht="18" customHeight="1">
       <c r="A139" s="42"/>
-      <c r="B139" s="96" t="s">
+      <c r="B139" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="C139" s="102" t="s">
+      <c r="C139" s="101" t="s">
         <v>74</v>
       </c>
       <c r="D139" s="30" t="s">
@@ -9650,10 +9658,10 @@
     </row>
     <row r="140" spans="1:20" ht="18" customHeight="1">
       <c r="A140" s="42"/>
-      <c r="B140" s="96" t="s">
+      <c r="B140" s="95" t="s">
         <v>207</v>
       </c>
-      <c r="C140" s="102" t="s">
+      <c r="C140" s="101" t="s">
         <v>75</v>
       </c>
       <c r="D140" s="30" t="s">
@@ -9694,10 +9702,10 @@
     </row>
     <row r="141" spans="1:20" ht="18" customHeight="1">
       <c r="A141" s="42"/>
-      <c r="B141" s="96" t="s">
+      <c r="B141" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="C141" s="102" t="s">
+      <c r="C141" s="101" t="s">
         <v>64</v>
       </c>
       <c r="D141" s="30" t="s">
@@ -9738,10 +9746,10 @@
     </row>
     <row r="142" spans="1:20" ht="18" customHeight="1">
       <c r="A142" s="55"/>
-      <c r="B142" s="96" t="s">
+      <c r="B142" s="95" t="s">
         <v>208</v>
       </c>
-      <c r="C142" s="102" t="s">
+      <c r="C142" s="101" t="s">
         <v>64</v>
       </c>
       <c r="D142" s="30" t="s">
@@ -9782,7 +9790,7 @@
     </row>
     <row r="143" spans="1:20" ht="18" customHeight="1">
       <c r="A143" s="42"/>
-      <c r="B143" s="96" t="s">
+      <c r="B143" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C143" s="30" t="s">
@@ -9823,7 +9831,7 @@
     </row>
     <row r="144" spans="1:20" ht="18" customHeight="1">
       <c r="A144" s="42"/>
-      <c r="B144" s="96" t="s">
+      <c r="B144" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C144" s="30" t="s">
@@ -9867,7 +9875,7 @@
     </row>
     <row r="145" spans="1:20" ht="18" customHeight="1">
       <c r="A145" s="42"/>
-      <c r="B145" s="96" t="s">
+      <c r="B145" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C145" s="30" t="s">
@@ -9911,7 +9919,7 @@
     </row>
     <row r="146" spans="1:20" ht="18" customHeight="1">
       <c r="A146" s="42"/>
-      <c r="B146" s="96" t="s">
+      <c r="B146" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C146" s="30" t="s">
@@ -9955,7 +9963,7 @@
     </row>
     <row r="147" spans="1:20" ht="18" customHeight="1">
       <c r="A147" s="55"/>
-      <c r="B147" s="96" t="s">
+      <c r="B147" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C147" s="30" t="s">
@@ -9999,7 +10007,7 @@
     </row>
     <row r="148" spans="1:20" ht="18" customHeight="1">
       <c r="A148" s="42"/>
-      <c r="B148" s="96" t="s">
+      <c r="B148" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C148" s="30" t="s">
@@ -10043,7 +10051,7 @@
     </row>
     <row r="149" spans="1:20" ht="18" customHeight="1">
       <c r="A149" s="42"/>
-      <c r="B149" s="96" t="s">
+      <c r="B149" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C149" s="30" t="s">
@@ -10087,7 +10095,7 @@
     </row>
     <row r="150" spans="1:20" ht="18" customHeight="1">
       <c r="A150" s="42"/>
-      <c r="B150" s="96" t="s">
+      <c r="B150" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C150" s="30" t="s">
@@ -10131,7 +10139,7 @@
     </row>
     <row r="151" spans="1:20" ht="18" customHeight="1">
       <c r="A151" s="42"/>
-      <c r="B151" s="96" t="s">
+      <c r="B151" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C151" s="30" t="s">
@@ -10175,7 +10183,7 @@
     </row>
     <row r="152" spans="1:20" ht="18" customHeight="1">
       <c r="A152" s="55"/>
-      <c r="B152" s="96" t="s">
+      <c r="B152" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C152" s="30" t="s">
@@ -10221,7 +10229,7 @@
     </row>
     <row r="153" spans="1:20" ht="18" customHeight="1">
       <c r="A153" s="42"/>
-      <c r="B153" s="96" t="s">
+      <c r="B153" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C153" s="30" t="s">
@@ -10267,7 +10275,7 @@
     </row>
     <row r="154" spans="1:20" ht="18" customHeight="1">
       <c r="A154" s="42"/>
-      <c r="B154" s="96" t="s">
+      <c r="B154" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C154" s="30" t="s">
@@ -10313,7 +10321,7 @@
     </row>
     <row r="155" spans="1:20" ht="18" customHeight="1">
       <c r="A155" s="42"/>
-      <c r="B155" s="96" t="s">
+      <c r="B155" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C155" s="30" t="s">
@@ -10359,7 +10367,7 @@
     </row>
     <row r="156" spans="1:20" ht="18" customHeight="1">
       <c r="A156" s="42"/>
-      <c r="B156" s="96" t="s">
+      <c r="B156" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C156" s="30" t="s">
@@ -10405,7 +10413,7 @@
     </row>
     <row r="157" spans="1:20" ht="18" customHeight="1">
       <c r="A157" s="30"/>
-      <c r="B157" s="96" t="s">
+      <c r="B157" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C157" s="30" t="s">
@@ -10451,7 +10459,7 @@
     </row>
     <row r="158" spans="1:20" ht="18" customHeight="1">
       <c r="A158" s="38"/>
-      <c r="B158" s="96" t="s">
+      <c r="B158" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C158" s="30" t="s">
@@ -10497,7 +10505,7 @@
     </row>
     <row r="159" spans="1:20" ht="18" customHeight="1">
       <c r="A159" s="38"/>
-      <c r="B159" s="96" t="s">
+      <c r="B159" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C159" s="30" t="s">
@@ -10543,7 +10551,7 @@
     </row>
     <row r="160" spans="1:20" ht="18" customHeight="1">
       <c r="A160" s="38"/>
-      <c r="B160" s="96" t="s">
+      <c r="B160" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C160" s="30" t="s">
@@ -10589,7 +10597,7 @@
     </row>
     <row r="161" spans="1:20" ht="18" customHeight="1">
       <c r="A161" s="38"/>
-      <c r="B161" s="96" t="s">
+      <c r="B161" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C161" s="30" t="s">
@@ -10635,7 +10643,7 @@
     </row>
     <row r="162" spans="1:20" ht="18" customHeight="1">
       <c r="A162" s="38"/>
-      <c r="B162" s="96" t="s">
+      <c r="B162" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C162" s="30" t="s">
@@ -10681,7 +10689,7 @@
     </row>
     <row r="163" spans="1:20" ht="18" customHeight="1">
       <c r="A163" s="38"/>
-      <c r="B163" s="96" t="s">
+      <c r="B163" s="95" t="s">
         <v>205</v>
       </c>
       <c r="C163" s="30" t="s">
@@ -13175,7 +13183,7 @@
       <c r="I215" s="38">
         <v>298</v>
       </c>
-      <c r="J215" s="100">
+      <c r="J215" s="99">
         <f t="shared" ref="J215:J221" si="9">P215*9807000</f>
         <v>1372652006.6889586</v>
       </c>
@@ -13224,7 +13232,7 @@
       <c r="I216" s="38">
         <v>298</v>
       </c>
-      <c r="J216" s="100">
+      <c r="J216" s="99">
         <f t="shared" si="9"/>
         <v>2986379096.9899654</v>
       </c>
@@ -13273,7 +13281,7 @@
       <c r="I217" s="38">
         <v>298</v>
       </c>
-      <c r="J217" s="100">
+      <c r="J217" s="99">
         <f t="shared" si="9"/>
         <v>5033057357.8595304</v>
       </c>
@@ -13322,7 +13330,7 @@
       <c r="I218" s="38">
         <v>298</v>
       </c>
-      <c r="J218" s="100">
+      <c r="J218" s="99">
         <f t="shared" si="9"/>
         <v>4993698160.5351105</v>
       </c>
@@ -13371,7 +13379,7 @@
       <c r="I219" s="38">
         <v>298</v>
       </c>
-      <c r="J219" s="100">
+      <c r="J219" s="99">
         <f t="shared" si="9"/>
         <v>5859600501.6722345</v>
       </c>
@@ -13420,7 +13428,7 @@
       <c r="I220" s="38">
         <v>298</v>
       </c>
-      <c r="J220" s="100">
+      <c r="J220" s="99">
         <f t="shared" si="9"/>
         <v>5879280100.334445</v>
       </c>
@@ -13469,7 +13477,7 @@
       <c r="I221" s="38">
         <v>298</v>
       </c>
-      <c r="J221" s="100">
+      <c r="J221" s="99">
         <f t="shared" si="9"/>
         <v>8024356354.5150414</v>
       </c>
@@ -14499,7 +14507,7 @@
       <c r="B243" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C243" s="103" t="s">
+      <c r="C243" s="102" t="s">
         <v>93</v>
       </c>
       <c r="D243" s="61" t="s">
@@ -14547,7 +14555,7 @@
       <c r="B244" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C244" s="103" t="s">
+      <c r="C244" s="102" t="s">
         <v>248</v>
       </c>
       <c r="D244" s="61" t="s">
@@ -14595,7 +14603,7 @@
       <c r="B245" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C245" s="103" t="s">
+      <c r="C245" s="102" t="s">
         <v>93</v>
       </c>
       <c r="D245" s="61" t="s">
@@ -14643,7 +14651,7 @@
       <c r="B246" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C246" s="103" t="s">
+      <c r="C246" s="102" t="s">
         <v>248</v>
       </c>
       <c r="D246" s="61" t="s">
@@ -14691,7 +14699,7 @@
       <c r="B247" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="C247" s="103" t="s">
+      <c r="C247" s="102" t="s">
         <v>93</v>
       </c>
       <c r="D247" s="61" t="s">
@@ -14739,7 +14747,7 @@
       <c r="B248" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="C248" s="103" t="s">
+      <c r="C248" s="102" t="s">
         <v>248</v>
       </c>
       <c r="D248" s="61" t="s">
@@ -14785,7 +14793,7 @@
       <c r="B249" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C249" s="103" t="s">
+      <c r="C249" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D249" s="61" t="s">
@@ -14829,7 +14837,7 @@
       <c r="B250" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C250" s="103" t="s">
+      <c r="C250" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D250" s="61"/>
@@ -14869,7 +14877,7 @@
       <c r="B251" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C251" s="103" t="s">
+      <c r="C251" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D251" s="61" t="s">
@@ -14913,7 +14921,7 @@
       <c r="B252" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C252" s="103" t="s">
+      <c r="C252" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D252" s="61"/>
@@ -14953,7 +14961,7 @@
       <c r="B253" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C253" s="103" t="s">
+      <c r="C253" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D253" s="61" t="s">
@@ -14997,7 +15005,7 @@
       <c r="B254" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C254" s="103" t="s">
+      <c r="C254" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D254" s="61"/>
@@ -15037,7 +15045,7 @@
       <c r="B255" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C255" s="103" t="s">
+      <c r="C255" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D255" s="61" t="s">
@@ -15079,7 +15087,7 @@
       <c r="B256" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C256" s="103" t="s">
+      <c r="C256" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D256" s="61"/>
@@ -15117,7 +15125,7 @@
       <c r="B257" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C257" s="103" t="s">
+      <c r="C257" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D257" s="61" t="s">
@@ -15158,7 +15166,7 @@
       <c r="B258" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="C258" s="103" t="s">
+      <c r="C258" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D258" s="61"/>
@@ -16063,7 +16071,7 @@
       <c r="N276" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="O276" s="104"/>
+      <c r="O276" s="103"/>
       <c r="P276" s="45">
         <v>164.444444444444</v>
       </c>
@@ -22280,28 +22288,28 @@
     </row>
     <row r="410" spans="1:20" ht="18" customHeight="1">
       <c r="A410" s="45"/>
-      <c r="B410" s="142" t="s">
+      <c r="B410" s="141" t="s">
         <v>308</v>
       </c>
-      <c r="C410" s="143" t="s">
+      <c r="C410" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="D410" s="143" t="s">
+      <c r="D410" s="142" t="s">
         <v>312</v>
       </c>
-      <c r="E410" s="143" t="s">
+      <c r="E410" s="142" t="s">
         <v>313</v>
       </c>
-      <c r="F410" s="143" t="s">
+      <c r="F410" s="142" t="s">
         <v>324</v>
       </c>
-      <c r="G410" s="143" t="s">
-        <v>29</v>
-      </c>
-      <c r="H410" s="143" t="s">
+      <c r="G410" s="142" t="s">
+        <v>29</v>
+      </c>
+      <c r="H410" s="142" t="s">
         <v>315</v>
       </c>
-      <c r="I410" s="143">
+      <c r="I410" s="142">
         <v>298</v>
       </c>
       <c r="J410" s="45">
@@ -22334,28 +22342,28 @@
     </row>
     <row r="411" spans="1:20" ht="18" customHeight="1">
       <c r="A411" s="45"/>
-      <c r="B411" s="144" t="s">
+      <c r="B411" s="143" t="s">
         <v>309</v>
       </c>
-      <c r="C411" s="145" t="s">
+      <c r="C411" s="144" t="s">
         <v>74</v>
       </c>
-      <c r="D411" s="145" t="s">
+      <c r="D411" s="144" t="s">
         <v>312</v>
       </c>
-      <c r="E411" s="145" t="s">
+      <c r="E411" s="144" t="s">
         <v>313</v>
       </c>
-      <c r="F411" s="143" t="s">
+      <c r="F411" s="142" t="s">
         <v>324</v>
       </c>
-      <c r="G411" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H411" s="145" t="s">
+      <c r="G411" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H411" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I411" s="145">
+      <c r="I411" s="144">
         <v>298</v>
       </c>
       <c r="J411" s="45">
@@ -22388,28 +22396,28 @@
     </row>
     <row r="412" spans="1:20" ht="18" customHeight="1">
       <c r="A412" s="45"/>
-      <c r="B412" s="144" t="s">
+      <c r="B412" s="143" t="s">
         <v>310</v>
       </c>
-      <c r="C412" s="145" t="s">
+      <c r="C412" s="144" t="s">
         <v>74</v>
       </c>
-      <c r="D412" s="145" t="s">
+      <c r="D412" s="144" t="s">
         <v>312</v>
       </c>
-      <c r="E412" s="145" t="s">
+      <c r="E412" s="144" t="s">
         <v>313</v>
       </c>
-      <c r="F412" s="143" t="s">
+      <c r="F412" s="142" t="s">
         <v>324</v>
       </c>
-      <c r="G412" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H412" s="145" t="s">
+      <c r="G412" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H412" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I412" s="145">
+      <c r="I412" s="144">
         <v>298</v>
       </c>
       <c r="J412" s="45">
@@ -22442,28 +22450,28 @@
     </row>
     <row r="413" spans="1:20" ht="18" customHeight="1">
       <c r="A413" s="45"/>
-      <c r="B413" s="144" t="s">
+      <c r="B413" s="143" t="s">
         <v>311</v>
       </c>
-      <c r="C413" s="145" t="s">
+      <c r="C413" s="144" t="s">
         <v>74</v>
       </c>
-      <c r="D413" s="145" t="s">
+      <c r="D413" s="144" t="s">
         <v>312</v>
       </c>
-      <c r="E413" s="145" t="s">
+      <c r="E413" s="144" t="s">
         <v>313</v>
       </c>
-      <c r="F413" s="143" t="s">
+      <c r="F413" s="142" t="s">
         <v>324</v>
       </c>
-      <c r="G413" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H413" s="145" t="s">
+      <c r="G413" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H413" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I413" s="145">
+      <c r="I413" s="144">
         <v>298</v>
       </c>
       <c r="J413" s="45">
@@ -22509,13 +22517,13 @@
       <c r="F414" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="G414" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H414" s="145" t="s">
+      <c r="G414" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H414" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I414" s="145">
+      <c r="I414" s="144">
         <v>298</v>
       </c>
       <c r="J414" s="62">
@@ -22553,13 +22561,13 @@
       <c r="F415" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="G415" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H415" s="145" t="s">
+      <c r="G415" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H415" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I415" s="145">
+      <c r="I415" s="144">
         <v>298</v>
       </c>
       <c r="J415" s="62">
@@ -22597,13 +22605,13 @@
       <c r="F416" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="G416" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H416" s="145" t="s">
+      <c r="G416" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H416" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I416" s="145">
+      <c r="I416" s="144">
         <v>298</v>
       </c>
       <c r="J416" s="62">
@@ -22641,13 +22649,13 @@
       <c r="F417" s="61" t="s">
         <v>324</v>
       </c>
-      <c r="G417" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H417" s="145" t="s">
+      <c r="G417" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H417" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I417" s="145">
+      <c r="I417" s="144">
         <v>298</v>
       </c>
       <c r="J417" s="62">
@@ -22685,13 +22693,13 @@
       <c r="F418" s="61" t="s">
         <v>324</v>
       </c>
-      <c r="G418" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H418" s="145" t="s">
+      <c r="G418" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H418" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I418" s="145">
+      <c r="I418" s="144">
         <v>298</v>
       </c>
       <c r="J418" s="62">
@@ -22729,13 +22737,13 @@
       <c r="F419" s="61" t="s">
         <v>324</v>
       </c>
-      <c r="G419" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H419" s="145" t="s">
+      <c r="G419" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H419" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I419" s="145">
+      <c r="I419" s="144">
         <v>298</v>
       </c>
       <c r="J419" s="62">
@@ -22760,26 +22768,26 @@
     </row>
     <row r="420" spans="1:20" ht="18" customHeight="1">
       <c r="A420" s="61"/>
-      <c r="B420" s="142" t="s">
+      <c r="B420" s="141" t="s">
         <v>317</v>
       </c>
-      <c r="C420" s="143" t="s">
+      <c r="C420" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="D420" s="143" t="s">
+      <c r="D420" s="142" t="s">
         <v>63</v>
       </c>
       <c r="E420" s="61"/>
       <c r="F420" s="61" t="s">
         <v>325</v>
       </c>
-      <c r="G420" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H420" s="145" t="s">
+      <c r="G420" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H420" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I420" s="145">
+      <c r="I420" s="144">
         <v>298</v>
       </c>
       <c r="J420" s="62">
@@ -22804,26 +22812,26 @@
     </row>
     <row r="421" spans="1:20" ht="18" customHeight="1">
       <c r="A421" s="61"/>
-      <c r="B421" s="144" t="s">
+      <c r="B421" s="143" t="s">
         <v>318</v>
       </c>
-      <c r="C421" s="145" t="s">
+      <c r="C421" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="D421" s="145" t="s">
+      <c r="D421" s="144" t="s">
         <v>63</v>
       </c>
       <c r="E421" s="61"/>
       <c r="F421" s="61" t="s">
         <v>325</v>
       </c>
-      <c r="G421" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H421" s="145" t="s">
+      <c r="G421" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H421" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I421" s="145">
+      <c r="I421" s="144">
         <v>298</v>
       </c>
       <c r="J421" s="62">
@@ -22848,26 +22856,26 @@
     </row>
     <row r="422" spans="1:20" ht="18" customHeight="1">
       <c r="A422" s="61"/>
-      <c r="B422" s="144" t="s">
+      <c r="B422" s="143" t="s">
         <v>319</v>
       </c>
-      <c r="C422" s="145" t="s">
+      <c r="C422" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="D422" s="145" t="s">
+      <c r="D422" s="144" t="s">
         <v>63</v>
       </c>
       <c r="E422" s="61"/>
       <c r="F422" s="61" t="s">
         <v>325</v>
       </c>
-      <c r="G422" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="H422" s="145" t="s">
+      <c r="G422" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H422" s="144" t="s">
         <v>315</v>
       </c>
-      <c r="I422" s="145">
+      <c r="I422" s="144">
         <v>298</v>
       </c>
       <c r="J422" s="62">
@@ -22892,19 +22900,41 @@
     </row>
     <row r="423" spans="1:20" ht="15" customHeight="1">
       <c r="A423" s="61"/>
-      <c r="B423" s="61"/>
-      <c r="C423" s="61"/>
-      <c r="D423" s="61"/>
+      <c r="B423" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C423" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D423" s="61" t="s">
+        <v>328</v>
+      </c>
       <c r="E423" s="61"/>
-      <c r="F423" s="61"/>
-      <c r="G423" s="61"/>
-      <c r="H423" s="45"/>
-      <c r="I423" s="45"/>
-      <c r="J423" s="62"/>
+      <c r="F423" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G423" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H423" s="144" t="s">
+        <v>315</v>
+      </c>
+      <c r="I423" s="144">
+        <v>298</v>
+      </c>
+      <c r="J423" s="62">
+        <v>-0.36</v>
+      </c>
       <c r="K423" s="45"/>
-      <c r="L423" s="61"/>
-      <c r="M423" s="61"/>
-      <c r="N423" s="61"/>
+      <c r="L423" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M423" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="N423" s="61" t="s">
+        <v>329</v>
+      </c>
       <c r="O423" s="45"/>
       <c r="P423" s="45"/>
       <c r="Q423" s="45"/>
@@ -22914,19 +22944,41 @@
     </row>
     <row r="424" spans="1:20" ht="15" customHeight="1">
       <c r="A424" s="61"/>
-      <c r="B424" s="45"/>
-      <c r="C424" s="61"/>
-      <c r="D424" s="61"/>
+      <c r="B424" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C424" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D424" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E424" s="61"/>
-      <c r="F424" s="61"/>
-      <c r="G424" s="61"/>
-      <c r="H424" s="45"/>
-      <c r="I424" s="45"/>
-      <c r="J424" s="62"/>
+      <c r="F424" s="61" t="s">
+        <v>323</v>
+      </c>
+      <c r="G424" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H424" s="144" t="s">
+        <v>315</v>
+      </c>
+      <c r="I424" s="144">
+        <v>298</v>
+      </c>
+      <c r="J424" s="62">
+        <v>-0.44</v>
+      </c>
       <c r="K424" s="45"/>
-      <c r="L424" s="61"/>
-      <c r="M424" s="61"/>
-      <c r="N424" s="61"/>
+      <c r="L424" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M424" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="N424" s="61" t="s">
+        <v>329</v>
+      </c>
       <c r="O424" s="45"/>
       <c r="P424" s="45"/>
       <c r="Q424" s="45"/>
@@ -22936,19 +22988,41 @@
     </row>
     <row r="425" spans="1:20" ht="15" customHeight="1">
       <c r="A425" s="61"/>
-      <c r="B425" s="45"/>
-      <c r="C425" s="63"/>
-      <c r="D425" s="61"/>
+      <c r="B425" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C425" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D425" s="61" t="s">
+        <v>328</v>
+      </c>
       <c r="E425" s="61"/>
-      <c r="F425" s="61"/>
-      <c r="G425" s="61"/>
-      <c r="H425" s="45"/>
-      <c r="I425" s="45"/>
-      <c r="J425" s="62"/>
+      <c r="F425" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="G425" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H425" s="144" t="s">
+        <v>315</v>
+      </c>
+      <c r="I425" s="144">
+        <v>298</v>
+      </c>
+      <c r="J425" s="62">
+        <v>2.4099999999999998E-3</v>
+      </c>
       <c r="K425" s="45"/>
-      <c r="L425" s="61"/>
-      <c r="M425" s="61"/>
-      <c r="N425" s="61"/>
+      <c r="L425" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="M425" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="N425" s="61" t="s">
+        <v>329</v>
+      </c>
       <c r="O425" s="45"/>
       <c r="P425" s="45"/>
       <c r="Q425" s="45"/>
@@ -22958,19 +23032,41 @@
     </row>
     <row r="426" spans="1:20" ht="15" customHeight="1">
       <c r="A426" s="61"/>
-      <c r="B426" s="45"/>
-      <c r="C426" s="61"/>
-      <c r="D426" s="61"/>
+      <c r="B426" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C426" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D426" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E426" s="61"/>
-      <c r="F426" s="61"/>
-      <c r="G426" s="61"/>
-      <c r="H426" s="45"/>
-      <c r="I426" s="45"/>
-      <c r="J426" s="45"/>
+      <c r="F426" s="61" t="s">
+        <v>325</v>
+      </c>
+      <c r="G426" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H426" s="144" t="s">
+        <v>315</v>
+      </c>
+      <c r="I426" s="144">
+        <v>298</v>
+      </c>
+      <c r="J426" s="62">
+        <v>0.19500000000000001</v>
+      </c>
       <c r="K426" s="45"/>
-      <c r="L426" s="61"/>
-      <c r="M426" s="61"/>
-      <c r="N426" s="61"/>
+      <c r="L426" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="M426" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="N426" s="61" t="s">
+        <v>329</v>
+      </c>
       <c r="O426" s="45"/>
       <c r="P426" s="45"/>
       <c r="Q426" s="45"/>
@@ -22980,19 +23076,41 @@
     </row>
     <row r="427" spans="1:20" ht="15" customHeight="1">
       <c r="A427" s="61"/>
-      <c r="B427" s="45"/>
-      <c r="C427" s="61"/>
-      <c r="D427" s="61"/>
+      <c r="B427" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C427" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D427" s="61" t="s">
+        <v>328</v>
+      </c>
       <c r="E427" s="61"/>
-      <c r="F427" s="61"/>
-      <c r="G427" s="61"/>
-      <c r="H427" s="45"/>
-      <c r="I427" s="45"/>
-      <c r="J427" s="45"/>
+      <c r="F427" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="G427" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H427" s="144" t="s">
+        <v>315</v>
+      </c>
+      <c r="I427" s="144">
+        <v>298</v>
+      </c>
+      <c r="J427" s="45">
+        <v>-0.01</v>
+      </c>
       <c r="K427" s="45"/>
-      <c r="L427" s="61"/>
-      <c r="M427" s="61"/>
-      <c r="N427" s="61"/>
+      <c r="L427" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M427" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="N427" s="61" t="s">
+        <v>329</v>
+      </c>
       <c r="O427" s="45"/>
       <c r="P427" s="45"/>
       <c r="Q427" s="45"/>
@@ -23002,19 +23120,41 @@
     </row>
     <row r="428" spans="1:20" ht="15" customHeight="1">
       <c r="A428" s="61"/>
-      <c r="B428" s="45"/>
-      <c r="C428" s="61"/>
-      <c r="D428" s="61"/>
+      <c r="B428" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C428" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D428" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="E428" s="61"/>
-      <c r="F428" s="61"/>
-      <c r="G428" s="61"/>
-      <c r="H428" s="45"/>
-      <c r="I428" s="45"/>
-      <c r="J428" s="45"/>
+      <c r="F428" s="61" t="s">
+        <v>324</v>
+      </c>
+      <c r="G428" s="144" t="s">
+        <v>29</v>
+      </c>
+      <c r="H428" s="144" t="s">
+        <v>315</v>
+      </c>
+      <c r="I428" s="144">
+        <v>298</v>
+      </c>
+      <c r="J428" s="45">
+        <v>-0.41</v>
+      </c>
       <c r="K428" s="45"/>
-      <c r="L428" s="61"/>
-      <c r="M428" s="61"/>
-      <c r="N428" s="61"/>
+      <c r="L428" s="61" t="s">
+        <v>316</v>
+      </c>
+      <c r="M428" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="N428" s="61" t="s">
+        <v>329</v>
+      </c>
       <c r="O428" s="45"/>
       <c r="P428" s="45"/>
       <c r="Q428" s="45"/>

</xml_diff>

<commit_message>
- adjusted magnetic data from `10.1016/j.matlet.2017.03.159` to more useful property of `saturation magnetic induction` and standardized the name over the other templates
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6491649-20B0-E541-8008-C773742055AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C988B181-5DB3-E54C-80A5-3028F5F6B31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1174,10 +1174,10 @@
     <t>F8</t>
   </si>
   <si>
-    <t>saturation induction</t>
+    <t>5e-4 strain rate</t>
   </si>
   <si>
-    <t>5e-4 strain rate</t>
+    <t>saturation magnetic induction</t>
   </si>
 </sst>
 </file>
@@ -3669,8 +3669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T962"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A430" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H477" sqref="H477"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A464" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J500" sqref="J500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -23798,7 +23798,7 @@
         <v>29</v>
       </c>
       <c r="H442" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I442" s="45">
         <v>298</v>
@@ -23845,7 +23845,7 @@
         <v>29</v>
       </c>
       <c r="H443" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I443" s="45">
         <v>298</v>
@@ -23892,7 +23892,7 @@
         <v>29</v>
       </c>
       <c r="H444" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I444" s="45">
         <v>298</v>
@@ -23939,7 +23939,7 @@
         <v>29</v>
       </c>
       <c r="H445" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I445" s="45">
         <v>298</v>
@@ -23986,7 +23986,7 @@
         <v>29</v>
       </c>
       <c r="H446" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I446" s="45">
         <v>298</v>
@@ -24035,7 +24035,7 @@
         <v>29</v>
       </c>
       <c r="H447" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I447" s="45">
         <v>298</v>
@@ -24084,7 +24084,7 @@
         <v>29</v>
       </c>
       <c r="H448" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I448" s="45">
         <v>298</v>
@@ -24133,7 +24133,7 @@
         <v>29</v>
       </c>
       <c r="H449" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I449" s="45">
         <v>298</v>
@@ -24182,7 +24182,7 @@
         <v>29</v>
       </c>
       <c r="H450" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I450" s="45">
         <v>298</v>
@@ -24229,7 +24229,7 @@
         <v>29</v>
       </c>
       <c r="H451" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I451" s="45">
         <v>298</v>
@@ -24276,7 +24276,7 @@
         <v>29</v>
       </c>
       <c r="H452" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I452" s="45">
         <v>298</v>
@@ -24323,7 +24323,7 @@
         <v>29</v>
       </c>
       <c r="H453" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I453" s="45">
         <v>298</v>
@@ -24370,7 +24370,7 @@
         <v>29</v>
       </c>
       <c r="H454" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I454" s="45">
         <v>298</v>
@@ -24417,7 +24417,7 @@
         <v>29</v>
       </c>
       <c r="H455" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I455" s="45">
         <v>298</v>
@@ -24466,7 +24466,7 @@
         <v>29</v>
       </c>
       <c r="H456" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I456" s="45">
         <v>298</v>
@@ -24515,7 +24515,7 @@
         <v>29</v>
       </c>
       <c r="H457" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I457" s="45">
         <v>298</v>
@@ -24564,7 +24564,7 @@
         <v>29</v>
       </c>
       <c r="H458" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I458" s="45">
         <v>298</v>
@@ -24613,7 +24613,7 @@
         <v>29</v>
       </c>
       <c r="H459" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I459" s="45">
         <v>298</v>
@@ -24660,7 +24660,7 @@
         <v>29</v>
       </c>
       <c r="H460" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I460" s="45">
         <v>298</v>
@@ -24712,7 +24712,7 @@
         <v>29</v>
       </c>
       <c r="H461" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I461" s="45">
         <v>298</v>
@@ -24764,7 +24764,7 @@
         <v>29</v>
       </c>
       <c r="H462" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I462" s="45">
         <v>298</v>
@@ -24816,7 +24816,7 @@
         <v>29</v>
       </c>
       <c r="H463" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I463" s="45">
         <v>298</v>
@@ -24868,7 +24868,7 @@
         <v>29</v>
       </c>
       <c r="H464" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I464" s="45">
         <v>298</v>
@@ -24922,7 +24922,7 @@
         <v>29</v>
       </c>
       <c r="H465" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I465" s="45">
         <v>298</v>
@@ -24976,7 +24976,7 @@
         <v>29</v>
       </c>
       <c r="H466" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I466" s="45">
         <v>298</v>
@@ -25030,7 +25030,7 @@
         <v>29</v>
       </c>
       <c r="H467" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I467" s="45">
         <v>298</v>
@@ -25084,7 +25084,7 @@
         <v>29</v>
       </c>
       <c r="H468" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I468" s="45">
         <v>298</v>
@@ -25580,7 +25580,7 @@
       </c>
       <c r="E479" s="142"/>
       <c r="F479" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G479" s="61" t="s">
         <v>29</v>
@@ -25622,7 +25622,7 @@
       </c>
       <c r="E480" s="144"/>
       <c r="F480" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G480" s="61" t="s">
         <v>29</v>
@@ -25664,7 +25664,7 @@
       </c>
       <c r="E481" s="144"/>
       <c r="F481" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G481" s="61" t="s">
         <v>29</v>
@@ -25706,7 +25706,7 @@
       </c>
       <c r="E482" s="144"/>
       <c r="F482" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G482" s="61" t="s">
         <v>29</v>
@@ -25748,7 +25748,7 @@
       </c>
       <c r="E483" s="144"/>
       <c r="F483" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G483" s="61" t="s">
         <v>29</v>
@@ -25792,7 +25792,7 @@
         <v>341</v>
       </c>
       <c r="F484" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G484" s="61" t="s">
         <v>29</v>
@@ -25836,7 +25836,7 @@
         <v>342</v>
       </c>
       <c r="F485" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G485" s="61" t="s">
         <v>29</v>
@@ -25880,7 +25880,7 @@
         <v>343</v>
       </c>
       <c r="F486" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G486" s="61" t="s">
         <v>29</v>
@@ -25924,7 +25924,7 @@
         <v>344</v>
       </c>
       <c r="F487" s="61" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G487" s="61" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
- extracted extra data from `10.1016/j.matdes.2024.113396`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C988B181-5DB3-E54C-80A5-3028F5F6B31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70C91EB-0A3C-334E-B2F5-635053051C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4494" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4620" uniqueCount="351">
   <si>
     <r>
       <rPr>
@@ -1178,6 +1178,12 @@
   </si>
   <si>
     <t>saturation magnetic induction</t>
+  </si>
+  <si>
+    <t>F11a</t>
+  </si>
+  <si>
+    <t>F11b</t>
   </si>
 </sst>
 </file>
@@ -3667,10 +3673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T962"/>
+  <dimension ref="A1:T961"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A464" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J500" sqref="J500"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A457" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N504" sqref="N504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -25955,19 +25961,41 @@
     </row>
     <row r="488" spans="1:20" ht="15" customHeight="1">
       <c r="A488" s="45"/>
-      <c r="B488" s="45"/>
-      <c r="C488" s="45"/>
-      <c r="D488" s="45"/>
-      <c r="E488" s="45"/>
-      <c r="F488" s="45"/>
-      <c r="G488" s="45"/>
+      <c r="B488" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="C488" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D488" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E488" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F488" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G488" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H488" s="45"/>
-      <c r="I488" s="45"/>
-      <c r="J488" s="45"/>
+      <c r="I488" s="45">
+        <v>300</v>
+      </c>
+      <c r="J488" s="45">
+        <v>2.9702970297029702E-2</v>
+      </c>
       <c r="K488" s="45"/>
-      <c r="L488" s="45"/>
-      <c r="M488" s="45"/>
-      <c r="N488" s="45"/>
+      <c r="L488" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M488" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="N488" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O488" s="45"/>
       <c r="P488" s="45"/>
       <c r="Q488" s="45"/>
@@ -25977,19 +26005,41 @@
     </row>
     <row r="489" spans="1:20" ht="15" customHeight="1">
       <c r="A489" s="45"/>
-      <c r="B489" s="45"/>
-      <c r="C489" s="45"/>
-      <c r="D489" s="45"/>
-      <c r="E489" s="45"/>
-      <c r="F489" s="45"/>
-      <c r="G489" s="45"/>
+      <c r="B489" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C489" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D489" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E489" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F489" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G489" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H489" s="45"/>
-      <c r="I489" s="45"/>
-      <c r="J489" s="45"/>
+      <c r="I489" s="45">
+        <v>300</v>
+      </c>
+      <c r="J489" s="45">
+        <v>0.14172560113154101</v>
+      </c>
       <c r="K489" s="45"/>
-      <c r="L489" s="45"/>
-      <c r="M489" s="45"/>
-      <c r="N489" s="45"/>
+      <c r="L489" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M489" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="N489" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O489" s="45"/>
       <c r="P489" s="45"/>
       <c r="Q489" s="45"/>
@@ -25999,19 +26049,41 @@
     </row>
     <row r="490" spans="1:20" ht="15" customHeight="1">
       <c r="A490" s="45"/>
-      <c r="B490" s="45"/>
-      <c r="C490" s="45"/>
-      <c r="D490" s="45"/>
-      <c r="E490" s="45"/>
-      <c r="F490" s="45"/>
-      <c r="G490" s="45"/>
+      <c r="B490" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C490" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D490" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E490" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F490" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G490" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H490" s="45"/>
-      <c r="I490" s="45"/>
-      <c r="J490" s="45"/>
+      <c r="I490" s="45">
+        <v>300</v>
+      </c>
+      <c r="J490" s="45">
+        <v>0.31485148514851402</v>
+      </c>
       <c r="K490" s="45"/>
-      <c r="L490" s="45"/>
-      <c r="M490" s="45"/>
-      <c r="N490" s="45"/>
+      <c r="L490" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M490" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="N490" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O490" s="45"/>
       <c r="P490" s="45"/>
       <c r="Q490" s="45"/>
@@ -26021,19 +26093,41 @@
     </row>
     <row r="491" spans="1:20" ht="15" customHeight="1">
       <c r="A491" s="45"/>
-      <c r="B491" s="45"/>
-      <c r="C491" s="45"/>
-      <c r="D491" s="45"/>
-      <c r="E491" s="45"/>
-      <c r="F491" s="45"/>
-      <c r="G491" s="45"/>
+      <c r="B491" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C491" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D491" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E491" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F491" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G491" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H491" s="45"/>
-      <c r="I491" s="45"/>
-      <c r="J491" s="45"/>
+      <c r="I491" s="45">
+        <v>300</v>
+      </c>
+      <c r="J491" s="45">
+        <v>0.481188118811881</v>
+      </c>
       <c r="K491" s="45"/>
-      <c r="L491" s="45"/>
-      <c r="M491" s="45"/>
-      <c r="N491" s="45"/>
+      <c r="L491" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M491" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="N491" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O491" s="45"/>
       <c r="P491" s="45"/>
       <c r="Q491" s="45"/>
@@ -26043,19 +26137,41 @@
     </row>
     <row r="492" spans="1:20" ht="15" customHeight="1">
       <c r="A492" s="45"/>
-      <c r="B492" s="45"/>
-      <c r="C492" s="45"/>
-      <c r="D492" s="45"/>
-      <c r="E492" s="45"/>
-      <c r="F492" s="45"/>
-      <c r="G492" s="45"/>
+      <c r="B492" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C492" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D492" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E492" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F492" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G492" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H492" s="45"/>
-      <c r="I492" s="45"/>
-      <c r="J492" s="45"/>
+      <c r="I492" s="45">
+        <v>300</v>
+      </c>
+      <c r="J492" s="45">
+        <v>0.53974540311173902</v>
+      </c>
       <c r="K492" s="45"/>
-      <c r="L492" s="45"/>
-      <c r="M492" s="45"/>
-      <c r="N492" s="45"/>
+      <c r="L492" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M492" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="N492" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O492" s="45"/>
       <c r="P492" s="45"/>
       <c r="Q492" s="45"/>
@@ -26065,19 +26181,41 @@
     </row>
     <row r="493" spans="1:20" ht="15" customHeight="1">
       <c r="A493" s="45"/>
-      <c r="B493" s="45"/>
-      <c r="C493" s="45"/>
-      <c r="D493" s="45"/>
-      <c r="E493" s="45"/>
-      <c r="F493" s="45"/>
-      <c r="G493" s="45"/>
+      <c r="B493" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C493" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D493" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E493" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F493" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G493" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H493" s="45"/>
-      <c r="I493" s="45"/>
-      <c r="J493" s="45"/>
+      <c r="I493" s="45">
+        <v>5</v>
+      </c>
+      <c r="J493" s="45">
+        <v>0.63878787878787802</v>
+      </c>
       <c r="K493" s="45"/>
-      <c r="L493" s="45"/>
-      <c r="M493" s="45"/>
-      <c r="N493" s="45"/>
+      <c r="L493" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M493" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N493" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O493" s="45"/>
       <c r="P493" s="45"/>
       <c r="Q493" s="45"/>
@@ -26087,19 +26225,41 @@
     </row>
     <row r="494" spans="1:20" ht="15" customHeight="1">
       <c r="A494" s="45"/>
-      <c r="B494" s="45"/>
-      <c r="C494" s="45"/>
-      <c r="D494" s="45"/>
-      <c r="E494" s="45"/>
-      <c r="F494" s="45"/>
-      <c r="G494" s="45"/>
+      <c r="B494" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C494" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D494" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E494" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F494" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G494" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H494" s="45"/>
-      <c r="I494" s="45"/>
-      <c r="J494" s="45"/>
+      <c r="I494" s="45">
+        <v>100</v>
+      </c>
+      <c r="J494" s="45">
+        <v>0.61939393939393905</v>
+      </c>
       <c r="K494" s="45"/>
-      <c r="L494" s="45"/>
-      <c r="M494" s="45"/>
-      <c r="N494" s="45"/>
+      <c r="L494" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M494" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N494" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O494" s="45"/>
       <c r="P494" s="45"/>
       <c r="Q494" s="45"/>
@@ -26109,19 +26269,41 @@
     </row>
     <row r="495" spans="1:20" ht="15" customHeight="1">
       <c r="A495" s="45"/>
-      <c r="B495" s="45"/>
-      <c r="C495" s="45"/>
-      <c r="D495" s="45"/>
-      <c r="E495" s="45"/>
-      <c r="F495" s="45"/>
-      <c r="G495" s="45"/>
+      <c r="B495" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C495" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D495" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E495" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F495" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G495" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H495" s="45"/>
-      <c r="I495" s="45"/>
-      <c r="J495" s="45"/>
+      <c r="I495" s="45">
+        <v>200</v>
+      </c>
+      <c r="J495" s="45">
+        <v>0.58545454545454501</v>
+      </c>
       <c r="K495" s="45"/>
-      <c r="L495" s="45"/>
-      <c r="M495" s="45"/>
-      <c r="N495" s="45"/>
+      <c r="L495" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M495" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N495" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O495" s="45"/>
       <c r="P495" s="45"/>
       <c r="Q495" s="45"/>
@@ -26131,19 +26313,41 @@
     </row>
     <row r="496" spans="1:20" ht="15" customHeight="1">
       <c r="A496" s="45"/>
-      <c r="B496" s="45"/>
-      <c r="C496" s="45"/>
-      <c r="D496" s="45"/>
-      <c r="E496" s="45"/>
-      <c r="F496" s="45"/>
-      <c r="G496" s="45"/>
+      <c r="B496" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C496" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D496" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E496" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F496" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G496" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H496" s="45"/>
-      <c r="I496" s="45"/>
-      <c r="J496" s="45"/>
+      <c r="I496" s="45">
+        <v>300</v>
+      </c>
+      <c r="J496" s="45">
+        <v>0.53939393939393898</v>
+      </c>
       <c r="K496" s="45"/>
-      <c r="L496" s="45"/>
-      <c r="M496" s="45"/>
-      <c r="N496" s="45"/>
+      <c r="L496" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M496" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N496" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O496" s="45"/>
       <c r="P496" s="45"/>
       <c r="Q496" s="45"/>
@@ -26153,19 +26357,41 @@
     </row>
     <row r="497" spans="1:20" ht="15" customHeight="1">
       <c r="A497" s="45"/>
-      <c r="B497" s="45"/>
-      <c r="C497" s="45"/>
-      <c r="D497" s="45"/>
-      <c r="E497" s="45"/>
-      <c r="F497" s="45"/>
-      <c r="G497" s="45"/>
+      <c r="B497" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C497" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D497" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E497" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F497" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G497" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H497" s="45"/>
-      <c r="I497" s="45"/>
-      <c r="J497" s="45"/>
+      <c r="I497" s="45">
+        <v>400</v>
+      </c>
+      <c r="J497" s="45">
+        <v>0.47636363636363599</v>
+      </c>
       <c r="K497" s="45"/>
-      <c r="L497" s="45"/>
-      <c r="M497" s="45"/>
-      <c r="N497" s="45"/>
+      <c r="L497" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M497" s="61" t="s">
+        <v>304</v>
+      </c>
+      <c r="N497" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O497" s="45"/>
       <c r="P497" s="45"/>
       <c r="Q497" s="45"/>
@@ -26175,19 +26401,41 @@
     </row>
     <row r="498" spans="1:20" ht="15" customHeight="1">
       <c r="A498" s="45"/>
-      <c r="B498" s="45"/>
-      <c r="C498" s="45"/>
-      <c r="D498" s="45"/>
-      <c r="E498" s="45"/>
-      <c r="F498" s="45"/>
-      <c r="G498" s="45"/>
+      <c r="B498" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C498" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D498" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E498" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F498" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G498" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H498" s="45"/>
-      <c r="I498" s="45"/>
-      <c r="J498" s="45"/>
+      <c r="I498" s="45">
+        <v>300</v>
+      </c>
+      <c r="J498" s="45">
+        <v>489.093701996927</v>
+      </c>
       <c r="K498" s="45"/>
-      <c r="L498" s="45"/>
-      <c r="M498" s="45"/>
-      <c r="N498" s="45"/>
+      <c r="L498" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M498" s="61" t="s">
+        <v>350</v>
+      </c>
+      <c r="N498" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O498" s="45"/>
       <c r="P498" s="45"/>
       <c r="Q498" s="45"/>
@@ -26197,19 +26445,41 @@
     </row>
     <row r="499" spans="1:20" ht="15" customHeight="1">
       <c r="A499" s="45"/>
-      <c r="B499" s="45"/>
-      <c r="C499" s="45"/>
-      <c r="D499" s="45"/>
-      <c r="E499" s="45"/>
-      <c r="F499" s="45"/>
-      <c r="G499" s="45"/>
+      <c r="B499" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="C499" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D499" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E499" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F499" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G499" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H499" s="45"/>
-      <c r="I499" s="45"/>
-      <c r="J499" s="45"/>
+      <c r="I499" s="45">
+        <v>300</v>
+      </c>
+      <c r="J499" s="45">
+        <v>323.19508448540699</v>
+      </c>
       <c r="K499" s="45"/>
-      <c r="L499" s="45"/>
-      <c r="M499" s="45"/>
-      <c r="N499" s="45"/>
+      <c r="L499" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M499" s="61" t="s">
+        <v>350</v>
+      </c>
+      <c r="N499" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O499" s="45"/>
       <c r="P499" s="45"/>
       <c r="Q499" s="45"/>
@@ -26219,19 +26489,41 @@
     </row>
     <row r="500" spans="1:20" ht="15" customHeight="1">
       <c r="A500" s="45"/>
-      <c r="B500" s="45"/>
-      <c r="C500" s="45"/>
-      <c r="D500" s="45"/>
-      <c r="E500" s="45"/>
-      <c r="F500" s="45"/>
-      <c r="G500" s="45"/>
+      <c r="B500" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="C500" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D500" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E500" s="61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F500" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G500" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H500" s="45"/>
-      <c r="I500" s="45"/>
-      <c r="J500" s="45"/>
+      <c r="I500" s="45">
+        <v>300</v>
+      </c>
+      <c r="J500" s="45">
+        <v>324.42396313363997</v>
+      </c>
       <c r="K500" s="45"/>
-      <c r="L500" s="45"/>
-      <c r="M500" s="45"/>
-      <c r="N500" s="45"/>
+      <c r="L500" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M500" s="61" t="s">
+        <v>350</v>
+      </c>
+      <c r="N500" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O500" s="45"/>
       <c r="P500" s="45"/>
       <c r="Q500" s="45"/>
@@ -26241,19 +26533,41 @@
     </row>
     <row r="501" spans="1:20" ht="15" customHeight="1">
       <c r="A501" s="45"/>
-      <c r="B501" s="45"/>
-      <c r="C501" s="45"/>
-      <c r="D501" s="45"/>
-      <c r="E501" s="45"/>
-      <c r="F501" s="45"/>
-      <c r="G501" s="45"/>
+      <c r="B501" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="C501" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="D501" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="E501" s="61" t="s">
+        <v>303</v>
+      </c>
+      <c r="F501" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G501" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="H501" s="45"/>
-      <c r="I501" s="45"/>
-      <c r="J501" s="45"/>
+      <c r="I501" s="45">
+        <v>300</v>
+      </c>
+      <c r="J501" s="45">
+        <v>342.85714285714198</v>
+      </c>
       <c r="K501" s="45"/>
-      <c r="L501" s="45"/>
-      <c r="M501" s="45"/>
-      <c r="N501" s="45"/>
+      <c r="L501" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="M501" s="61" t="s">
+        <v>350</v>
+      </c>
+      <c r="N501" s="61" t="s">
+        <v>307</v>
+      </c>
       <c r="O501" s="45"/>
       <c r="P501" s="45"/>
       <c r="Q501" s="45"/>
@@ -28945,7 +29259,7 @@
       <c r="S623" s="37"/>
       <c r="T623" s="37"/>
     </row>
-    <row r="624" spans="1:20" ht="15" customHeight="1">
+    <row r="624" spans="1:20" ht="16" customHeight="1">
       <c r="A624" s="45"/>
       <c r="B624" s="45"/>
       <c r="C624" s="45"/>
@@ -29580,7 +29894,7 @@
       <c r="P652" s="45"/>
       <c r="Q652" s="45"/>
       <c r="R652" s="45"/>
-      <c r="S652" s="37"/>
+      <c r="S652" s="46"/>
       <c r="T652" s="37"/>
     </row>
     <row r="653" spans="1:20" ht="16" customHeight="1">
@@ -31428,7 +31742,7 @@
       <c r="P736" s="45"/>
       <c r="Q736" s="45"/>
       <c r="R736" s="45"/>
-      <c r="S736" s="46"/>
+      <c r="S736" s="37"/>
       <c r="T736" s="37"/>
     </row>
     <row r="737" spans="1:20" ht="16" customHeight="1">
@@ -31472,7 +31786,7 @@
       <c r="P738" s="45"/>
       <c r="Q738" s="45"/>
       <c r="R738" s="45"/>
-      <c r="S738" s="37"/>
+      <c r="S738" s="46"/>
       <c r="T738" s="37"/>
     </row>
     <row r="739" spans="1:20" ht="16" customHeight="1">
@@ -31758,7 +32072,7 @@
       <c r="P751" s="45"/>
       <c r="Q751" s="45"/>
       <c r="R751" s="45"/>
-      <c r="S751" s="46"/>
+      <c r="S751" s="37"/>
       <c r="T751" s="37"/>
     </row>
     <row r="752" spans="1:20" ht="16" customHeight="1">
@@ -34027,7 +34341,7 @@
       <c r="S854" s="37"/>
       <c r="T854" s="37"/>
     </row>
-    <row r="855" spans="1:20" ht="16" customHeight="1">
+    <row r="855" spans="1:20" ht="15" customHeight="1">
       <c r="A855" s="45"/>
       <c r="B855" s="45"/>
       <c r="C855" s="45"/>
@@ -34046,8 +34360,8 @@
       <c r="P855" s="45"/>
       <c r="Q855" s="45"/>
       <c r="R855" s="45"/>
-      <c r="S855" s="37"/>
-      <c r="T855" s="37"/>
+      <c r="S855" s="45"/>
+      <c r="T855" s="45"/>
     </row>
     <row r="856" spans="1:20" ht="15" customHeight="1">
       <c r="A856" s="45"/>
@@ -35899,7 +36213,6 @@
     </row>
     <row r="940" spans="1:20" ht="15" customHeight="1">
       <c r="A940" s="45"/>
-      <c r="B940" s="45"/>
       <c r="C940" s="45"/>
       <c r="D940" s="45"/>
       <c r="E940" s="45"/>
@@ -36026,7 +36339,6 @@
     </row>
     <row r="946" spans="1:20" ht="15" customHeight="1">
       <c r="A946" s="45"/>
-      <c r="C946" s="45"/>
       <c r="D946" s="45"/>
       <c r="E946" s="45"/>
       <c r="F946" s="45"/>
@@ -36052,9 +36364,6 @@
       <c r="F947" s="45"/>
       <c r="G947" s="45"/>
       <c r="H947" s="45"/>
-      <c r="I947" s="45"/>
-      <c r="J947" s="45"/>
-      <c r="K947" s="45"/>
       <c r="L947" s="45"/>
       <c r="M947" s="45"/>
       <c r="N947" s="45"/>
@@ -36106,7 +36415,6 @@
       <c r="F950" s="45"/>
       <c r="G950" s="45"/>
       <c r="H950" s="45"/>
-      <c r="L950" s="45"/>
       <c r="M950" s="45"/>
       <c r="N950" s="45"/>
       <c r="O950" s="45"/>
@@ -36222,23 +36530,12 @@
       <c r="M957" s="45"/>
       <c r="N957" s="45"/>
       <c r="O957" s="45"/>
-      <c r="P957" s="45"/>
       <c r="Q957" s="45"/>
       <c r="R957" s="45"/>
       <c r="S957" s="45"/>
       <c r="T957" s="45"/>
     </row>
     <row r="958" spans="1:20" ht="15" customHeight="1">
-      <c r="A958" s="45"/>
-      <c r="D958" s="45"/>
-      <c r="E958" s="45"/>
-      <c r="F958" s="45"/>
-      <c r="G958" s="45"/>
-      <c r="H958" s="45"/>
-      <c r="M958" s="45"/>
-      <c r="N958" s="45"/>
-      <c r="O958" s="45"/>
-      <c r="Q958" s="45"/>
       <c r="R958" s="45"/>
       <c r="S958" s="45"/>
       <c r="T958" s="45"/>
@@ -36257,11 +36554,6 @@
       <c r="R961" s="45"/>
       <c r="S961" s="45"/>
       <c r="T961" s="45"/>
-    </row>
-    <row r="962" spans="18:20" ht="15" customHeight="1">
-      <c r="R962" s="45"/>
-      <c r="S962" s="45"/>
-      <c r="T962" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- extracted extra data from `10.1016/j.msea.2016.05.082`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA390F61-1A72-2344-9A5A-3CE631FB43AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBA2321-74CE-3547-9431-2650D1A5CB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7900" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6273" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6287" uniqueCount="490">
   <si>
     <r>
       <rPr>
@@ -1647,6 +1647,18 @@
   </si>
   <si>
     <t>bulk sample; liquid maintained at 1550*C for 15min and poured into a preheated ZrO2-coated MgO cruicible; R is hR7; sigma is FeCr-type tP30; annealed at 1273K for 6h and furnace cooled; hardness converted from HRC of 48.5</t>
+  </si>
+  <si>
+    <t>NiCoFeCrAl</t>
+  </si>
+  <si>
+    <t>NiCoFeCr</t>
+  </si>
+  <si>
+    <t>nanohardness</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2016.05.082</t>
   </si>
 </sst>
 </file>
@@ -4156,8 +4168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A657" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H682" sqref="H682"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A663" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J689" sqref="J689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -35341,19 +35353,37 @@
     </row>
     <row r="679" spans="1:20" ht="16" customHeight="1">
       <c r="A679" s="45"/>
-      <c r="B679" s="45"/>
-      <c r="C679" s="45"/>
-      <c r="D679" s="45"/>
+      <c r="B679" s="61" t="s">
+        <v>486</v>
+      </c>
+      <c r="C679" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D679" s="61" t="s">
+        <v>172</v>
+      </c>
       <c r="E679" s="45"/>
-      <c r="F679" s="45"/>
-      <c r="G679" s="45"/>
+      <c r="F679" s="61" t="s">
+        <v>488</v>
+      </c>
+      <c r="G679" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H679" s="45"/>
-      <c r="I679" s="45"/>
-      <c r="J679" s="45"/>
+      <c r="I679" s="45">
+        <v>298</v>
+      </c>
+      <c r="J679" s="62">
+        <v>7210000000</v>
+      </c>
       <c r="K679" s="45"/>
-      <c r="L679" s="45"/>
+      <c r="L679" s="61" t="s">
+        <v>33</v>
+      </c>
       <c r="M679" s="45"/>
-      <c r="N679" s="45"/>
+      <c r="N679" s="61" t="s">
+        <v>489</v>
+      </c>
       <c r="O679" s="45"/>
       <c r="P679" s="45"/>
       <c r="Q679" s="45"/>
@@ -35363,19 +35393,37 @@
     </row>
     <row r="680" spans="1:20" ht="16" customHeight="1">
       <c r="A680" s="45"/>
-      <c r="B680" s="45"/>
-      <c r="C680" s="45"/>
-      <c r="D680" s="45"/>
+      <c r="B680" s="61" t="s">
+        <v>487</v>
+      </c>
+      <c r="C680" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D680" s="61" t="s">
+        <v>172</v>
+      </c>
       <c r="E680" s="45"/>
-      <c r="F680" s="45"/>
-      <c r="G680" s="45"/>
+      <c r="F680" s="61" t="s">
+        <v>488</v>
+      </c>
+      <c r="G680" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H680" s="45"/>
-      <c r="I680" s="45"/>
-      <c r="J680" s="45"/>
+      <c r="I680" s="45">
+        <v>298</v>
+      </c>
+      <c r="J680" s="62">
+        <v>3860000000</v>
+      </c>
       <c r="K680" s="45"/>
-      <c r="L680" s="45"/>
+      <c r="L680" s="61" t="s">
+        <v>33</v>
+      </c>
       <c r="M680" s="45"/>
-      <c r="N680" s="45"/>
+      <c r="N680" s="61" t="s">
+        <v>489</v>
+      </c>
       <c r="O680" s="45"/>
       <c r="P680" s="45"/>
       <c r="Q680" s="45"/>

</xml_diff>

<commit_message>
- extracted extra data from `10.3390/cryst12020219`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBA2321-74CE-3547-9431-2650D1A5CB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2CAB8-BDCA-F343-861D-1CE751CBFFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="7900" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6287" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6341" uniqueCount="496">
   <si>
     <r>
       <rPr>
@@ -1660,6 +1660,24 @@
   <si>
     <t>10.1016/j.msea.2016.05.082</t>
   </si>
+  <si>
+    <t>10.3390/cryst12020219</t>
+  </si>
+  <si>
+    <t>MA+FAST(SPS)</t>
+  </si>
+  <si>
+    <t>Upgraded Field Assisted Sintering technology (U-FAST) at 1873K under 90MPa for 10min</t>
+  </si>
+  <si>
+    <t>CrNbTaVW</t>
+  </si>
+  <si>
+    <t>CrNbTaVW1.7</t>
+  </si>
+  <si>
+    <t>reduced elastic modulus</t>
+  </si>
 </sst>
 </file>
 
@@ -1668,7 +1686,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1771,6 +1789,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
       <family val="2"/>
@@ -2692,7 +2716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3006,6 +3030,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4169,7 +4194,7 @@
   <dimension ref="A1:T960"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A663" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J689" sqref="J689"/>
+      <selection activeCell="H691" sqref="H691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -35433,63 +35458,147 @@
     </row>
     <row r="681" spans="1:20" ht="16" customHeight="1">
       <c r="A681" s="45"/>
-      <c r="B681" s="45"/>
-      <c r="C681" s="45"/>
-      <c r="D681" s="45"/>
-      <c r="E681" s="45"/>
-      <c r="F681" s="45"/>
-      <c r="G681" s="45"/>
+      <c r="B681" s="149" t="s">
+        <v>493</v>
+      </c>
+      <c r="C681" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D681" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E681" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F681" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G681" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H681" s="45"/>
-      <c r="I681" s="45"/>
-      <c r="J681" s="45"/>
-      <c r="K681" s="45"/>
-      <c r="L681" s="45"/>
-      <c r="M681" s="45"/>
-      <c r="N681" s="45"/>
+      <c r="I681" s="45">
+        <v>298</v>
+      </c>
+      <c r="J681" s="99">
+        <f t="shared" ref="J681:K682" si="43">P681*9807000</f>
+        <v>13533660000</v>
+      </c>
+      <c r="K681" s="99">
+        <f t="shared" si="43"/>
+        <v>392280000</v>
+      </c>
+      <c r="L681" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M681" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="N681" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="O681" s="45"/>
-      <c r="P681" s="45"/>
-      <c r="Q681" s="45"/>
+      <c r="P681" s="45">
+        <v>1380</v>
+      </c>
+      <c r="Q681" s="45">
+        <v>40</v>
+      </c>
       <c r="R681" s="45"/>
       <c r="S681" s="46"/>
       <c r="T681" s="37"/>
     </row>
     <row r="682" spans="1:20" ht="16" customHeight="1">
       <c r="A682" s="45"/>
-      <c r="B682" s="45"/>
-      <c r="C682" s="45"/>
-      <c r="D682" s="45"/>
-      <c r="E682" s="45"/>
-      <c r="F682" s="45"/>
-      <c r="G682" s="45"/>
+      <c r="B682" s="149" t="s">
+        <v>494</v>
+      </c>
+      <c r="C682" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D682" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E682" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F682" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G682" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H682" s="45"/>
-      <c r="I682" s="45"/>
-      <c r="J682" s="45"/>
-      <c r="K682" s="45"/>
-      <c r="L682" s="45"/>
-      <c r="M682" s="45"/>
-      <c r="N682" s="45"/>
+      <c r="I682" s="45">
+        <v>298</v>
+      </c>
+      <c r="J682" s="99">
+        <f t="shared" si="43"/>
+        <v>12160680000</v>
+      </c>
+      <c r="K682" s="99">
+        <f t="shared" si="43"/>
+        <v>196140000</v>
+      </c>
+      <c r="L682" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M682" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="N682" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="O682" s="45"/>
-      <c r="P682" s="45"/>
-      <c r="Q682" s="45"/>
+      <c r="P682" s="45">
+        <v>1240</v>
+      </c>
+      <c r="Q682" s="45">
+        <v>20</v>
+      </c>
       <c r="R682" s="45"/>
       <c r="S682" s="46"/>
       <c r="T682" s="37"/>
     </row>
     <row r="683" spans="1:20" ht="16" customHeight="1">
       <c r="A683" s="45"/>
-      <c r="B683" s="45"/>
-      <c r="C683" s="45"/>
-      <c r="D683" s="45"/>
-      <c r="E683" s="45"/>
-      <c r="F683" s="45"/>
-      <c r="G683" s="45"/>
+      <c r="B683" s="149" t="s">
+        <v>493</v>
+      </c>
+      <c r="C683" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D683" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E683" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F683" s="61" t="s">
+        <v>488</v>
+      </c>
+      <c r="G683" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H683" s="45"/>
-      <c r="I683" s="45"/>
-      <c r="J683" s="45"/>
-      <c r="K683" s="45"/>
-      <c r="L683" s="45"/>
-      <c r="M683" s="45"/>
-      <c r="N683" s="45"/>
+      <c r="I683" s="45">
+        <v>298</v>
+      </c>
+      <c r="J683" s="62">
+        <v>19000000000</v>
+      </c>
+      <c r="K683" s="62">
+        <v>700000000</v>
+      </c>
+      <c r="L683" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M683" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="N683" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="O683" s="45"/>
       <c r="P683" s="45"/>
       <c r="Q683" s="45"/>
@@ -35499,19 +35608,43 @@
     </row>
     <row r="684" spans="1:20" ht="16" customHeight="1">
       <c r="A684" s="45"/>
-      <c r="B684" s="45"/>
-      <c r="C684" s="45"/>
-      <c r="D684" s="45"/>
-      <c r="E684" s="45"/>
-      <c r="F684" s="45"/>
-      <c r="G684" s="45"/>
+      <c r="B684" s="149" t="s">
+        <v>494</v>
+      </c>
+      <c r="C684" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D684" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E684" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F684" s="61" t="s">
+        <v>488</v>
+      </c>
+      <c r="G684" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H684" s="45"/>
-      <c r="I684" s="45"/>
-      <c r="J684" s="45"/>
-      <c r="K684" s="45"/>
-      <c r="L684" s="45"/>
-      <c r="M684" s="45"/>
-      <c r="N684" s="45"/>
+      <c r="I684" s="45">
+        <v>298</v>
+      </c>
+      <c r="J684" s="62">
+        <v>17500000000</v>
+      </c>
+      <c r="K684" s="62">
+        <v>300000000</v>
+      </c>
+      <c r="L684" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M684" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="N684" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="O684" s="45"/>
       <c r="P684" s="45"/>
       <c r="Q684" s="45"/>
@@ -35521,19 +35654,43 @@
     </row>
     <row r="685" spans="1:20" ht="16" customHeight="1">
       <c r="A685" s="45"/>
-      <c r="B685" s="45"/>
-      <c r="C685" s="45"/>
-      <c r="D685" s="45"/>
-      <c r="E685" s="45"/>
-      <c r="F685" s="45"/>
-      <c r="G685" s="45"/>
+      <c r="B685" s="149" t="s">
+        <v>493</v>
+      </c>
+      <c r="C685" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D685" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E685" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F685" s="61" t="s">
+        <v>495</v>
+      </c>
+      <c r="G685" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H685" s="45"/>
-      <c r="I685" s="45"/>
-      <c r="J685" s="45"/>
-      <c r="K685" s="45"/>
-      <c r="L685" s="45"/>
-      <c r="M685" s="45"/>
-      <c r="N685" s="45"/>
+      <c r="I685" s="45">
+        <v>298</v>
+      </c>
+      <c r="J685" s="62">
+        <v>329000000000</v>
+      </c>
+      <c r="K685" s="62">
+        <v>7000000000</v>
+      </c>
+      <c r="L685" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M685" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="N685" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="O685" s="45"/>
       <c r="P685" s="45"/>
       <c r="Q685" s="45"/>
@@ -35543,19 +35700,43 @@
     </row>
     <row r="686" spans="1:20" ht="16" customHeight="1">
       <c r="A686" s="45"/>
-      <c r="B686" s="45"/>
-      <c r="C686" s="45"/>
-      <c r="D686" s="45"/>
-      <c r="E686" s="45"/>
-      <c r="F686" s="45"/>
-      <c r="G686" s="45"/>
+      <c r="B686" s="149" t="s">
+        <v>494</v>
+      </c>
+      <c r="C686" s="61" t="s">
+        <v>189</v>
+      </c>
+      <c r="D686" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="E686" s="61" t="s">
+        <v>492</v>
+      </c>
+      <c r="F686" s="61" t="s">
+        <v>495</v>
+      </c>
+      <c r="G686" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H686" s="45"/>
-      <c r="I686" s="45"/>
-      <c r="J686" s="45"/>
-      <c r="K686" s="45"/>
-      <c r="L686" s="45"/>
-      <c r="M686" s="45"/>
-      <c r="N686" s="45"/>
+      <c r="I686" s="45">
+        <v>298</v>
+      </c>
+      <c r="J686" s="62">
+        <v>316000000000</v>
+      </c>
+      <c r="K686" s="62">
+        <v>4000000000</v>
+      </c>
+      <c r="L686" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M686" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="N686" s="61" t="s">
+        <v>490</v>
+      </c>
       <c r="O686" s="45"/>
       <c r="P686" s="45"/>
       <c r="Q686" s="45"/>

</xml_diff>

<commit_message>
- extracted extra data from `10.1016/j.msea.2015.08.024` missed by Citrine/UCSB
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2CAB8-BDCA-F343-861D-1CE751CBFFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D347855-26B9-404E-A5D9-77E9E163F5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7900" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6540" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6341" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6349" uniqueCount="500">
   <si>
     <r>
       <rPr>
@@ -1677,6 +1677,18 @@
   </si>
   <si>
     <t>reduced elastic modulus</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2015.08.024</t>
+  </si>
+  <si>
+    <t>HfNbTaTiZr</t>
+  </si>
+  <si>
+    <t>AAM+AIM</t>
+  </si>
+  <si>
+    <t>actual gas atmosphere of He instead of Ar</t>
   </si>
 </sst>
 </file>
@@ -2918,57 +2930,8 @@
     <xf numFmtId="164" fontId="14" fillId="10" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3029,8 +2992,57 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4193,8 +4205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A663" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H691" sqref="H691"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A669" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J690" sqref="J690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4251,19 +4263,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="128" t="s">
+      <c r="D2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="129"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
-      <c r="N2" s="136"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="121"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4279,17 +4291,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="137"/>
-      <c r="N3" s="140"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="125"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4330,43 +4342,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="141" t="s">
+      <c r="C5" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="143" t="s">
+      <c r="D5" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="143" t="s">
+      <c r="E5" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="143" t="s">
+      <c r="F5" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="143" t="s">
+      <c r="G5" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="144" t="s">
+      <c r="H5" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="143" t="s">
+      <c r="I5" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="143" t="s">
+      <c r="J5" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="143" t="s">
+      <c r="K5" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="143" t="s">
+      <c r="L5" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="143" t="s">
+      <c r="M5" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="143" t="s">
+      <c r="N5" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="111" t="s">
+      <c r="O5" s="133" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4382,19 +4394,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="146"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="147"/>
-      <c r="L6" s="142"/>
-      <c r="M6" s="142"/>
-      <c r="N6" s="142"/>
-      <c r="O6" s="112"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="131"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+      <c r="O6" s="134"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4444,7 +4456,7 @@
       <c r="N7" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="113"/>
+      <c r="O7" s="135"/>
       <c r="P7" s="68" t="s">
         <v>77</v>
       </c>
@@ -4459,35 +4471,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="63"/>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="136" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="115"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="117" t="s">
+      <c r="C8" s="137"/>
+      <c r="D8" s="137"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="122" t="s">
+      <c r="G8" s="140"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="143"/>
+      <c r="M8" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="123"/>
+      <c r="N8" s="145"/>
       <c r="O8" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="124" t="s">
+      <c r="P8" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="126"/>
-      <c r="T8" s="127"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="148"/>
+      <c r="S8" s="148"/>
+      <c r="T8" s="149"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="64" t="s">
@@ -31270,10 +31282,10 @@
       <c r="T589" s="37"/>
     </row>
     <row r="590" spans="1:20" ht="15" customHeight="1">
-      <c r="A590" s="148" t="s">
+      <c r="A590" s="111" t="s">
         <v>391</v>
       </c>
-      <c r="B590" s="148" t="s">
+      <c r="B590" s="111" t="s">
         <v>392</v>
       </c>
       <c r="C590" s="61" t="s">
@@ -35458,7 +35470,7 @@
     </row>
     <row r="681" spans="1:20" ht="16" customHeight="1">
       <c r="A681" s="45"/>
-      <c r="B681" s="149" t="s">
+      <c r="B681" s="112" t="s">
         <v>493</v>
       </c>
       <c r="C681" s="61" t="s">
@@ -35510,7 +35522,7 @@
     </row>
     <row r="682" spans="1:20" ht="16" customHeight="1">
       <c r="A682" s="45"/>
-      <c r="B682" s="149" t="s">
+      <c r="B682" s="112" t="s">
         <v>494</v>
       </c>
       <c r="C682" s="61" t="s">
@@ -35562,7 +35574,7 @@
     </row>
     <row r="683" spans="1:20" ht="16" customHeight="1">
       <c r="A683" s="45"/>
-      <c r="B683" s="149" t="s">
+      <c r="B683" s="112" t="s">
         <v>493</v>
       </c>
       <c r="C683" s="61" t="s">
@@ -35608,7 +35620,7 @@
     </row>
     <row r="684" spans="1:20" ht="16" customHeight="1">
       <c r="A684" s="45"/>
-      <c r="B684" s="149" t="s">
+      <c r="B684" s="112" t="s">
         <v>494</v>
       </c>
       <c r="C684" s="61" t="s">
@@ -35654,7 +35666,7 @@
     </row>
     <row r="685" spans="1:20" ht="16" customHeight="1">
       <c r="A685" s="45"/>
-      <c r="B685" s="149" t="s">
+      <c r="B685" s="112" t="s">
         <v>493</v>
       </c>
       <c r="C685" s="61" t="s">
@@ -35700,7 +35712,7 @@
     </row>
     <row r="686" spans="1:20" ht="16" customHeight="1">
       <c r="A686" s="45"/>
-      <c r="B686" s="149" t="s">
+      <c r="B686" s="112" t="s">
         <v>494</v>
       </c>
       <c r="C686" s="61" t="s">
@@ -35746,19 +35758,39 @@
     </row>
     <row r="687" spans="1:20" ht="16" customHeight="1">
       <c r="A687" s="45"/>
-      <c r="B687" s="45"/>
-      <c r="C687" s="45"/>
-      <c r="D687" s="45"/>
-      <c r="E687" s="45"/>
-      <c r="F687" s="45"/>
-      <c r="G687" s="45"/>
+      <c r="B687" s="61" t="s">
+        <v>497</v>
+      </c>
+      <c r="C687" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="D687" s="61" t="s">
+        <v>498</v>
+      </c>
+      <c r="E687" s="61" t="s">
+        <v>499</v>
+      </c>
+      <c r="F687" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="G687" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H687" s="45"/>
-      <c r="I687" s="45"/>
-      <c r="J687" s="45"/>
+      <c r="I687" s="45">
+        <v>298</v>
+      </c>
+      <c r="J687" s="45">
+        <v>20</v>
+      </c>
       <c r="K687" s="45"/>
-      <c r="L687" s="45"/>
+      <c r="L687" s="61" t="s">
+        <v>67</v>
+      </c>
       <c r="M687" s="45"/>
-      <c r="N687" s="45"/>
+      <c r="N687" s="61" t="s">
+        <v>496</v>
+      </c>
       <c r="O687" s="45"/>
       <c r="P687" s="45"/>
       <c r="Q687" s="45"/>
@@ -41634,6 +41666,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -41648,11 +41685,6 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- extracted extra data from `10.1016/j.intermet.2021.107239`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D347855-26B9-404E-A5D9-77E9E163F5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7441E9E0-AD08-C648-93A6-85551015DF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6540" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="5720" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6349" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6709" uniqueCount="512">
   <si>
     <r>
       <rPr>
@@ -1689,6 +1689,42 @@
   </si>
   <si>
     <t>actual gas atmosphere of He instead of Ar</t>
+  </si>
+  <si>
+    <t>(CoCrMnNi)20 Fe20</t>
+  </si>
+  <si>
+    <t>(CoCrMnNi)15 Fe40</t>
+  </si>
+  <si>
+    <t>(CoCrMnNi)12.5 Fe50</t>
+  </si>
+  <si>
+    <t>(CoCrMnNi)10 Fe60</t>
+  </si>
+  <si>
+    <t>VAM+H+CR+A+WQ</t>
+  </si>
+  <si>
+    <t>homogenized at 1273K for 24h and cold rolled with 90% reduction to achieve initial alloy; homogenized at 1173K for 3min and quenched to arrive at grain size around 4um; finegrained</t>
+  </si>
+  <si>
+    <t>homogenized at 1273K for 24h and cold rolled with 90% reduction to achieve initial alloy; homogenized at 1273K for 10h and quenched to arrive at grain size around 57um; large grains</t>
+  </si>
+  <si>
+    <t>homogenized at 1273K for 24h and cold rolled with 90% reduction to achieve initial alloy; homogenized at 1173K for 2h and quenched to arrive at grain size around 17um; medium grains</t>
+  </si>
+  <si>
+    <t>homogenized at 1273K for 24h and cold rolled with 90% reduction to achieve initial alloy; hall-petch coefficients derived from fidderent annealing conditions</t>
+  </si>
+  <si>
+    <t>hall-petch coefficient</t>
+  </si>
+  <si>
+    <t>Pa/m^0.5</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2021.107239</t>
   </si>
 </sst>
 </file>
@@ -4205,8 +4241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A669" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J690" sqref="J690"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C694" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O714" sqref="O714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -35800,19 +35836,41 @@
     </row>
     <row r="688" spans="1:20" ht="16" customHeight="1">
       <c r="A688" s="45"/>
-      <c r="B688" s="45"/>
-      <c r="C688" s="45"/>
-      <c r="D688" s="45"/>
-      <c r="E688" s="45"/>
-      <c r="F688" s="45"/>
-      <c r="G688" s="45"/>
+      <c r="B688" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C688" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D688" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E688" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F688" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G688" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H688" s="45"/>
-      <c r="I688" s="45"/>
-      <c r="J688" s="45"/>
+      <c r="I688" s="45">
+        <v>298</v>
+      </c>
+      <c r="J688" s="62">
+        <v>406000000</v>
+      </c>
       <c r="K688" s="45"/>
-      <c r="L688" s="45"/>
-      <c r="M688" s="45"/>
-      <c r="N688" s="45"/>
+      <c r="L688" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M688" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N688" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O688" s="45"/>
       <c r="P688" s="45"/>
       <c r="Q688" s="45"/>
@@ -35822,19 +35880,41 @@
     </row>
     <row r="689" spans="1:20" ht="16" customHeight="1">
       <c r="A689" s="45"/>
-      <c r="B689" s="45"/>
-      <c r="C689" s="45"/>
-      <c r="D689" s="45"/>
-      <c r="E689" s="45"/>
-      <c r="F689" s="45"/>
-      <c r="G689" s="45"/>
+      <c r="B689" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C689" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D689" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E689" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F689" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G689" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H689" s="45"/>
-      <c r="I689" s="45"/>
-      <c r="J689" s="45"/>
+      <c r="I689" s="45">
+        <v>298</v>
+      </c>
+      <c r="J689" s="62">
+        <v>296000000</v>
+      </c>
       <c r="K689" s="45"/>
-      <c r="L689" s="45"/>
-      <c r="M689" s="45"/>
-      <c r="N689" s="45"/>
+      <c r="L689" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M689" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N689" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O689" s="45"/>
       <c r="P689" s="45"/>
       <c r="Q689" s="45"/>
@@ -35844,19 +35924,41 @@
     </row>
     <row r="690" spans="1:20" ht="16" customHeight="1">
       <c r="A690" s="45"/>
-      <c r="B690" s="45"/>
-      <c r="C690" s="45"/>
-      <c r="D690" s="45"/>
-      <c r="E690" s="45"/>
-      <c r="F690" s="45"/>
-      <c r="G690" s="45"/>
+      <c r="B690" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C690" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D690" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E690" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F690" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G690" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H690" s="45"/>
-      <c r="I690" s="45"/>
-      <c r="J690" s="45"/>
+      <c r="I690" s="45">
+        <v>298</v>
+      </c>
+      <c r="J690" s="62">
+        <v>276000000</v>
+      </c>
       <c r="K690" s="45"/>
-      <c r="L690" s="45"/>
-      <c r="M690" s="45"/>
-      <c r="N690" s="45"/>
+      <c r="L690" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M690" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N690" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O690" s="45"/>
       <c r="P690" s="45"/>
       <c r="Q690" s="45"/>
@@ -35866,19 +35968,41 @@
     </row>
     <row r="691" spans="1:20" ht="16" customHeight="1">
       <c r="A691" s="45"/>
-      <c r="B691" s="45"/>
-      <c r="C691" s="45"/>
-      <c r="D691" s="45"/>
-      <c r="E691" s="45"/>
-      <c r="F691" s="45"/>
-      <c r="G691" s="45"/>
+      <c r="B691" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C691" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D691" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E691" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F691" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G691" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H691" s="45"/>
-      <c r="I691" s="45"/>
-      <c r="J691" s="45"/>
+      <c r="I691" s="45">
+        <v>298</v>
+      </c>
+      <c r="J691" s="62">
+        <v>235000000</v>
+      </c>
       <c r="K691" s="45"/>
-      <c r="L691" s="45"/>
-      <c r="M691" s="45"/>
-      <c r="N691" s="45"/>
+      <c r="L691" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M691" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N691" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O691" s="45"/>
       <c r="P691" s="45"/>
       <c r="Q691" s="45"/>
@@ -35888,19 +36012,41 @@
     </row>
     <row r="692" spans="1:20" ht="16" customHeight="1">
       <c r="A692" s="45"/>
-      <c r="B692" s="45"/>
-      <c r="C692" s="45"/>
-      <c r="D692" s="45"/>
-      <c r="E692" s="45"/>
-      <c r="F692" s="45"/>
-      <c r="G692" s="45"/>
+      <c r="B692" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C692" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D692" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E692" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F692" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G692" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H692" s="45"/>
-      <c r="I692" s="45"/>
-      <c r="J692" s="45"/>
+      <c r="I692" s="45">
+        <v>298</v>
+      </c>
+      <c r="J692" s="62">
+        <v>257000000</v>
+      </c>
       <c r="K692" s="45"/>
-      <c r="L692" s="45"/>
-      <c r="M692" s="45"/>
-      <c r="N692" s="45"/>
+      <c r="L692" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M692" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N692" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O692" s="45"/>
       <c r="P692" s="45"/>
       <c r="Q692" s="45"/>
@@ -35910,19 +36056,41 @@
     </row>
     <row r="693" spans="1:20" ht="16" customHeight="1">
       <c r="A693" s="45"/>
-      <c r="B693" s="45"/>
-      <c r="C693" s="45"/>
-      <c r="D693" s="45"/>
-      <c r="E693" s="45"/>
-      <c r="F693" s="45"/>
-      <c r="G693" s="45"/>
+      <c r="B693" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C693" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D693" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E693" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F693" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G693" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H693" s="45"/>
-      <c r="I693" s="45"/>
-      <c r="J693" s="45"/>
+      <c r="I693" s="45">
+        <v>298</v>
+      </c>
+      <c r="J693" s="62">
+        <v>221000000</v>
+      </c>
       <c r="K693" s="45"/>
-      <c r="L693" s="45"/>
-      <c r="M693" s="45"/>
-      <c r="N693" s="45"/>
+      <c r="L693" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M693" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N693" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O693" s="45"/>
       <c r="P693" s="45"/>
       <c r="Q693" s="45"/>
@@ -35932,19 +36100,41 @@
     </row>
     <row r="694" spans="1:20" ht="16" customHeight="1">
       <c r="A694" s="45"/>
-      <c r="B694" s="45"/>
-      <c r="C694" s="45"/>
-      <c r="D694" s="45"/>
-      <c r="E694" s="45"/>
-      <c r="F694" s="45"/>
-      <c r="G694" s="45"/>
+      <c r="B694" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C694" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D694" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E694" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F694" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G694" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H694" s="45"/>
-      <c r="I694" s="45"/>
-      <c r="J694" s="45"/>
+      <c r="I694" s="45">
+        <v>298</v>
+      </c>
+      <c r="J694" s="62">
+        <v>209000000</v>
+      </c>
       <c r="K694" s="45"/>
-      <c r="L694" s="45"/>
-      <c r="M694" s="45"/>
-      <c r="N694" s="45"/>
+      <c r="L694" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M694" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N694" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O694" s="45"/>
       <c r="P694" s="45"/>
       <c r="Q694" s="45"/>
@@ -35954,19 +36144,41 @@
     </row>
     <row r="695" spans="1:20" ht="16" customHeight="1">
       <c r="A695" s="45"/>
-      <c r="B695" s="45"/>
-      <c r="C695" s="45"/>
-      <c r="D695" s="45"/>
-      <c r="E695" s="45"/>
-      <c r="F695" s="45"/>
-      <c r="G695" s="45"/>
+      <c r="B695" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C695" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D695" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E695" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F695" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G695" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H695" s="45"/>
-      <c r="I695" s="45"/>
-      <c r="J695" s="45"/>
+      <c r="I695" s="45">
+        <v>298</v>
+      </c>
+      <c r="J695" s="62">
+        <v>182000000</v>
+      </c>
       <c r="K695" s="45"/>
-      <c r="L695" s="45"/>
-      <c r="M695" s="45"/>
-      <c r="N695" s="45"/>
+      <c r="L695" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M695" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N695" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O695" s="45"/>
       <c r="P695" s="45"/>
       <c r="Q695" s="45"/>
@@ -35976,19 +36188,41 @@
     </row>
     <row r="696" spans="1:20" ht="16" customHeight="1">
       <c r="A696" s="45"/>
-      <c r="B696" s="45"/>
-      <c r="C696" s="45"/>
-      <c r="D696" s="45"/>
-      <c r="E696" s="45"/>
-      <c r="F696" s="45"/>
-      <c r="G696" s="45"/>
+      <c r="B696" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C696" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D696" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E696" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F696" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G696" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H696" s="45"/>
-      <c r="I696" s="45"/>
-      <c r="J696" s="45"/>
+      <c r="I696" s="45">
+        <v>298</v>
+      </c>
+      <c r="J696" s="62">
+        <v>198000000</v>
+      </c>
       <c r="K696" s="45"/>
-      <c r="L696" s="45"/>
-      <c r="M696" s="45"/>
-      <c r="N696" s="45"/>
+      <c r="L696" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M696" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N696" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O696" s="45"/>
       <c r="P696" s="45"/>
       <c r="Q696" s="45"/>
@@ -35998,19 +36232,41 @@
     </row>
     <row r="697" spans="1:20" ht="16" customHeight="1">
       <c r="A697" s="45"/>
-      <c r="B697" s="45"/>
-      <c r="C697" s="45"/>
-      <c r="D697" s="45"/>
-      <c r="E697" s="45"/>
-      <c r="F697" s="45"/>
-      <c r="G697" s="45"/>
+      <c r="B697" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C697" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D697" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E697" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F697" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G697" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H697" s="45"/>
-      <c r="I697" s="45"/>
-      <c r="J697" s="45"/>
+      <c r="I697" s="45">
+        <v>298</v>
+      </c>
+      <c r="J697" s="62">
+        <v>192000000</v>
+      </c>
       <c r="K697" s="45"/>
-      <c r="L697" s="45"/>
-      <c r="M697" s="45"/>
-      <c r="N697" s="45"/>
+      <c r="L697" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M697" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N697" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O697" s="45"/>
       <c r="P697" s="45"/>
       <c r="Q697" s="45"/>
@@ -36020,19 +36276,41 @@
     </row>
     <row r="698" spans="1:20" ht="16" customHeight="1">
       <c r="A698" s="45"/>
-      <c r="B698" s="45"/>
-      <c r="C698" s="45"/>
-      <c r="D698" s="45"/>
-      <c r="E698" s="45"/>
-      <c r="F698" s="45"/>
-      <c r="G698" s="45"/>
+      <c r="B698" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C698" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D698" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E698" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F698" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G698" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H698" s="45"/>
-      <c r="I698" s="45"/>
-      <c r="J698" s="45"/>
+      <c r="I698" s="45">
+        <v>298</v>
+      </c>
+      <c r="J698" s="62">
+        <v>163000000</v>
+      </c>
       <c r="K698" s="45"/>
-      <c r="L698" s="45"/>
-      <c r="M698" s="45"/>
-      <c r="N698" s="45"/>
+      <c r="L698" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M698" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N698" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O698" s="45"/>
       <c r="P698" s="45"/>
       <c r="Q698" s="45"/>
@@ -36042,19 +36320,41 @@
     </row>
     <row r="699" spans="1:20" ht="16" customHeight="1">
       <c r="A699" s="45"/>
-      <c r="B699" s="45"/>
-      <c r="C699" s="45"/>
-      <c r="D699" s="45"/>
-      <c r="E699" s="45"/>
-      <c r="F699" s="45"/>
-      <c r="G699" s="45"/>
+      <c r="B699" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C699" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D699" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E699" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F699" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G699" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H699" s="45"/>
-      <c r="I699" s="45"/>
-      <c r="J699" s="45"/>
+      <c r="I699" s="45">
+        <v>298</v>
+      </c>
+      <c r="J699" s="62">
+        <v>154000000</v>
+      </c>
       <c r="K699" s="45"/>
-      <c r="L699" s="45"/>
-      <c r="M699" s="45"/>
-      <c r="N699" s="45"/>
+      <c r="L699" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M699" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N699" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O699" s="45"/>
       <c r="P699" s="45"/>
       <c r="Q699" s="45"/>
@@ -36064,19 +36364,41 @@
     </row>
     <row r="700" spans="1:20" ht="16" customHeight="1">
       <c r="A700" s="45"/>
-      <c r="B700" s="45"/>
-      <c r="C700" s="45"/>
-      <c r="D700" s="45"/>
-      <c r="E700" s="45"/>
-      <c r="F700" s="45"/>
-      <c r="G700" s="45"/>
+      <c r="B700" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C700" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D700" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E700" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F700" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G700" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H700" s="45"/>
-      <c r="I700" s="45"/>
-      <c r="J700" s="45"/>
+      <c r="I700" s="45">
+        <v>298</v>
+      </c>
+      <c r="J700" s="62">
+        <v>700000000</v>
+      </c>
       <c r="K700" s="45"/>
-      <c r="L700" s="45"/>
-      <c r="M700" s="45"/>
-      <c r="N700" s="45"/>
+      <c r="L700" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M700" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N700" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O700" s="45"/>
       <c r="P700" s="45"/>
       <c r="Q700" s="45"/>
@@ -36086,19 +36408,41 @@
     </row>
     <row r="701" spans="1:20" ht="16" customHeight="1">
       <c r="A701" s="45"/>
-      <c r="B701" s="45"/>
-      <c r="C701" s="45"/>
-      <c r="D701" s="45"/>
-      <c r="E701" s="45"/>
-      <c r="F701" s="45"/>
-      <c r="G701" s="45"/>
+      <c r="B701" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C701" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D701" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E701" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F701" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G701" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H701" s="45"/>
-      <c r="I701" s="45"/>
-      <c r="J701" s="45"/>
+      <c r="I701" s="45">
+        <v>298</v>
+      </c>
+      <c r="J701" s="62">
+        <v>627000000</v>
+      </c>
       <c r="K701" s="45"/>
-      <c r="L701" s="45"/>
-      <c r="M701" s="45"/>
-      <c r="N701" s="45"/>
+      <c r="L701" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M701" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N701" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O701" s="45"/>
       <c r="P701" s="45"/>
       <c r="Q701" s="45"/>
@@ -36108,19 +36452,41 @@
     </row>
     <row r="702" spans="1:20" ht="16" customHeight="1">
       <c r="A702" s="45"/>
-      <c r="B702" s="45"/>
-      <c r="C702" s="45"/>
-      <c r="D702" s="45"/>
-      <c r="E702" s="45"/>
-      <c r="F702" s="45"/>
-      <c r="G702" s="45"/>
+      <c r="B702" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C702" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D702" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E702" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F702" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G702" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H702" s="45"/>
-      <c r="I702" s="45"/>
-      <c r="J702" s="45"/>
+      <c r="I702" s="45">
+        <v>298</v>
+      </c>
+      <c r="J702" s="62">
+        <v>626000000</v>
+      </c>
       <c r="K702" s="45"/>
-      <c r="L702" s="45"/>
-      <c r="M702" s="45"/>
-      <c r="N702" s="45"/>
+      <c r="L702" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M702" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N702" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O702" s="45"/>
       <c r="P702" s="45"/>
       <c r="Q702" s="45"/>
@@ -36130,19 +36496,41 @@
     </row>
     <row r="703" spans="1:20" ht="16" customHeight="1">
       <c r="A703" s="45"/>
-      <c r="B703" s="45"/>
-      <c r="C703" s="45"/>
-      <c r="D703" s="45"/>
-      <c r="E703" s="45"/>
-      <c r="F703" s="45"/>
-      <c r="G703" s="45"/>
+      <c r="B703" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C703" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D703" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E703" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="F703" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G703" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H703" s="45"/>
-      <c r="I703" s="45"/>
-      <c r="J703" s="45"/>
+      <c r="I703" s="45">
+        <v>298</v>
+      </c>
+      <c r="J703" s="62">
+        <v>644000000</v>
+      </c>
       <c r="K703" s="45"/>
-      <c r="L703" s="45"/>
-      <c r="M703" s="45"/>
-      <c r="N703" s="45"/>
+      <c r="L703" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M703" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N703" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O703" s="45"/>
       <c r="P703" s="45"/>
       <c r="Q703" s="45"/>
@@ -36152,19 +36540,41 @@
     </row>
     <row r="704" spans="1:20" ht="16" customHeight="1">
       <c r="A704" s="45"/>
-      <c r="B704" s="45"/>
-      <c r="C704" s="45"/>
-      <c r="D704" s="45"/>
-      <c r="E704" s="45"/>
-      <c r="F704" s="45"/>
-      <c r="G704" s="45"/>
+      <c r="B704" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C704" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D704" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E704" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F704" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G704" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H704" s="45"/>
-      <c r="I704" s="45"/>
-      <c r="J704" s="45"/>
+      <c r="I704" s="45">
+        <v>298</v>
+      </c>
+      <c r="J704" s="62">
+        <v>619000000</v>
+      </c>
       <c r="K704" s="45"/>
-      <c r="L704" s="45"/>
-      <c r="M704" s="45"/>
-      <c r="N704" s="45"/>
+      <c r="L704" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M704" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N704" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O704" s="45"/>
       <c r="P704" s="45"/>
       <c r="Q704" s="45"/>
@@ -36174,19 +36584,41 @@
     </row>
     <row r="705" spans="1:20" ht="16" customHeight="1">
       <c r="A705" s="45"/>
-      <c r="B705" s="45"/>
-      <c r="C705" s="45"/>
-      <c r="D705" s="45"/>
-      <c r="E705" s="45"/>
-      <c r="F705" s="45"/>
-      <c r="G705" s="45"/>
+      <c r="B705" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C705" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D705" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E705" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F705" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G705" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H705" s="45"/>
-      <c r="I705" s="45"/>
-      <c r="J705" s="45"/>
+      <c r="I705" s="45">
+        <v>298</v>
+      </c>
+      <c r="J705" s="62">
+        <v>561000000</v>
+      </c>
       <c r="K705" s="45"/>
-      <c r="L705" s="45"/>
-      <c r="M705" s="45"/>
-      <c r="N705" s="45"/>
+      <c r="L705" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M705" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N705" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O705" s="45"/>
       <c r="P705" s="45"/>
       <c r="Q705" s="45"/>
@@ -36196,19 +36628,41 @@
     </row>
     <row r="706" spans="1:20" ht="16" customHeight="1">
       <c r="A706" s="45"/>
-      <c r="B706" s="45"/>
-      <c r="C706" s="45"/>
-      <c r="D706" s="45"/>
-      <c r="E706" s="45"/>
-      <c r="F706" s="45"/>
-      <c r="G706" s="45"/>
+      <c r="B706" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C706" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D706" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E706" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F706" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G706" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H706" s="45"/>
-      <c r="I706" s="45"/>
-      <c r="J706" s="45"/>
+      <c r="I706" s="45">
+        <v>298</v>
+      </c>
+      <c r="J706" s="62">
+        <v>576000000</v>
+      </c>
       <c r="K706" s="45"/>
-      <c r="L706" s="45"/>
-      <c r="M706" s="45"/>
-      <c r="N706" s="45"/>
+      <c r="L706" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M706" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N706" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O706" s="45"/>
       <c r="P706" s="45"/>
       <c r="Q706" s="45"/>
@@ -36218,19 +36672,41 @@
     </row>
     <row r="707" spans="1:20" ht="16" customHeight="1">
       <c r="A707" s="45"/>
-      <c r="B707" s="45"/>
-      <c r="C707" s="45"/>
-      <c r="D707" s="45"/>
-      <c r="E707" s="45"/>
-      <c r="F707" s="45"/>
-      <c r="G707" s="45"/>
+      <c r="B707" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C707" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D707" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E707" s="61" t="s">
+        <v>507</v>
+      </c>
+      <c r="F707" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G707" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H707" s="45"/>
-      <c r="I707" s="45"/>
-      <c r="J707" s="45"/>
+      <c r="I707" s="45">
+        <v>298</v>
+      </c>
+      <c r="J707" s="62">
+        <v>583000000</v>
+      </c>
       <c r="K707" s="45"/>
-      <c r="L707" s="45"/>
-      <c r="M707" s="45"/>
-      <c r="N707" s="45"/>
+      <c r="L707" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M707" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N707" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O707" s="45"/>
       <c r="P707" s="45"/>
       <c r="Q707" s="45"/>
@@ -36240,19 +36716,41 @@
     </row>
     <row r="708" spans="1:20" ht="16" customHeight="1">
       <c r="A708" s="45"/>
-      <c r="B708" s="45"/>
-      <c r="C708" s="45"/>
-      <c r="D708" s="45"/>
-      <c r="E708" s="45"/>
-      <c r="F708" s="45"/>
-      <c r="G708" s="45"/>
+      <c r="B708" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C708" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D708" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E708" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F708" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G708" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H708" s="45"/>
-      <c r="I708" s="45"/>
-      <c r="J708" s="45"/>
+      <c r="I708" s="45">
+        <v>298</v>
+      </c>
+      <c r="J708" s="62">
+        <v>564000000</v>
+      </c>
       <c r="K708" s="45"/>
-      <c r="L708" s="45"/>
-      <c r="M708" s="45"/>
-      <c r="N708" s="45"/>
+      <c r="L708" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M708" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N708" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O708" s="45"/>
       <c r="P708" s="45"/>
       <c r="Q708" s="45"/>
@@ -36262,19 +36760,41 @@
     </row>
     <row r="709" spans="1:20" ht="16" customHeight="1">
       <c r="A709" s="45"/>
-      <c r="B709" s="45"/>
-      <c r="C709" s="45"/>
-      <c r="D709" s="45"/>
-      <c r="E709" s="45"/>
-      <c r="F709" s="45"/>
-      <c r="G709" s="45"/>
+      <c r="B709" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C709" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D709" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E709" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F709" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G709" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H709" s="45"/>
-      <c r="I709" s="45"/>
-      <c r="J709" s="45"/>
+      <c r="I709" s="45">
+        <v>298</v>
+      </c>
+      <c r="J709" s="62">
+        <v>537000000</v>
+      </c>
       <c r="K709" s="45"/>
-      <c r="L709" s="45"/>
-      <c r="M709" s="45"/>
-      <c r="N709" s="45"/>
+      <c r="L709" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M709" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N709" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O709" s="45"/>
       <c r="P709" s="45"/>
       <c r="Q709" s="45"/>
@@ -36284,19 +36804,41 @@
     </row>
     <row r="710" spans="1:20" ht="16" customHeight="1">
       <c r="A710" s="45"/>
-      <c r="B710" s="45"/>
-      <c r="C710" s="45"/>
-      <c r="D710" s="45"/>
-      <c r="E710" s="45"/>
-      <c r="F710" s="45"/>
-      <c r="G710" s="45"/>
+      <c r="B710" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C710" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D710" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E710" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F710" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G710" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H710" s="45"/>
-      <c r="I710" s="45"/>
-      <c r="J710" s="45"/>
+      <c r="I710" s="45">
+        <v>298</v>
+      </c>
+      <c r="J710" s="62">
+        <v>539000000</v>
+      </c>
       <c r="K710" s="45"/>
-      <c r="L710" s="45"/>
-      <c r="M710" s="45"/>
-      <c r="N710" s="45"/>
+      <c r="L710" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M710" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N710" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O710" s="45"/>
       <c r="P710" s="45"/>
       <c r="Q710" s="45"/>
@@ -36306,19 +36848,41 @@
     </row>
     <row r="711" spans="1:20" ht="16" customHeight="1">
       <c r="A711" s="45"/>
-      <c r="B711" s="45"/>
-      <c r="C711" s="45"/>
-      <c r="D711" s="45"/>
-      <c r="E711" s="45"/>
-      <c r="F711" s="45"/>
-      <c r="G711" s="45"/>
+      <c r="B711" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C711" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D711" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E711" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F711" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="G711" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H711" s="45"/>
-      <c r="I711" s="45"/>
-      <c r="J711" s="45"/>
+      <c r="I711" s="45">
+        <v>298</v>
+      </c>
+      <c r="J711" s="62">
+        <v>561000000</v>
+      </c>
       <c r="K711" s="45"/>
-      <c r="L711" s="45"/>
-      <c r="M711" s="45"/>
-      <c r="N711" s="45"/>
+      <c r="L711" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M711" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N711" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O711" s="45"/>
       <c r="P711" s="45"/>
       <c r="Q711" s="45"/>
@@ -36328,19 +36892,41 @@
     </row>
     <row r="712" spans="1:20" ht="16" customHeight="1">
       <c r="A712" s="45"/>
-      <c r="B712" s="45"/>
-      <c r="C712" s="45"/>
-      <c r="D712" s="45"/>
-      <c r="E712" s="45"/>
-      <c r="F712" s="45"/>
-      <c r="G712" s="45"/>
+      <c r="B712" s="104" t="s">
+        <v>500</v>
+      </c>
+      <c r="C712" s="105" t="s">
+        <v>74</v>
+      </c>
+      <c r="D712" s="105" t="s">
+        <v>504</v>
+      </c>
+      <c r="E712" s="105" t="s">
+        <v>505</v>
+      </c>
+      <c r="F712" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G712" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H712" s="45"/>
-      <c r="I712" s="45"/>
-      <c r="J712" s="45"/>
+      <c r="I712" s="45">
+        <v>298</v>
+      </c>
+      <c r="J712" s="45">
+        <v>43.8</v>
+      </c>
       <c r="K712" s="45"/>
-      <c r="L712" s="45"/>
-      <c r="M712" s="45"/>
-      <c r="N712" s="45"/>
+      <c r="L712" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M712" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N712" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O712" s="45"/>
       <c r="P712" s="45"/>
       <c r="Q712" s="45"/>
@@ -36350,19 +36936,41 @@
     </row>
     <row r="713" spans="1:20" ht="16" customHeight="1">
       <c r="A713" s="45"/>
-      <c r="B713" s="45"/>
-      <c r="C713" s="45"/>
-      <c r="D713" s="45"/>
-      <c r="E713" s="45"/>
-      <c r="F713" s="45"/>
-      <c r="G713" s="45"/>
+      <c r="B713" s="106" t="s">
+        <v>501</v>
+      </c>
+      <c r="C713" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D713" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E713" s="107" t="s">
+        <v>505</v>
+      </c>
+      <c r="F713" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G713" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H713" s="45"/>
-      <c r="I713" s="45"/>
-      <c r="J713" s="45"/>
+      <c r="I713" s="45">
+        <v>298</v>
+      </c>
+      <c r="J713" s="45">
+        <v>56.4</v>
+      </c>
       <c r="K713" s="45"/>
-      <c r="L713" s="45"/>
-      <c r="M713" s="45"/>
-      <c r="N713" s="45"/>
+      <c r="L713" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M713" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N713" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O713" s="45"/>
       <c r="P713" s="45"/>
       <c r="Q713" s="45"/>
@@ -36372,19 +36980,41 @@
     </row>
     <row r="714" spans="1:20" ht="16" customHeight="1">
       <c r="A714" s="45"/>
-      <c r="B714" s="45"/>
-      <c r="C714" s="45"/>
-      <c r="D714" s="45"/>
-      <c r="E714" s="45"/>
-      <c r="F714" s="45"/>
-      <c r="G714" s="45"/>
+      <c r="B714" s="106" t="s">
+        <v>502</v>
+      </c>
+      <c r="C714" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D714" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E714" s="107" t="s">
+        <v>505</v>
+      </c>
+      <c r="F714" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G714" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H714" s="45"/>
-      <c r="I714" s="45"/>
-      <c r="J714" s="45"/>
+      <c r="I714" s="45">
+        <v>298</v>
+      </c>
+      <c r="J714" s="45">
+        <v>60.3</v>
+      </c>
       <c r="K714" s="45"/>
-      <c r="L714" s="45"/>
-      <c r="M714" s="45"/>
-      <c r="N714" s="45"/>
+      <c r="L714" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M714" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N714" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O714" s="45"/>
       <c r="P714" s="45"/>
       <c r="Q714" s="45"/>
@@ -36394,19 +37024,41 @@
     </row>
     <row r="715" spans="1:20" ht="16" customHeight="1">
       <c r="A715" s="45"/>
-      <c r="B715" s="45"/>
-      <c r="C715" s="45"/>
-      <c r="D715" s="45"/>
-      <c r="E715" s="45"/>
-      <c r="F715" s="45"/>
-      <c r="G715" s="45"/>
+      <c r="B715" s="106" t="s">
+        <v>503</v>
+      </c>
+      <c r="C715" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D715" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E715" s="107" t="s">
+        <v>505</v>
+      </c>
+      <c r="F715" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G715" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H715" s="45"/>
-      <c r="I715" s="45"/>
-      <c r="J715" s="45"/>
+      <c r="I715" s="45">
+        <v>298</v>
+      </c>
+      <c r="J715" s="62">
+        <v>67.599999999999994</v>
+      </c>
       <c r="K715" s="45"/>
-      <c r="L715" s="45"/>
-      <c r="M715" s="45"/>
-      <c r="N715" s="45"/>
+      <c r="L715" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M715" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N715" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O715" s="45"/>
       <c r="P715" s="45"/>
       <c r="Q715" s="45"/>
@@ -36416,19 +37068,41 @@
     </row>
     <row r="716" spans="1:20" ht="16" customHeight="1">
       <c r="A716" s="45"/>
-      <c r="B716" s="45"/>
-      <c r="C716" s="45"/>
-      <c r="D716" s="45"/>
-      <c r="E716" s="45"/>
-      <c r="F716" s="45"/>
-      <c r="G716" s="45"/>
+      <c r="B716" s="106" t="s">
+        <v>500</v>
+      </c>
+      <c r="C716" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D716" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E716" s="107" t="s">
+        <v>507</v>
+      </c>
+      <c r="F716" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G716" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H716" s="45"/>
-      <c r="I716" s="45"/>
-      <c r="J716" s="45"/>
+      <c r="I716" s="45">
+        <v>298</v>
+      </c>
+      <c r="J716" s="45">
+        <v>53.9</v>
+      </c>
       <c r="K716" s="45"/>
-      <c r="L716" s="45"/>
-      <c r="M716" s="45"/>
-      <c r="N716" s="45"/>
+      <c r="L716" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M716" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N716" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O716" s="45"/>
       <c r="P716" s="45"/>
       <c r="Q716" s="45"/>
@@ -36438,19 +37112,41 @@
     </row>
     <row r="717" spans="1:20" ht="16" customHeight="1">
       <c r="A717" s="45"/>
-      <c r="B717" s="45"/>
-      <c r="C717" s="45"/>
-      <c r="D717" s="45"/>
-      <c r="E717" s="45"/>
-      <c r="F717" s="45"/>
-      <c r="G717" s="45"/>
+      <c r="B717" s="106" t="s">
+        <v>501</v>
+      </c>
+      <c r="C717" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D717" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E717" s="107" t="s">
+        <v>507</v>
+      </c>
+      <c r="F717" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G717" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H717" s="45"/>
-      <c r="I717" s="45"/>
-      <c r="J717" s="45"/>
+      <c r="I717" s="45">
+        <v>298</v>
+      </c>
+      <c r="J717" s="45">
+        <v>58.5</v>
+      </c>
       <c r="K717" s="45"/>
-      <c r="L717" s="45"/>
-      <c r="M717" s="45"/>
-      <c r="N717" s="45"/>
+      <c r="L717" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M717" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N717" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O717" s="45"/>
       <c r="P717" s="45"/>
       <c r="Q717" s="45"/>
@@ -36460,19 +37156,41 @@
     </row>
     <row r="718" spans="1:20" ht="16" customHeight="1">
       <c r="A718" s="45"/>
-      <c r="B718" s="45"/>
-      <c r="C718" s="45"/>
-      <c r="D718" s="45"/>
-      <c r="E718" s="45"/>
-      <c r="F718" s="45"/>
-      <c r="G718" s="45"/>
+      <c r="B718" s="106" t="s">
+        <v>502</v>
+      </c>
+      <c r="C718" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D718" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E718" s="107" t="s">
+        <v>507</v>
+      </c>
+      <c r="F718" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G718" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H718" s="45"/>
-      <c r="I718" s="45"/>
-      <c r="J718" s="45"/>
+      <c r="I718" s="45">
+        <v>298</v>
+      </c>
+      <c r="J718" s="45">
+        <v>70.099999999999994</v>
+      </c>
       <c r="K718" s="45"/>
-      <c r="L718" s="45"/>
-      <c r="M718" s="45"/>
-      <c r="N718" s="45"/>
+      <c r="L718" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M718" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N718" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O718" s="45"/>
       <c r="P718" s="45"/>
       <c r="Q718" s="45"/>
@@ -36482,19 +37200,41 @@
     </row>
     <row r="719" spans="1:20" ht="16" customHeight="1">
       <c r="A719" s="45"/>
-      <c r="B719" s="45"/>
-      <c r="C719" s="45"/>
-      <c r="D719" s="45"/>
-      <c r="E719" s="45"/>
-      <c r="F719" s="45"/>
-      <c r="G719" s="45"/>
+      <c r="B719" s="106" t="s">
+        <v>503</v>
+      </c>
+      <c r="C719" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D719" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E719" s="107" t="s">
+        <v>507</v>
+      </c>
+      <c r="F719" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G719" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H719" s="45"/>
-      <c r="I719" s="45"/>
-      <c r="J719" s="45"/>
+      <c r="I719" s="45">
+        <v>298</v>
+      </c>
+      <c r="J719" s="45">
+        <v>80.2</v>
+      </c>
       <c r="K719" s="45"/>
-      <c r="L719" s="45"/>
-      <c r="M719" s="45"/>
-      <c r="N719" s="45"/>
+      <c r="L719" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M719" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N719" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O719" s="45"/>
       <c r="P719" s="45"/>
       <c r="Q719" s="45"/>
@@ -36504,19 +37244,41 @@
     </row>
     <row r="720" spans="1:20" ht="16" customHeight="1">
       <c r="A720" s="45"/>
-      <c r="B720" s="45"/>
-      <c r="C720" s="45"/>
-      <c r="D720" s="45"/>
-      <c r="E720" s="45"/>
-      <c r="F720" s="45"/>
-      <c r="G720" s="45"/>
+      <c r="B720" s="106" t="s">
+        <v>500</v>
+      </c>
+      <c r="C720" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D720" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E720" s="107" t="s">
+        <v>506</v>
+      </c>
+      <c r="F720" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G720" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H720" s="45"/>
-      <c r="I720" s="45"/>
-      <c r="J720" s="45"/>
+      <c r="I720" s="45">
+        <v>298</v>
+      </c>
+      <c r="J720" s="45">
+        <v>61.3</v>
+      </c>
       <c r="K720" s="45"/>
-      <c r="L720" s="45"/>
-      <c r="M720" s="45"/>
-      <c r="N720" s="45"/>
+      <c r="L720" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M720" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N720" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O720" s="45"/>
       <c r="P720" s="45"/>
       <c r="Q720" s="45"/>
@@ -36526,19 +37288,41 @@
     </row>
     <row r="721" spans="1:20" ht="16" customHeight="1">
       <c r="A721" s="45"/>
-      <c r="B721" s="45"/>
-      <c r="C721" s="45"/>
-      <c r="D721" s="45"/>
-      <c r="E721" s="45"/>
-      <c r="F721" s="45"/>
-      <c r="G721" s="45"/>
+      <c r="B721" s="106" t="s">
+        <v>501</v>
+      </c>
+      <c r="C721" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D721" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E721" s="107" t="s">
+        <v>506</v>
+      </c>
+      <c r="F721" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G721" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H721" s="45"/>
-      <c r="I721" s="45"/>
-      <c r="J721" s="45"/>
+      <c r="I721" s="45">
+        <v>298</v>
+      </c>
+      <c r="J721" s="45">
+        <v>69.599999999999994</v>
+      </c>
       <c r="K721" s="45"/>
-      <c r="L721" s="45"/>
-      <c r="M721" s="45"/>
-      <c r="N721" s="45"/>
+      <c r="L721" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M721" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N721" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O721" s="45"/>
       <c r="P721" s="45"/>
       <c r="Q721" s="45"/>
@@ -36548,19 +37332,41 @@
     </row>
     <row r="722" spans="1:20" ht="16" customHeight="1">
       <c r="A722" s="45"/>
-      <c r="B722" s="45"/>
-      <c r="C722" s="45"/>
-      <c r="D722" s="45"/>
-      <c r="E722" s="45"/>
-      <c r="F722" s="45"/>
-      <c r="G722" s="45"/>
+      <c r="B722" s="106" t="s">
+        <v>502</v>
+      </c>
+      <c r="C722" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D722" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E722" s="107" t="s">
+        <v>506</v>
+      </c>
+      <c r="F722" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G722" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H722" s="45"/>
-      <c r="I722" s="45"/>
-      <c r="J722" s="45"/>
+      <c r="I722" s="45">
+        <v>298</v>
+      </c>
+      <c r="J722" s="45">
+        <v>71.400000000000006</v>
+      </c>
       <c r="K722" s="45"/>
-      <c r="L722" s="45"/>
-      <c r="M722" s="45"/>
-      <c r="N722" s="45"/>
+      <c r="L722" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M722" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N722" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O722" s="45"/>
       <c r="P722" s="45"/>
       <c r="Q722" s="45"/>
@@ -36570,19 +37376,41 @@
     </row>
     <row r="723" spans="1:20" ht="16" customHeight="1">
       <c r="A723" s="45"/>
-      <c r="B723" s="45"/>
-      <c r="C723" s="45"/>
-      <c r="D723" s="45"/>
-      <c r="E723" s="45"/>
-      <c r="F723" s="45"/>
-      <c r="G723" s="45"/>
+      <c r="B723" s="106" t="s">
+        <v>503</v>
+      </c>
+      <c r="C723" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="D723" s="107" t="s">
+        <v>504</v>
+      </c>
+      <c r="E723" s="107" t="s">
+        <v>506</v>
+      </c>
+      <c r="F723" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G723" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H723" s="45"/>
-      <c r="I723" s="45"/>
-      <c r="J723" s="45"/>
+      <c r="I723" s="45">
+        <v>298</v>
+      </c>
+      <c r="J723" s="45">
+        <v>75.8</v>
+      </c>
       <c r="K723" s="45"/>
-      <c r="L723" s="45"/>
-      <c r="M723" s="45"/>
-      <c r="N723" s="45"/>
+      <c r="L723" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="M723" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="N723" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O723" s="45"/>
       <c r="P723" s="45"/>
       <c r="Q723" s="45"/>
@@ -36592,19 +37420,41 @@
     </row>
     <row r="724" spans="1:20" ht="16" customHeight="1">
       <c r="A724" s="45"/>
-      <c r="B724" s="45"/>
-      <c r="C724" s="45"/>
-      <c r="D724" s="45"/>
-      <c r="E724" s="45"/>
-      <c r="F724" s="45"/>
-      <c r="G724" s="45"/>
+      <c r="B724" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C724" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D724" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E724" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F724" s="61" t="s">
+        <v>509</v>
+      </c>
+      <c r="G724" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H724" s="45"/>
-      <c r="I724" s="45"/>
-      <c r="J724" s="45"/>
+      <c r="I724" s="45">
+        <v>298</v>
+      </c>
+      <c r="J724" s="62">
+        <v>491000000000</v>
+      </c>
       <c r="K724" s="45"/>
-      <c r="L724" s="45"/>
-      <c r="M724" s="45"/>
-      <c r="N724" s="45"/>
+      <c r="L724" s="61" t="s">
+        <v>510</v>
+      </c>
+      <c r="M724" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N724" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O724" s="45"/>
       <c r="P724" s="45"/>
       <c r="Q724" s="45"/>
@@ -36614,19 +37464,41 @@
     </row>
     <row r="725" spans="1:20" ht="16" customHeight="1">
       <c r="A725" s="45"/>
-      <c r="B725" s="45"/>
-      <c r="C725" s="45"/>
-      <c r="D725" s="45"/>
-      <c r="E725" s="45"/>
-      <c r="F725" s="45"/>
-      <c r="G725" s="45"/>
+      <c r="B725" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C725" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D725" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E725" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F725" s="61" t="s">
+        <v>509</v>
+      </c>
+      <c r="G725" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H725" s="45"/>
-      <c r="I725" s="45"/>
-      <c r="J725" s="45"/>
+      <c r="I725" s="45">
+        <v>298</v>
+      </c>
+      <c r="J725" s="62">
+        <v>302000000000</v>
+      </c>
       <c r="K725" s="45"/>
-      <c r="L725" s="45"/>
-      <c r="M725" s="45"/>
-      <c r="N725" s="45"/>
+      <c r="L725" s="61" t="s">
+        <v>510</v>
+      </c>
+      <c r="M725" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N725" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O725" s="45"/>
       <c r="P725" s="45"/>
       <c r="Q725" s="45"/>
@@ -36636,19 +37508,41 @@
     </row>
     <row r="726" spans="1:20" ht="16" customHeight="1">
       <c r="A726" s="45"/>
-      <c r="B726" s="45"/>
-      <c r="C726" s="45"/>
-      <c r="D726" s="45"/>
-      <c r="E726" s="45"/>
-      <c r="F726" s="45"/>
-      <c r="G726" s="45"/>
+      <c r="B726" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C726" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D726" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E726" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F726" s="61" t="s">
+        <v>509</v>
+      </c>
+      <c r="G726" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H726" s="45"/>
-      <c r="I726" s="45"/>
-      <c r="J726" s="45"/>
+      <c r="I726" s="45">
+        <v>298</v>
+      </c>
+      <c r="J726" s="62">
+        <v>268000000000</v>
+      </c>
       <c r="K726" s="45"/>
-      <c r="L726" s="45"/>
-      <c r="M726" s="45"/>
-      <c r="N726" s="45"/>
+      <c r="L726" s="61" t="s">
+        <v>510</v>
+      </c>
+      <c r="M726" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N726" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O726" s="45"/>
       <c r="P726" s="45"/>
       <c r="Q726" s="45"/>
@@ -36658,19 +37552,41 @@
     </row>
     <row r="727" spans="1:20" ht="16" customHeight="1">
       <c r="A727" s="45"/>
-      <c r="B727" s="45"/>
-      <c r="C727" s="45"/>
-      <c r="D727" s="45"/>
-      <c r="E727" s="45"/>
-      <c r="F727" s="45"/>
-      <c r="G727" s="45"/>
+      <c r="B727" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C727" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D727" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E727" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F727" s="61" t="s">
+        <v>509</v>
+      </c>
+      <c r="G727" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H727" s="45"/>
-      <c r="I727" s="45"/>
-      <c r="J727" s="45"/>
+      <c r="I727" s="45">
+        <v>298</v>
+      </c>
+      <c r="J727" s="62">
+        <v>208000000000</v>
+      </c>
       <c r="K727" s="45"/>
-      <c r="L727" s="45"/>
-      <c r="M727" s="45"/>
-      <c r="N727" s="45"/>
+      <c r="L727" s="61" t="s">
+        <v>510</v>
+      </c>
+      <c r="M727" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N727" s="61" t="s">
+        <v>511</v>
+      </c>
       <c r="O727" s="45"/>
       <c r="P727" s="45"/>
       <c r="Q727" s="45"/>

</xml_diff>

<commit_message>
- extracted extra data from some older papers and `10.1016/j.intermet.2021.107239`
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7441E9E0-AD08-C648-93A6-85551015DF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4FFED6-940E-2045-A2AD-E52B843C98EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="5720" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="7380" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6709" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6774" uniqueCount="523">
   <si>
     <r>
       <rPr>
@@ -1718,13 +1718,46 @@
     <t>homogenized at 1273K for 24h and cold rolled with 90% reduction to achieve initial alloy; hall-petch coefficients derived from fidderent annealing conditions</t>
   </si>
   <si>
-    <t>hall-petch coefficient</t>
-  </si>
-  <si>
-    <t>Pa/m^0.5</t>
-  </si>
-  <si>
     <t>10.1016/j.intermet.2021.107239</t>
+  </si>
+  <si>
+    <t>Pa m^0.5</t>
+  </si>
+  <si>
+    <t>tensile hall-petch coefficient</t>
+  </si>
+  <si>
+    <t>tensile friction stress</t>
+  </si>
+  <si>
+    <t>AuCuNiPdPt</t>
+  </si>
+  <si>
+    <t>AAM+H+WQ+RX+WQ</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 1100*C for 20h and water quenched  then deformed by rotary swaging to 0.6 true strain then recrystallized at 1100*C for 1h and water quenched</t>
+  </si>
+  <si>
+    <t>P409</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2019.12.020</t>
+  </si>
+  <si>
+    <t>Au25 (CuPdPt)25</t>
+  </si>
+  <si>
+    <t>after arc melting samples were homogenized at 0.9 homologous temperature and water quenched then deformed by rotary swaging to 0.71 true strain then recrystallized at 0.9 homologous temperature and water quenched</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2024.175273</t>
+  </si>
+  <si>
+    <t>Ni10 Pt15 (AuCuPd)25</t>
+  </si>
+  <si>
+    <t>compressive friction stress</t>
   </si>
 </sst>
 </file>
@@ -2764,7 +2797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3079,6 +3112,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4241,8 +4275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C694" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O714" sqref="O714"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A719" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J740" sqref="J740"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -35869,7 +35903,7 @@
         <v>126</v>
       </c>
       <c r="N688" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O688" s="45"/>
       <c r="P688" s="45"/>
@@ -35913,7 +35947,7 @@
         <v>126</v>
       </c>
       <c r="N689" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O689" s="45"/>
       <c r="P689" s="45"/>
@@ -35957,7 +35991,7 @@
         <v>126</v>
       </c>
       <c r="N690" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O690" s="45"/>
       <c r="P690" s="45"/>
@@ -36001,7 +36035,7 @@
         <v>126</v>
       </c>
       <c r="N691" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O691" s="45"/>
       <c r="P691" s="45"/>
@@ -36045,7 +36079,7 @@
         <v>126</v>
       </c>
       <c r="N692" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O692" s="45"/>
       <c r="P692" s="45"/>
@@ -36089,7 +36123,7 @@
         <v>126</v>
       </c>
       <c r="N693" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O693" s="45"/>
       <c r="P693" s="45"/>
@@ -36133,7 +36167,7 @@
         <v>126</v>
       </c>
       <c r="N694" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O694" s="45"/>
       <c r="P694" s="45"/>
@@ -36177,7 +36211,7 @@
         <v>126</v>
       </c>
       <c r="N695" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O695" s="45"/>
       <c r="P695" s="45"/>
@@ -36221,7 +36255,7 @@
         <v>126</v>
       </c>
       <c r="N696" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O696" s="45"/>
       <c r="P696" s="45"/>
@@ -36265,7 +36299,7 @@
         <v>126</v>
       </c>
       <c r="N697" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O697" s="45"/>
       <c r="P697" s="45"/>
@@ -36309,7 +36343,7 @@
         <v>126</v>
       </c>
       <c r="N698" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O698" s="45"/>
       <c r="P698" s="45"/>
@@ -36353,7 +36387,7 @@
         <v>126</v>
       </c>
       <c r="N699" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O699" s="45"/>
       <c r="P699" s="45"/>
@@ -36397,7 +36431,7 @@
         <v>126</v>
       </c>
       <c r="N700" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O700" s="45"/>
       <c r="P700" s="45"/>
@@ -36441,7 +36475,7 @@
         <v>126</v>
       </c>
       <c r="N701" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O701" s="45"/>
       <c r="P701" s="45"/>
@@ -36485,7 +36519,7 @@
         <v>126</v>
       </c>
       <c r="N702" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O702" s="45"/>
       <c r="P702" s="45"/>
@@ -36529,7 +36563,7 @@
         <v>126</v>
       </c>
       <c r="N703" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O703" s="45"/>
       <c r="P703" s="45"/>
@@ -36573,7 +36607,7 @@
         <v>126</v>
       </c>
       <c r="N704" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O704" s="45"/>
       <c r="P704" s="45"/>
@@ -36617,7 +36651,7 @@
         <v>126</v>
       </c>
       <c r="N705" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O705" s="45"/>
       <c r="P705" s="45"/>
@@ -36661,7 +36695,7 @@
         <v>126</v>
       </c>
       <c r="N706" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O706" s="45"/>
       <c r="P706" s="45"/>
@@ -36705,7 +36739,7 @@
         <v>126</v>
       </c>
       <c r="N707" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O707" s="45"/>
       <c r="P707" s="45"/>
@@ -36749,7 +36783,7 @@
         <v>126</v>
       </c>
       <c r="N708" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O708" s="45"/>
       <c r="P708" s="45"/>
@@ -36793,7 +36827,7 @@
         <v>126</v>
       </c>
       <c r="N709" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O709" s="45"/>
       <c r="P709" s="45"/>
@@ -36837,7 +36871,7 @@
         <v>126</v>
       </c>
       <c r="N710" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O710" s="45"/>
       <c r="P710" s="45"/>
@@ -36881,7 +36915,7 @@
         <v>126</v>
       </c>
       <c r="N711" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O711" s="45"/>
       <c r="P711" s="45"/>
@@ -36925,7 +36959,7 @@
         <v>126</v>
       </c>
       <c r="N712" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O712" s="45"/>
       <c r="P712" s="45"/>
@@ -36969,7 +37003,7 @@
         <v>126</v>
       </c>
       <c r="N713" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O713" s="45"/>
       <c r="P713" s="45"/>
@@ -37013,7 +37047,7 @@
         <v>126</v>
       </c>
       <c r="N714" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O714" s="45"/>
       <c r="P714" s="45"/>
@@ -37057,7 +37091,7 @@
         <v>126</v>
       </c>
       <c r="N715" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O715" s="45"/>
       <c r="P715" s="45"/>
@@ -37101,7 +37135,7 @@
         <v>126</v>
       </c>
       <c r="N716" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O716" s="45"/>
       <c r="P716" s="45"/>
@@ -37145,7 +37179,7 @@
         <v>126</v>
       </c>
       <c r="N717" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O717" s="45"/>
       <c r="P717" s="45"/>
@@ -37189,7 +37223,7 @@
         <v>126</v>
       </c>
       <c r="N718" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O718" s="45"/>
       <c r="P718" s="45"/>
@@ -37233,7 +37267,7 @@
         <v>126</v>
       </c>
       <c r="N719" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O719" s="45"/>
       <c r="P719" s="45"/>
@@ -37277,7 +37311,7 @@
         <v>126</v>
       </c>
       <c r="N720" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O720" s="45"/>
       <c r="P720" s="45"/>
@@ -37321,7 +37355,7 @@
         <v>126</v>
       </c>
       <c r="N721" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O721" s="45"/>
       <c r="P721" s="45"/>
@@ -37365,7 +37399,7 @@
         <v>126</v>
       </c>
       <c r="N722" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O722" s="45"/>
       <c r="P722" s="45"/>
@@ -37409,7 +37443,7 @@
         <v>126</v>
       </c>
       <c r="N723" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O723" s="45"/>
       <c r="P723" s="45"/>
@@ -37433,7 +37467,7 @@
         <v>508</v>
       </c>
       <c r="F724" s="61" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G724" s="61" t="s">
         <v>29</v>
@@ -37443,7 +37477,7 @@
         <v>298</v>
       </c>
       <c r="J724" s="62">
-        <v>491000000000</v>
+        <v>491000</v>
       </c>
       <c r="K724" s="45"/>
       <c r="L724" s="61" t="s">
@@ -37453,7 +37487,7 @@
         <v>79</v>
       </c>
       <c r="N724" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O724" s="45"/>
       <c r="P724" s="45"/>
@@ -37477,7 +37511,7 @@
         <v>508</v>
       </c>
       <c r="F725" s="61" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G725" s="61" t="s">
         <v>29</v>
@@ -37487,7 +37521,7 @@
         <v>298</v>
       </c>
       <c r="J725" s="62">
-        <v>302000000000</v>
+        <v>302000</v>
       </c>
       <c r="K725" s="45"/>
       <c r="L725" s="61" t="s">
@@ -37497,7 +37531,7 @@
         <v>79</v>
       </c>
       <c r="N725" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O725" s="45"/>
       <c r="P725" s="45"/>
@@ -37521,7 +37555,7 @@
         <v>508</v>
       </c>
       <c r="F726" s="61" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G726" s="61" t="s">
         <v>29</v>
@@ -37531,7 +37565,7 @@
         <v>298</v>
       </c>
       <c r="J726" s="62">
-        <v>268000000000</v>
+        <v>268000</v>
       </c>
       <c r="K726" s="45"/>
       <c r="L726" s="61" t="s">
@@ -37541,7 +37575,7 @@
         <v>79</v>
       </c>
       <c r="N726" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O726" s="45"/>
       <c r="P726" s="45"/>
@@ -37565,7 +37599,7 @@
         <v>508</v>
       </c>
       <c r="F727" s="61" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="G727" s="61" t="s">
         <v>29</v>
@@ -37575,7 +37609,7 @@
         <v>298</v>
       </c>
       <c r="J727" s="62">
-        <v>208000000000</v>
+        <v>208000</v>
       </c>
       <c r="K727" s="45"/>
       <c r="L727" s="61" t="s">
@@ -37585,7 +37619,7 @@
         <v>79</v>
       </c>
       <c r="N727" s="61" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="O727" s="45"/>
       <c r="P727" s="45"/>
@@ -37596,21 +37630,46 @@
     </row>
     <row r="728" spans="1:20" ht="16" customHeight="1">
       <c r="A728" s="45"/>
-      <c r="B728" s="45"/>
-      <c r="C728" s="45"/>
-      <c r="D728" s="45"/>
-      <c r="E728" s="45"/>
-      <c r="F728" s="45"/>
-      <c r="G728" s="45"/>
+      <c r="B728" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="C728" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D728" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E728" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F728" s="61" t="s">
+        <v>512</v>
+      </c>
+      <c r="G728" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H728" s="45"/>
-      <c r="I728" s="45"/>
-      <c r="J728" s="45"/>
+      <c r="I728" s="45">
+        <v>298</v>
+      </c>
+      <c r="J728" s="45">
+        <f>P728*1000000</f>
+        <v>194021739.13043401</v>
+      </c>
       <c r="K728" s="45"/>
-      <c r="L728" s="45"/>
-      <c r="M728" s="45"/>
-      <c r="N728" s="45"/>
+      <c r="L728" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M728" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N728" s="61" t="s">
+        <v>509</v>
+      </c>
       <c r="O728" s="45"/>
-      <c r="P728" s="45"/>
+      <c r="P728" s="45">
+        <v>194.02173913043401</v>
+      </c>
       <c r="Q728" s="45"/>
       <c r="R728" s="45"/>
       <c r="S728" s="46"/>
@@ -37618,21 +37677,46 @@
     </row>
     <row r="729" spans="1:20" ht="16" customHeight="1">
       <c r="A729" s="45"/>
-      <c r="B729" s="45"/>
-      <c r="C729" s="45"/>
-      <c r="D729" s="45"/>
-      <c r="E729" s="45"/>
-      <c r="F729" s="45"/>
-      <c r="G729" s="45"/>
+      <c r="B729" s="61" t="s">
+        <v>501</v>
+      </c>
+      <c r="C729" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D729" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E729" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F729" s="61" t="s">
+        <v>512</v>
+      </c>
+      <c r="G729" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H729" s="45"/>
-      <c r="I729" s="45"/>
-      <c r="J729" s="45"/>
+      <c r="I729" s="45">
+        <v>298</v>
+      </c>
+      <c r="J729" s="45">
+        <f t="shared" ref="J729:J731" si="44">P729*1000000</f>
+        <v>169082125.60386401</v>
+      </c>
       <c r="K729" s="45"/>
-      <c r="L729" s="45"/>
-      <c r="M729" s="45"/>
-      <c r="N729" s="45"/>
+      <c r="L729" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M729" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N729" s="61" t="s">
+        <v>509</v>
+      </c>
       <c r="O729" s="45"/>
-      <c r="P729" s="45"/>
+      <c r="P729" s="45">
+        <v>169.082125603864</v>
+      </c>
       <c r="Q729" s="45"/>
       <c r="R729" s="45"/>
       <c r="S729" s="46"/>
@@ -37640,21 +37724,46 @@
     </row>
     <row r="730" spans="1:20" ht="16" customHeight="1">
       <c r="A730" s="45"/>
-      <c r="B730" s="45"/>
-      <c r="C730" s="45"/>
-      <c r="D730" s="45"/>
-      <c r="E730" s="45"/>
-      <c r="F730" s="45"/>
-      <c r="G730" s="45"/>
+      <c r="B730" s="61" t="s">
+        <v>502</v>
+      </c>
+      <c r="C730" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D730" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E730" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F730" s="61" t="s">
+        <v>512</v>
+      </c>
+      <c r="G730" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H730" s="45"/>
-      <c r="I730" s="45"/>
-      <c r="J730" s="45"/>
+      <c r="I730" s="45">
+        <v>298</v>
+      </c>
+      <c r="J730" s="45">
+        <f t="shared" si="44"/>
+        <v>159118357.48792198</v>
+      </c>
       <c r="K730" s="45"/>
-      <c r="L730" s="45"/>
-      <c r="M730" s="45"/>
-      <c r="N730" s="45"/>
+      <c r="L730" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M730" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N730" s="61" t="s">
+        <v>509</v>
+      </c>
       <c r="O730" s="45"/>
-      <c r="P730" s="45"/>
+      <c r="P730" s="45">
+        <v>159.118357487922</v>
+      </c>
       <c r="Q730" s="45"/>
       <c r="R730" s="45"/>
       <c r="S730" s="46"/>
@@ -37662,21 +37771,46 @@
     </row>
     <row r="731" spans="1:20" ht="16" customHeight="1">
       <c r="A731" s="45"/>
-      <c r="B731" s="45"/>
-      <c r="C731" s="45"/>
-      <c r="D731" s="45"/>
-      <c r="E731" s="45"/>
-      <c r="F731" s="45"/>
-      <c r="G731" s="45"/>
+      <c r="B731" s="61" t="s">
+        <v>503</v>
+      </c>
+      <c r="C731" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D731" s="61" t="s">
+        <v>504</v>
+      </c>
+      <c r="E731" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="F731" s="61" t="s">
+        <v>512</v>
+      </c>
+      <c r="G731" s="61" t="s">
+        <v>29</v>
+      </c>
       <c r="H731" s="45"/>
-      <c r="I731" s="45"/>
-      <c r="J731" s="45"/>
+      <c r="I731" s="45">
+        <v>298</v>
+      </c>
+      <c r="J731" s="45">
+        <f t="shared" si="44"/>
+        <v>149094202.89855</v>
+      </c>
       <c r="K731" s="45"/>
-      <c r="L731" s="45"/>
-      <c r="M731" s="45"/>
-      <c r="N731" s="45"/>
+      <c r="L731" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M731" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="N731" s="61" t="s">
+        <v>509</v>
+      </c>
       <c r="O731" s="45"/>
-      <c r="P731" s="45"/>
+      <c r="P731" s="45">
+        <v>149.09420289855001</v>
+      </c>
       <c r="Q731" s="45"/>
       <c r="R731" s="45"/>
       <c r="S731" s="46"/>
@@ -37684,19 +37818,41 @@
     </row>
     <row r="732" spans="1:20" ht="16" customHeight="1">
       <c r="A732" s="45"/>
-      <c r="B732" s="45"/>
-      <c r="C732" s="45"/>
-      <c r="D732" s="45"/>
-      <c r="E732" s="45"/>
-      <c r="F732" s="45"/>
-      <c r="G732" s="45"/>
+      <c r="B732" s="45" t="s">
+        <v>513</v>
+      </c>
+      <c r="C732" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D732" s="45" t="s">
+        <v>514</v>
+      </c>
+      <c r="E732" s="45" t="s">
+        <v>515</v>
+      </c>
+      <c r="F732" s="61" t="s">
+        <v>512</v>
+      </c>
+      <c r="G732" s="45" t="s">
+        <v>29</v>
+      </c>
       <c r="H732" s="45"/>
-      <c r="I732" s="45"/>
-      <c r="J732" s="45"/>
+      <c r="I732" s="45">
+        <v>298</v>
+      </c>
+      <c r="J732" s="150">
+        <v>160000000</v>
+      </c>
       <c r="K732" s="45"/>
-      <c r="L732" s="45"/>
-      <c r="M732" s="45"/>
-      <c r="N732" s="45"/>
+      <c r="L732" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M732" s="45" t="s">
+        <v>516</v>
+      </c>
+      <c r="N732" s="45" t="s">
+        <v>517</v>
+      </c>
       <c r="O732" s="45"/>
       <c r="P732" s="45"/>
       <c r="Q732" s="45"/>
@@ -37706,19 +37862,43 @@
     </row>
     <row r="733" spans="1:20" ht="16" customHeight="1">
       <c r="A733" s="45"/>
-      <c r="B733" s="45"/>
-      <c r="C733" s="45"/>
-      <c r="D733" s="45"/>
-      <c r="E733" s="45"/>
-      <c r="F733" s="45"/>
-      <c r="G733" s="45"/>
-      <c r="H733" s="45"/>
-      <c r="I733" s="45"/>
-      <c r="J733" s="45"/>
+      <c r="B733" s="45" t="s">
+        <v>518</v>
+      </c>
+      <c r="C733" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D733" s="45" t="s">
+        <v>514</v>
+      </c>
+      <c r="E733" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="F733" s="61" t="s">
+        <v>522</v>
+      </c>
+      <c r="G733" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H733" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="I733" s="45">
+        <v>298</v>
+      </c>
+      <c r="J733" s="62">
+        <v>339000000</v>
+      </c>
       <c r="K733" s="45"/>
-      <c r="L733" s="45"/>
-      <c r="M733" s="45"/>
-      <c r="N733" s="45"/>
+      <c r="L733" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M733" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="N733" s="45" t="s">
+        <v>520</v>
+      </c>
       <c r="O733" s="45"/>
       <c r="P733" s="45"/>
       <c r="Q733" s="45"/>
@@ -37728,19 +37908,43 @@
     </row>
     <row r="734" spans="1:20" ht="16" customHeight="1">
       <c r="A734" s="45"/>
-      <c r="B734" s="45"/>
-      <c r="C734" s="45"/>
-      <c r="D734" s="45"/>
-      <c r="E734" s="45"/>
-      <c r="F734" s="45"/>
-      <c r="G734" s="45"/>
-      <c r="H734" s="45"/>
-      <c r="I734" s="45"/>
-      <c r="J734" s="45"/>
+      <c r="B734" s="45" t="s">
+        <v>521</v>
+      </c>
+      <c r="C734" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D734" s="45" t="s">
+        <v>514</v>
+      </c>
+      <c r="E734" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="F734" s="61" t="s">
+        <v>522</v>
+      </c>
+      <c r="G734" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H734" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="I734" s="45">
+        <v>298</v>
+      </c>
+      <c r="J734" s="62">
+        <v>489000000</v>
+      </c>
       <c r="K734" s="45"/>
-      <c r="L734" s="45"/>
-      <c r="M734" s="45"/>
-      <c r="N734" s="45"/>
+      <c r="L734" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M734" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="N734" s="45" t="s">
+        <v>520</v>
+      </c>
       <c r="O734" s="45"/>
       <c r="P734" s="45"/>
       <c r="Q734" s="45"/>

</xml_diff>

<commit_message>
- typo fix in one DOI
</commit_message>
<xml_diff>
--- a/MiscSmallUploads_Jun2025.xlsx
+++ b/MiscSmallUploads_Jun2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C948185A-F985-2E46-99A8-94F97587B598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C75B2EA-F5C4-0249-BEA1-AE08F4FCE2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="5420" windowWidth="31960" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7363" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7363" uniqueCount="551">
   <si>
     <r>
       <rPr>
@@ -1839,6 +1839,9 @@
   </si>
   <si>
     <t>10.1016/j.msea.2018.11.054</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2018.02.015</t>
   </si>
 </sst>
 </file>
@@ -3082,6 +3085,58 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3142,58 +3197,6 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="9" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4356,8 +4359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T960"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A771" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M803" sqref="M803"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B340" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -4414,19 +4417,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="121"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="139"/>
       <c r="O2" s="13"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -4442,17 +4445,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="125"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="143"/>
       <c r="O3" s="13"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -4493,43 +4496,43 @@
       <c r="B5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="126" t="s">
+      <c r="C5" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="128" t="s">
+      <c r="D5" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="128" t="s">
+      <c r="E5" s="146" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="128" t="s">
+      <c r="F5" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="128" t="s">
+      <c r="G5" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="129" t="s">
+      <c r="H5" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="128" t="s">
+      <c r="I5" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="128" t="s">
+      <c r="J5" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="128" t="s">
+      <c r="K5" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="128" t="s">
+      <c r="L5" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="128" t="s">
+      <c r="M5" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="128" t="s">
+      <c r="N5" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="133" t="s">
+      <c r="O5" s="114" t="s">
         <v>20</v>
       </c>
       <c r="P5" s="25"/>
@@ -4545,19 +4548,19 @@
       <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="130"/>
-      <c r="I6" s="131"/>
-      <c r="J6" s="132"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="127"/>
-      <c r="M6" s="127"/>
-      <c r="N6" s="127"/>
-      <c r="O6" s="134"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="145"/>
+      <c r="M6" s="145"/>
+      <c r="N6" s="145"/>
+      <c r="O6" s="115"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="9"/>
@@ -4607,7 +4610,7 @@
       <c r="N7" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="135"/>
+      <c r="O7" s="116"/>
       <c r="P7" s="68" t="s">
         <v>77</v>
       </c>
@@ -4622,35 +4625,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" thickBot="1">
       <c r="A8" s="63"/>
-      <c r="B8" s="136" t="s">
+      <c r="B8" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="137"/>
-      <c r="D8" s="137"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="139" t="s">
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="140"/>
-      <c r="H8" s="140"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="142"/>
-      <c r="K8" s="142"/>
-      <c r="L8" s="143"/>
-      <c r="M8" s="144" t="s">
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="125" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="145"/>
+      <c r="N8" s="126"/>
       <c r="O8" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="146" t="s">
+      <c r="P8" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="147"/>
-      <c r="R8" s="148"/>
-      <c r="S8" s="148"/>
-      <c r="T8" s="149"/>
+      <c r="Q8" s="128"/>
+      <c r="R8" s="129"/>
+      <c r="S8" s="129"/>
+      <c r="T8" s="130"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1">
       <c r="A9" s="64" t="s">
@@ -6259,7 +6262,7 @@
       </c>
       <c r="M44" s="40"/>
       <c r="N44" s="98" t="s">
-        <v>144</v>
+        <v>550</v>
       </c>
       <c r="O44" s="46"/>
       <c r="P44" s="46"/>
@@ -37921,7 +37924,7 @@
       <c r="I732" s="45">
         <v>298</v>
       </c>
-      <c r="J732" s="150">
+      <c r="J732" s="113">
         <v>160000000</v>
       </c>
       <c r="K732" s="45"/>
@@ -44429,11 +44432,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -44448,6 +44446,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>

</xml_diff>